<commit_message>
Show more detailed information about related resources in full record view (fixes #316)
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="389">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1506,6 +1506,15 @@
     <t xml:space="preserve">In: Hermes (1991), p. 173-213</t>
   </si>
   <si>
+    <t xml:space="preserve">787 $i, $n, $t und $w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erscheint auch als Online-Ausgabe: Gesundheitsrecht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erscheint auch als Online-Ausgabe: Klausurtraining Verfassungsrecht</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vorheriger / Späterer Titel</t>
   </si>
   <si>
@@ -1556,7 +1565,7 @@
 Darin aufgeg.: Management-Praxis
 Darin aufgeg.: Wirtschaftswoche &lt;Düsseldorf&gt; / Ostausgabe
 1988 Beil. u. 1991 darin aufgeg.: Profitravel
-Darin aufgegangen: Wirtschaftswoche &lt;Düsseldorf&gt; / Green economy. Green economy</t>
+Darin aufgegangen 2016, 23-: Wirtschaftswoche &lt;Düsseldorf&gt; / Green economy. Green economy</t>
   </si>
   <si>
     <t xml:space="preserve">Anmerkungen</t>
@@ -2806,9 +2815,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3880080</xdr:colOff>
+      <xdr:colOff>3879720</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2818,7 +2827,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13262040" cy="9518760"/>
+          <a:ext cx="13547520" cy="9518400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2858,13 +2867,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.0837209302326"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="73.5906976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.9162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="92.7906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="75.8046511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3147,13 +3157,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3364,14 +3374,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,14 +3586,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,14 +3798,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,14 +4010,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,20 +4218,21 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4437,13 +4452,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4618,21 +4633,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4770,6 +4785,34 @@
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
       <c r="F13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>876614268</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>894531530</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4791,18 +4834,18 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.8558139534884"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.153488372093"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4810,7 +4853,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4822,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4830,7 +4873,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4838,7 +4881,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4846,7 +4889,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4858,7 +4901,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -4883,18 +4926,18 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4903,10 +4946,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>259</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4915,7 +4958,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>0</v>
@@ -4973,27 +5016,27 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>130559555</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B18" s="24" t="n">
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -5027,13 +5070,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.1162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5041,7 +5084,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5053,7 +5096,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,7 +5104,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,7 +5112,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,7 +5120,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -5089,7 +5132,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -5116,42 +5159,42 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="275.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C11" s="50"/>
       <c r="F11" s="51"/>
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C12" s="50"/>
       <c r="E12" s="3"/>
@@ -5159,10 +5202,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="52"/>
@@ -5171,10 +5214,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="3"/>
@@ -5183,10 +5226,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="3"/>
@@ -5241,13 +5284,13 @@
     </row>
     <row r="20" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B20" s="24" t="n">
         <v>129993549</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -5255,13 +5298,13 @@
     </row>
     <row r="21" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="17" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B21" s="24" t="n">
         <v>129494860</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -5269,13 +5312,13 @@
     </row>
     <row r="22" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="17" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B22" s="24" t="n">
         <v>129292834</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -5283,13 +5326,13 @@
     </row>
     <row r="23" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B23" s="24" t="n">
         <v>329875515</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -5297,13 +5340,13 @@
     </row>
     <row r="24" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B24" s="24" t="n">
         <v>888820720</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -5311,13 +5354,13 @@
     </row>
     <row r="25" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="17" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B25" s="24" t="n">
         <v>487757955</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -5351,13 +5394,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5568,14 +5611,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.004651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5583,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5597,7 +5641,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5611,7 +5655,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5625,7 +5669,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5639,7 +5683,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5653,7 +5697,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5689,7 +5733,7 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B9" s="38" t="s">
         <v>235</v>
@@ -5742,13 +5786,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>509133061</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -5756,13 +5800,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -5770,13 +5814,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>349876193</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -5784,13 +5828,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>129495476</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="43"/>
@@ -5798,13 +5842,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>336079826</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="43"/>
@@ -5812,13 +5856,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B18" s="24" t="n">
         <v>787199796</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="43"/>
@@ -5826,13 +5870,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B19" s="24" t="n">
         <v>872316203</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="43"/>
@@ -5840,13 +5884,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B20" s="24" t="n">
         <v>683536028</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="43"/>
@@ -5854,13 +5898,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B21" s="24" t="n">
         <v>826257127</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="43"/>
@@ -5893,13 +5937,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5907,7 +5952,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5921,7 +5966,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5935,7 +5980,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5949,7 +5994,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5963,7 +6008,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5977,7 +6022,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6013,10 +6058,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -6066,13 +6111,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -6080,13 +6125,13 @@
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>770927416</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -6094,13 +6139,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>194273989</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -6133,13 +6178,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6147,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -6161,7 +6207,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -6175,7 +6221,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6189,7 +6235,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -6203,7 +6249,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -6217,7 +6263,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6253,10 +6299,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -6306,13 +6352,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -6320,13 +6366,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>193804867</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -6334,13 +6380,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>409606901</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -6373,13 +6419,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.1023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.1209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.0883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.1023255813953"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6387,7 +6433,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6399,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6407,7 +6453,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6415,7 +6461,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6423,7 +6469,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6435,7 +6481,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6464,20 +6510,20 @@
     </row>
     <row r="9" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="3"/>
@@ -6542,13 +6588,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>187029679</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -6556,13 +6602,13 @@
     </row>
     <row r="17" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>884572641</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -6570,13 +6616,13 @@
     </row>
     <row r="18" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -6610,13 +6656,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.1488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.5023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6624,7 +6670,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6636,7 +6682,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6644,7 +6690,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6652,7 +6698,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6660,7 +6706,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6672,7 +6718,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6701,13 +6747,13 @@
     </row>
     <row r="9" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="D9" s="10"/>
     </row>
@@ -6769,13 +6815,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -6783,13 +6829,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>885659430</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -6823,14 +6869,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6838,7 +6885,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -6852,7 +6899,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -6866,7 +6913,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6880,7 +6927,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -6894,7 +6941,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -6908,7 +6955,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6944,7 +6991,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -6995,13 +7042,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -7034,14 +7081,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.8837209302326"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7049,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -7063,7 +7111,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -7077,7 +7125,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -7091,7 +7139,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -7105,7 +7153,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -7119,7 +7167,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -7155,13 +7203,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -7170,10 +7218,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -7183,10 +7231,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -7236,18 +7284,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -7280,11 +7328,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.5813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7579,11 +7627,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7906,17 +7954,17 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.4232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.6558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8294,10 +8342,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.8046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.5116279069767"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8528,14 +8576,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8741,14 +8790,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8980,14 +9030,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adjusted test case comment (refs #316)
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1556,7 +1556,7 @@
 Forts.: Code de procédure civile</t>
   </si>
   <si>
-    <t xml:space="preserve">780 $i und $t</t>
+    <t xml:space="preserve">780 $i, $n und $t</t>
   </si>
   <si>
     <t xml:space="preserve">Vorg.: Wirtschaftswoche, der Volkswirt, Aktionär
@@ -2815,9 +2815,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3879720</xdr:colOff>
+      <xdr:colOff>3879360</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2827,7 +2827,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13547520" cy="9518400"/>
+          <a:ext cx="13832640" cy="9518040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2867,14 +2867,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="92.7906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="75.8046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="95.4976744186046"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="78.0232558139535"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="72.3627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3157,13 +3157,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3374,15 +3374,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,15 +3586,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,15 +3798,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4010,15 +4010,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,15 +4224,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4452,13 +4452,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4635,19 +4635,19 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4833,19 +4833,19 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.0883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.9162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.5209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5028,7 +5028,7 @@
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
         <v>269</v>
       </c>
@@ -5070,13 +5070,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.5441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.9209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5394,13 +5394,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.6046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5611,15 +5611,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.004651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.079069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5937,14 +5937,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.7767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.6232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6178,14 +6178,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6419,13 +6419,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.0883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.1023255813953"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,13 +6656,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.5023255813954"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.6883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8558139534884"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,15 +6869,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7081,15 +7081,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.8837209302326"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.7302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7328,11 +7328,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7627,11 +7627,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7960,11 +7960,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.6558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.0093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8342,10 +8342,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.5116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.3441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8576,15 +8576,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8790,15 +8790,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9030,15 +9030,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.3581395348837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adjusted unit test to fit to changed data (refs #187, refs #120)
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1794,7 +1794,7 @@
     <t xml:space="preserve">246 $i, $a</t>
   </si>
   <si>
-    <t xml:space="preserve">Nebent.: Nature, science, progrès
+    <t xml:space="preserve">Nebent: Nature, science, progrès
 Zusatz bis 88.1960: Revue des sciences et de leurs applications</t>
   </si>
   <si>
@@ -2815,9 +2815,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3879360</xdr:colOff>
+      <xdr:colOff>3879000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2827,7 +2827,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13832640" cy="9518040"/>
+          <a:ext cx="14127840" cy="9517680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2867,14 +2867,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="95.4976744186046"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="78.0232558139535"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="72.3627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.4837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="98.3255813953488"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="80.3581395348837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3157,13 +3157,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3374,15 +3374,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,15 +3586,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,15 +3798,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4010,15 +4010,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,15 +4224,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4452,13 +4452,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4641,13 +4641,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4833,19 +4833,19 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.8883720930233"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5064,19 +5064,19 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.5441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.7581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.1674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5394,13 +5394,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5611,15 +5611,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="106.079069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="109.279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5937,14 +5937,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6178,14 +6178,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6419,13 +6419,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,13 +6656,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.6883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,15 +6869,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7081,15 +7081,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.7302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.6976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7328,11 +7328,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7627,11 +7627,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7960,11 +7960,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.0093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.3627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8342,10 +8342,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.3441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.297674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8576,15 +8576,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8790,15 +8790,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9030,15 +9030,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="82.8186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.4511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Show the title of work in record metadata (refs #145)
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,13 +27,14 @@
     <sheet name="Verwandte Ressourcen" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Vorheriger Späterer Titel" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Anmerkungen" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="Umfang" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="Fingerprint" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="Bibliographische Zitate" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="ISBN" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="Falsche ISBN" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="ZDB-Nummer" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="Basisklassifikation" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Werktitel" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Umfang" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Fingerprint" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Bibliographische Zitate" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="ISBN" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="Falsche ISBN" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="ZDB-Nummer" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Basisklassifikation" sheetId="27" state="visible" r:id="rId28"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -219,7 +220,7 @@
 </comments>
 </file>
 
-<file path=xl/comments23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -245,6 +246,31 @@
 </file>
 
 <file path=xl/comments24.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments25.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -370,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="458">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1824,6 +1850,296 @@
   <si>
     <t xml:space="preserve">With: Index emendatus perfecit / J. Christian Bay
 Die Vorlage enthält insgesamt 2 Werke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wektitel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darstellung des Titels des Werkes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Werktitel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title of work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform title</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Der Werktitel kann unter Marc 130 oder 240 vorkommen.
+240 wird nicht verwendet wenn 130 bereits belegt ist.
+240 ist wiederholbar.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Darstellungsregel
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Die Daten werden in Vollanzeige nach der Zeile "Anmerkungen" dargestellt.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptorzeichen:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Komma und Leerzeichen ", "
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Darstellungsregel:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+130 $a(, $d)(, $f)(, $g)(, $h)(, $k)(, $l)(, $m)(, $n)(, $o)(, $p)(, $r)(, $s)(, $t)
+240 $a(, $d)(, $f)(, $g)(, $h)(, $k)(, $l)(, $m)(, $n)(, $o)(, $p)(, $r)(, $s)(, $t)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of treaty signing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneus information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form subheading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium of performance for music</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of part/section of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arranged statement for music</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of part/section of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key for music</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plein soleil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64430636X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The language of life &lt;dt.&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">878078703 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tannöd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le phénomène évangélique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $a, $f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibel, 1824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89896363X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprache für die Arbeitswelt, Deutsch. Material, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 $a, $r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The original copy: photography of sculpture, 1839 to today, dt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essentials of ecology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wirtschaftsrecht, Arbeitsrecht, Sozialrecht
+Wirtschaft, Arbeit und Soziales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $a, $f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgaben mit Lösungen zum Grundwissen Elektrotechnik, 2005
+Aufgaben mit Lösungen zur Elektrotechnik, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $a (GND)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der @Ehrentag</t>
   </si>
   <si>
     <t xml:space="preserve">Umfang</t>
@@ -2815,9 +3131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3879000</xdr:colOff>
+      <xdr:colOff>3878640</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2827,7 +3143,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="14127840" cy="9517680"/>
+          <a:ext cx="14432040" cy="9517320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2867,14 +3183,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.4837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="98.3255813953488"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="80.3581395348837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="101.279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="82.8186046511628"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3157,13 +3473,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.004651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.3767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3374,15 +3690,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,15 +3902,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,15 +4114,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4010,15 +4326,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,15 +4540,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4452,13 +4768,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.004651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.3767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4641,13 +4957,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.004651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.3767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4839,13 +5155,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.4837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="15.2604651162791"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5064,19 +5380,19 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.7581395348837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.0976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.4139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5394,13 +5710,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.1581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.004651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.3767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5603,6 +5919,583 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F52"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.353488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2976744186046"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.9674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5023255813953"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C27" s="15"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C28" s="15"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C30" s="15"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C31" s="15"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C35" s="15"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="F37" s="26"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B42" s="24" t="n">
+        <v>772027102</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B45" s="24" t="n">
+        <v>774856556</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="B46" s="24" t="n">
+        <v>147213592</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="B48" s="24" t="n">
+        <v>622487175</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="B49" s="24" t="n">
+        <v>859958280</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="B50" s="24" t="n">
+        <v>871478110</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="B51" s="24" t="n">
+        <v>881131350</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="B52" s="24" t="n">
+        <v>882661418</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="D52" s="20"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #145"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -5611,15 +6504,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="109.279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="112.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5627,7 +6520,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>302</v>
+        <v>371</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5641,7 +6534,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>303</v>
+        <v>372</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5655,7 +6548,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>304</v>
+        <v>373</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5669,7 +6562,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>302</v>
+        <v>371</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5683,7 +6576,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>305</v>
+        <v>374</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5697,7 +6590,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>306</v>
+        <v>375</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5733,7 +6626,7 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>307</v>
+        <v>376</v>
       </c>
       <c r="B9" s="38" t="s">
         <v>235</v>
@@ -5786,13 +6679,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>308</v>
+        <v>377</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>509133061</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>309</v>
+        <v>378</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -5800,13 +6693,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>310</v>
+        <v>379</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>311</v>
+        <v>380</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -5814,13 +6707,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>312</v>
+        <v>381</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>349876193</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>313</v>
+        <v>382</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -5828,13 +6721,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="s">
-        <v>314</v>
+        <v>383</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>129495476</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>315</v>
+        <v>384</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="43"/>
@@ -5842,13 +6735,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>316</v>
+        <v>385</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>336079826</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>317</v>
+        <v>386</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="43"/>
@@ -5856,13 +6749,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>318</v>
+        <v>387</v>
       </c>
       <c r="B18" s="24" t="n">
         <v>787199796</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>319</v>
+        <v>388</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="43"/>
@@ -5870,13 +6763,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="s">
-        <v>308</v>
+        <v>377</v>
       </c>
       <c r="B19" s="24" t="n">
         <v>872316203</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>320</v>
+        <v>389</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="43"/>
@@ -5884,13 +6777,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="s">
-        <v>308</v>
+        <v>377</v>
       </c>
       <c r="B20" s="24" t="n">
         <v>683536028</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>321</v>
+        <v>390</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="43"/>
@@ -5898,13 +6791,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="s">
-        <v>322</v>
+        <v>391</v>
       </c>
       <c r="B21" s="24" t="n">
         <v>826257127</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>323</v>
+        <v>392</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="43"/>
@@ -5913,247 +6806,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="Ticket #128"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.4697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-    </row>
-    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="s">
-        <v>328</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-    </row>
-    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
-        <v>328</v>
-      </c>
-      <c r="B13" s="24" t="n">
-        <v>151797196</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>329</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-    </row>
-    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
-        <v>328</v>
-      </c>
-      <c r="B14" s="24" t="n">
-        <v>770927416</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>330</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41" t="s">
-        <v>331</v>
-      </c>
-      <c r="B15" s="24" t="n">
-        <v>194273989</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>332</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #149"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6172,20 +6824,20 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.4372093023256"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6193,7 +6845,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>333</v>
+        <v>393</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -6202,12 +6854,12 @@
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>334</v>
+        <v>394</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -6216,12 +6868,12 @@
       <c r="G2" s="31"/>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>335</v>
+        <v>395</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6235,7 +6887,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>336</v>
+        <v>393</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -6249,7 +6901,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>337</v>
+        <v>393</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -6263,7 +6915,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>338</v>
+        <v>396</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6299,10 +6951,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>339</v>
+        <v>397</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>340</v>
+        <v>393</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -6350,43 +7002,43 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>339</v>
+        <v>397</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>341</v>
+        <v>398</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
       <c r="F13" s="44"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>339</v>
+        <v>397</v>
       </c>
       <c r="B14" s="24" t="n">
-        <v>193804867</v>
+        <v>770927416</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>342</v>
+        <v>399</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
       <c r="F14" s="44"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>343</v>
+        <v>400</v>
       </c>
       <c r="B15" s="24" t="n">
-        <v>409606901</v>
+        <v>194273989</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>344</v>
+        <v>401</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -6394,7 +7046,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #150"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #149"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6411,6 +7063,247 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="37" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>151797196</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>410</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>193804867</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>411</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="41" t="s">
+        <v>412</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>409606901</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="44"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #150"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6419,13 +7312,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.1813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.6093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6433,7 +7326,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>345</v>
+        <v>414</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6445,7 +7338,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>345</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6453,7 +7346,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>346</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6461,7 +7354,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>345</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6469,7 +7362,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>345</v>
+        <v>414</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6481,7 +7374,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>347</v>
+        <v>416</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6510,20 +7403,20 @@
     </row>
     <row r="9" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>348</v>
+        <v>417</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>349</v>
+        <v>418</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>350</v>
+        <v>419</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>351</v>
+        <v>420</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="3"/>
@@ -6588,13 +7481,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>352</v>
+        <v>421</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>187029679</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>353</v>
+        <v>422</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -6602,13 +7495,13 @@
     </row>
     <row r="17" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>354</v>
+        <v>423</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>884572641</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>355</v>
+        <v>424</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -6616,230 +7509,17 @@
     </row>
     <row r="18" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>354</v>
+        <v>423</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>356</v>
+        <v>425</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>357</v>
+        <v>426</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId2" display="Ticket #170"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="C15" s="55" t="s">
-        <v>364</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="B16" s="24" t="n">
-        <v>885659430</v>
-      </c>
-      <c r="C16" s="56" t="s">
-        <v>365</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6861,6 +7541,219 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.8093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.9209302325581"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>425</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>885659430</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>434</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #170"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6869,15 +7762,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6885,7 +7778,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>366</v>
+        <v>435</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -6899,7 +7792,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>367</v>
+        <v>436</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -6913,7 +7806,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>368</v>
+        <v>437</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6927,7 +7820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>366</v>
+        <v>435</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -6941,7 +7834,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>369</v>
+        <v>438</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -6955,7 +7848,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>370</v>
+        <v>439</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6991,7 +7884,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>371</v>
+        <v>440</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -7042,13 +7935,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>371</v>
+        <v>440</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>372</v>
+        <v>441</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -7068,7 +7961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7081,15 +7974,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.6976744186047"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="68.7906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7097,7 +7990,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>373</v>
+        <v>442</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -7111,7 +8004,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>374</v>
+        <v>443</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -7125,7 +8018,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>375</v>
+        <v>444</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -7139,7 +8032,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>376</v>
+        <v>445</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -7153,7 +8046,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>377</v>
+        <v>446</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -7167,7 +8060,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>378</v>
+        <v>447</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -7203,13 +8096,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>379</v>
+        <v>448</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>380</v>
+        <v>449</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>381</v>
+        <v>450</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -7218,10 +8111,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>382</v>
+        <v>451</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>383</v>
+        <v>452</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -7231,10 +8124,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>384</v>
+        <v>453</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>385</v>
+        <v>454</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -7284,18 +8177,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>386</v>
+        <v>455</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>387</v>
+        <v>456</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44" t="s">
-        <v>388</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -7328,11 +8221,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7627,11 +8520,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.3627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7960,11 +8853,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.3627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8342,10 +9235,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.297674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.3627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="103.251162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8576,15 +9469,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8790,15 +9683,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9030,15 +9923,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added new version of rda.xlsx. Added reproduction test. refs #368
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fe57gop\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fe57gop\Desktop\beispiele\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="29040" windowHeight="15675" tabRatio="992" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="29040" windowHeight="15675" tabRatio="992" firstSheet="19" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,13 @@
     <sheet name="Anmerkungen" sheetId="20" r:id="rId20"/>
     <sheet name="Werktitel" sheetId="21" r:id="rId21"/>
     <sheet name="Umfang" sheetId="22" r:id="rId22"/>
-    <sheet name="Fingerprint" sheetId="23" r:id="rId23"/>
-    <sheet name="Bibliographische Zitate" sheetId="24" r:id="rId24"/>
-    <sheet name="ISBN" sheetId="25" r:id="rId25"/>
-    <sheet name="Falsche ISBN" sheetId="26" r:id="rId26"/>
-    <sheet name="ZDB-Nummer" sheetId="27" r:id="rId27"/>
-    <sheet name="Basisklassifikation" sheetId="28" r:id="rId28"/>
+    <sheet name="Sekundäre Ausgabe" sheetId="29" r:id="rId23"/>
+    <sheet name="Fingerprint" sheetId="23" r:id="rId24"/>
+    <sheet name="Bibliographische Zitate" sheetId="24" r:id="rId25"/>
+    <sheet name="ISBN" sheetId="25" r:id="rId26"/>
+    <sheet name="Falsche ISBN" sheetId="26" r:id="rId27"/>
+    <sheet name="ZDB-Nummer" sheetId="27" r:id="rId28"/>
+    <sheet name="Basisklassifikation" sheetId="28" r:id="rId29"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -429,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="487">
   <si>
     <t>Titel</t>
   </si>
@@ -1945,6 +1946,324 @@
     <t>Uniform title</t>
   </si>
   <si>
+    <t>130 $d</t>
+  </si>
+  <si>
+    <t>Date of treaty signing</t>
+  </si>
+  <si>
+    <t>130 $f</t>
+  </si>
+  <si>
+    <t>Date of a work</t>
+  </si>
+  <si>
+    <t>130 $g</t>
+  </si>
+  <si>
+    <t>Miscellaneus information</t>
+  </si>
+  <si>
+    <t>130 $h</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>130 $k</t>
+  </si>
+  <si>
+    <t>Form subheading</t>
+  </si>
+  <si>
+    <t>130 $l</t>
+  </si>
+  <si>
+    <t>Language of a work</t>
+  </si>
+  <si>
+    <t>130 $m</t>
+  </si>
+  <si>
+    <t>Medium of performance for music</t>
+  </si>
+  <si>
+    <t>130 $n</t>
+  </si>
+  <si>
+    <t>Number of part/section of a work</t>
+  </si>
+  <si>
+    <t>130 $o</t>
+  </si>
+  <si>
+    <t>Arranged statement for music</t>
+  </si>
+  <si>
+    <t>130 $p</t>
+  </si>
+  <si>
+    <t>Name of part/section of a work</t>
+  </si>
+  <si>
+    <t>130 $r</t>
+  </si>
+  <si>
+    <t>Key for music</t>
+  </si>
+  <si>
+    <t>130 $s</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>130 $t</t>
+  </si>
+  <si>
+    <t>Title of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 $a </t>
+  </si>
+  <si>
+    <t>240 $d</t>
+  </si>
+  <si>
+    <t>240 $f</t>
+  </si>
+  <si>
+    <t>240 $g</t>
+  </si>
+  <si>
+    <t>240 $h</t>
+  </si>
+  <si>
+    <t>240 $k</t>
+  </si>
+  <si>
+    <t>240 $l</t>
+  </si>
+  <si>
+    <t>240 $m</t>
+  </si>
+  <si>
+    <t>240 $n</t>
+  </si>
+  <si>
+    <t>240 $o</t>
+  </si>
+  <si>
+    <t>240 $p</t>
+  </si>
+  <si>
+    <t>240 $r</t>
+  </si>
+  <si>
+    <t>240 $s</t>
+  </si>
+  <si>
+    <t>240 $t</t>
+  </si>
+  <si>
+    <t>130 $a</t>
+  </si>
+  <si>
+    <t>Plein soleil</t>
+  </si>
+  <si>
+    <t>64430636X</t>
+  </si>
+  <si>
+    <t>The language of life &lt;dt.&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">878078703 </t>
+  </si>
+  <si>
+    <t>Tannöd</t>
+  </si>
+  <si>
+    <t>Le phénomène évangélique</t>
+  </si>
+  <si>
+    <t>130 $a, $f</t>
+  </si>
+  <si>
+    <t>89896363X</t>
+  </si>
+  <si>
+    <t>130 $a, $r</t>
+  </si>
+  <si>
+    <t>The original copy: photography of sculpture, 1839 to today, dt.</t>
+  </si>
+  <si>
+    <t>240 $a</t>
+  </si>
+  <si>
+    <t>Essentials of ecology</t>
+  </si>
+  <si>
+    <t>Wirtschaftsrecht, Arbeitsrecht, Sozialrecht
+Wirtschaft, Arbeit und Soziales</t>
+  </si>
+  <si>
+    <t>240 $a, $f</t>
+  </si>
+  <si>
+    <t>Aufgaben mit Lösungen zum Grundwissen Elektrotechnik, 2005
+Aufgaben mit Lösungen zur Elektrotechnik, 2008</t>
+  </si>
+  <si>
+    <t>240 $a (GND)</t>
+  </si>
+  <si>
+    <t>Der @Ehrentag</t>
+  </si>
+  <si>
+    <t>Umfang</t>
+  </si>
+  <si>
+    <t>Anzeige der Umfangsangaben</t>
+  </si>
+  <si>
+    <t>Physical Description</t>
+  </si>
+  <si>
+    <t>Physical description</t>
+  </si>
+  <si>
+    <t>Ticket #128</t>
+  </si>
+  <si>
+    <t>300 $a,$b,$c und $d</t>
+  </si>
+  <si>
+    <t>300 $a, $b, $c</t>
+  </si>
+  <si>
+    <t>12 S. : Ill., graph. Darst. ; 30 cm</t>
+  </si>
+  <si>
+    <t>300 2x$a, $b</t>
+  </si>
+  <si>
+    <t>300 $a, $c, $e</t>
+  </si>
+  <si>
+    <t>Online-Ressource</t>
+  </si>
+  <si>
+    <t>300 $c</t>
+  </si>
+  <si>
+    <t>30 cm</t>
+  </si>
+  <si>
+    <t>300 $a, $c</t>
+  </si>
+  <si>
+    <t>62 Bl ; 19 x 17 cm</t>
+  </si>
+  <si>
+    <t>300 $a, $e</t>
+  </si>
+  <si>
+    <t>6 S. ; Chorpartitur, 6 St.</t>
+  </si>
+  <si>
+    <t>1 Karte : farbig ; 56 x 58 cm, auf Blatt 60 x 76 cm, gefaltet 23 x 11 cm</t>
+  </si>
+  <si>
+    <t>1 DVD-Video (7 Min.) : s/w, stumm ; 12 cm</t>
+  </si>
+  <si>
+    <t>300 $a, $b, $c, $e</t>
+  </si>
+  <si>
+    <t>1 CD : digital ; 22 cm ; 1 Blatt</t>
+  </si>
+  <si>
+    <t>Fingerprint</t>
+  </si>
+  <si>
+    <t>Fingerprint bei alten Drucken mit Herkunftsangabe aus Pica-Feld 2275 mit Unterfeld $a</t>
+  </si>
+  <si>
+    <t>Fingerprint Identifier (Unparsed fingerprint, Institution to which field applies)</t>
+  </si>
+  <si>
+    <t>Ticket #149</t>
+  </si>
+  <si>
+    <t>026 $e $5</t>
+  </si>
+  <si>
+    <t>S.ME u-r- m-r- siRe 3 1700R (UFB Erfurt/Gotha; NLB Hannover; Bibliothek des Herzog Anton Ulrich-Museums Braunschweig; SBB-PK Berlin)</t>
+  </si>
+  <si>
+    <t>t,n, o-s- e-n- Dese C 1539A (SBB; ThULB Jena; Wartburg-Stiftung Eisenach)</t>
+  </si>
+  <si>
+    <t>026 $e, ohne $5</t>
+  </si>
+  <si>
+    <t>UMUM s.m, m.it quRe 3 1779R 1,1</t>
+  </si>
+  <si>
+    <t>Bibliographische Zitate</t>
+  </si>
+  <si>
+    <t>Anzeige des Felds Bibliografische Zitate (PICA-Feld 2277).
+Dient der Identifikation und dem Nachweis von alten Drucken und wird auch für die Suche verwendet.
+Anzeige des Felds:
+Bibliografische Zitate: 510a
+Bibliographic citations: 510a</t>
+  </si>
+  <si>
+    <t>Bibliographic (Name of source)</t>
+  </si>
+  <si>
+    <t>Bibliografische Zitate</t>
+  </si>
+  <si>
+    <t>Bibliographic citations</t>
+  </si>
+  <si>
+    <t>Ticket #150</t>
+  </si>
+  <si>
+    <t>510 $a</t>
+  </si>
+  <si>
+    <t>Bibliographisches Zitat</t>
+  </si>
+  <si>
+    <t>SBN On-line IT\ICCU\MODE\018621</t>
+  </si>
+  <si>
+    <t>VD17 3:009152Z</t>
+  </si>
+  <si>
+    <t>510 $a (wiederholt)</t>
+  </si>
+  <si>
+    <t>IG 1281 ; GW 12189 ; ISTC ih00015000 ; BSB-Ink H-41 ; H 8426</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>International Standard Book Number</t>
+  </si>
+  <si>
+    <t>Ticket #170</t>
+  </si>
+  <si>
+    <t>020 $9</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1953,6 +2272,299 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">Verwende $9 statt $a für die Anzeige, weil es die vorlagetreue Schreibweise (mit den Bindestrichen) enthält.
+Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ISBN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $9 : $c
+           $9 : $c
+020 ist wiederholbar. Wenn mehrfach belegt, ISBN untereinander anzeigen</t>
+    </r>
+  </si>
+  <si>
+    <t>020 $c</t>
+  </si>
+  <si>
+    <t>Terms of availability</t>
+  </si>
+  <si>
+    <t>$9</t>
+  </si>
+  <si>
+    <t>3-86025-284-4</t>
+  </si>
+  <si>
+    <t>$9 und $c</t>
+  </si>
+  <si>
+    <t>978-92-897-1568-3
+978-92-2-130471-5 : ILO
+978-92-897-1569-0 : web
+978-92-2-130472-2 : PDF</t>
+  </si>
+  <si>
+    <t>52680498X</t>
+  </si>
+  <si>
+    <t>3-540-69713-6 : EUR 29.95, sfr 46.00
+978-3-540-69713-8 : EUR 29.95, sfr 46.00
+978-3-540-69739-8</t>
+  </si>
+  <si>
+    <t>Falsche ISBN</t>
+  </si>
+  <si>
+    <t>Invalid ISBN</t>
+  </si>
+  <si>
+    <t>020 $z</t>
+  </si>
+  <si>
+    <t>Canceled/invalid ISBN</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">In Solr-Marc ist die falsche ISBN leider nur ohne "-" vorhanden.
+Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Falsche</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ISBN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $z
+</t>
+    </r>
+  </si>
+  <si>
+    <t>$z</t>
+  </si>
+  <si>
+    <t>9784540697138</t>
+  </si>
+  <si>
+    <t>9783643137173</t>
+  </si>
+  <si>
+    <t>ZDB-Nummer</t>
+  </si>
+  <si>
+    <t>Anzeige der ZDB-Nummer</t>
+  </si>
+  <si>
+    <t>System Control Number</t>
+  </si>
+  <si>
+    <t>ZDB-Number</t>
+  </si>
+  <si>
+    <t>Ticket #132</t>
+  </si>
+  <si>
+    <t>035 $a</t>
+  </si>
+  <si>
+    <t>1393051-5</t>
+  </si>
+  <si>
+    <t>Basisklassifikation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Detailanzeige</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:
+Wenn 084 $2 rvk:
+084 $a
+Trennzeichen bei Wiederholungen von 084 mit $2 = rvk: _;_ (in Worten: Blank Semikolon Blank)
+Auf jede Notation einen </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Suchlink </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">legen: Indexsuche mit Inhalt von 084 $a in rvk_full
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Other Classification Number</t>
+  </si>
+  <si>
+    <t>Sachgebiete</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Ticket #97</t>
+  </si>
+  <si>
+    <t>084 $a</t>
+  </si>
+  <si>
+    <t>Klassifikationsnummer</t>
+  </si>
+  <si>
+    <t>084 ist wiederholbar und darin ist wiederum Subfeld |9 wiederholbar</t>
+  </si>
+  <si>
+    <t>084 $2</t>
+  </si>
+  <si>
+    <t>Klassifikation, hier: bcl</t>
+  </si>
+  <si>
+    <t>084 $9</t>
+  </si>
+  <si>
+    <t>Titel der Klassifikation</t>
+  </si>
+  <si>
+    <t>3x 084 $2 = rvk</t>
+  </si>
+  <si>
+    <t>79.65 Lebenslanges Lernen
+81.92 Berufliche Weiterbildung</t>
+  </si>
+  <si>
+    <t>/vufind/Search/Results?lookfor=“Lebenslanges+Lernen“&amp;type=bklname</t>
+  </si>
+  <si>
+    <t>Gross, Herbert [VerfasserIn]</t>
+  </si>
+  <si>
+    <t>Beerbohm, Max (Sir, 1872-1956) [VerfasserIn]</t>
+  </si>
+  <si>
+    <t>Sherwood, Mary Martha (Mrs, 1775-1851) [VerfasserIn]</t>
+  </si>
+  <si>
+    <t>In: Kommunikation (1991), Seite 173-213</t>
+  </si>
+  <si>
+    <t>Sprache für die Arbeitswelt, 2017</t>
+  </si>
+  <si>
+    <t>Bibel, Luther</t>
+  </si>
+  <si>
+    <t>219 Bl. : graph. Darst.</t>
+  </si>
+  <si>
+    <t>Sekundäre Ausgabe</t>
+  </si>
+  <si>
+    <t>Anzeige der Reproduktionen und derer Umfang</t>
+  </si>
+  <si>
+    <t>Reproduction note</t>
+  </si>
+  <si>
+    <t>Reproduction</t>
+  </si>
+  <si>
+    <t>533 $a,$b,$c,$d,$e,$f,$n und $7</t>
+  </si>
+  <si>
+    <t>Enhält Daten aus Pica 4022 und 4068. Beide sind nicht wiederholbar.</t>
+  </si>
+  <si>
+    <t>Ticket #368</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Der Werktitel kann unter Marc 130 oder 240 vorkommen.
 240 wird nicht verwendet wenn 130 bereits belegt ist.
 240 ist wiederholbar.
@@ -2029,608 +2641,88 @@
     </r>
   </si>
   <si>
-    <t>130 $d</t>
-  </si>
-  <si>
-    <t>Date of treaty signing</t>
-  </si>
-  <si>
-    <t>130 $f</t>
-  </si>
-  <si>
-    <t>Date of a work</t>
-  </si>
-  <si>
-    <t>130 $g</t>
-  </si>
-  <si>
-    <t>Miscellaneus information</t>
-  </si>
-  <si>
-    <t>130 $h</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>130 $k</t>
-  </si>
-  <si>
-    <t>Form subheading</t>
-  </si>
-  <si>
-    <t>130 $l</t>
-  </si>
-  <si>
-    <t>Language of a work</t>
-  </si>
-  <si>
-    <t>130 $m</t>
-  </si>
-  <si>
-    <t>Medium of performance for music</t>
-  </si>
-  <si>
-    <t>130 $n</t>
-  </si>
-  <si>
-    <t>Number of part/section of a work</t>
-  </si>
-  <si>
-    <t>130 $o</t>
-  </si>
-  <si>
-    <t>Arranged statement for music</t>
-  </si>
-  <si>
-    <t>130 $p</t>
-  </si>
-  <si>
-    <t>Name of part/section of a work</t>
-  </si>
-  <si>
-    <t>130 $r</t>
-  </si>
-  <si>
-    <t>Key for music</t>
-  </si>
-  <si>
-    <t>130 $s</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>130 $t</t>
-  </si>
-  <si>
-    <t>Title of a work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">240 $a </t>
-  </si>
-  <si>
-    <t>240 $d</t>
-  </si>
-  <si>
-    <t>240 $f</t>
-  </si>
-  <si>
-    <t>240 $g</t>
-  </si>
-  <si>
-    <t>240 $h</t>
-  </si>
-  <si>
-    <t>240 $k</t>
-  </si>
-  <si>
-    <t>240 $l</t>
-  </si>
-  <si>
-    <t>240 $m</t>
-  </si>
-  <si>
-    <t>240 $n</t>
-  </si>
-  <si>
-    <t>240 $o</t>
-  </si>
-  <si>
-    <t>240 $p</t>
-  </si>
-  <si>
-    <t>240 $r</t>
-  </si>
-  <si>
-    <t>240 $s</t>
-  </si>
-  <si>
-    <t>240 $t</t>
-  </si>
-  <si>
-    <t>130 $a</t>
-  </si>
-  <si>
-    <t>Plein soleil</t>
-  </si>
-  <si>
-    <t>64430636X</t>
-  </si>
-  <si>
-    <t>The language of life &lt;dt.&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">878078703 </t>
-  </si>
-  <si>
-    <t>Tannöd</t>
-  </si>
-  <si>
-    <t>Le phénomène évangélique</t>
-  </si>
-  <si>
-    <t>130 $a, $f</t>
-  </si>
-  <si>
-    <t>89896363X</t>
-  </si>
-  <si>
-    <t>130 $a, $r</t>
-  </si>
-  <si>
-    <t>The original copy: photography of sculpture, 1839 to today, dt.</t>
-  </si>
-  <si>
-    <t>240 $a</t>
-  </si>
-  <si>
-    <t>Essentials of ecology</t>
-  </si>
-  <si>
-    <t>Wirtschaftsrecht, Arbeitsrecht, Sozialrecht
-Wirtschaft, Arbeit und Soziales</t>
-  </si>
-  <si>
-    <t>240 $a, $f</t>
-  </si>
-  <si>
-    <t>Aufgaben mit Lösungen zum Grundwissen Elektrotechnik, 2005
-Aufgaben mit Lösungen zur Elektrotechnik, 2008</t>
-  </si>
-  <si>
-    <t>240 $a (GND)</t>
-  </si>
-  <si>
-    <t>Der @Ehrentag</t>
-  </si>
-  <si>
-    <t>Umfang</t>
-  </si>
-  <si>
-    <t>Anzeige der Umfangsangaben</t>
-  </si>
-  <si>
-    <t>Physical Description</t>
-  </si>
-  <si>
-    <t>Physical description</t>
-  </si>
-  <si>
-    <t>Ticket #128</t>
-  </si>
-  <si>
-    <t>300 $a,$b,$c und $d</t>
-  </si>
-  <si>
-    <t>300 $a, $b, $c</t>
-  </si>
-  <si>
-    <t>12 S. : Ill., graph. Darst. ; 30 cm</t>
-  </si>
-  <si>
-    <t>300 2x$a, $b</t>
-  </si>
-  <si>
-    <t>300 $a, $c, $e</t>
-  </si>
-  <si>
-    <t>Online-Ressource</t>
-  </si>
-  <si>
-    <t>300 $c</t>
-  </si>
-  <si>
-    <t>30 cm</t>
-  </si>
-  <si>
-    <t>300 $a, $c</t>
-  </si>
-  <si>
-    <t>62 Bl ; 19 x 17 cm</t>
-  </si>
-  <si>
-    <t>300 $a, $e</t>
-  </si>
-  <si>
-    <t>6 S. ; Chorpartitur, 6 St.</t>
-  </si>
-  <si>
-    <t>1 Karte : farbig ; 56 x 58 cm, auf Blatt 60 x 76 cm, gefaltet 23 x 11 cm</t>
-  </si>
-  <si>
-    <t>1 DVD-Video (7 Min.) : s/w, stumm ; 12 cm</t>
-  </si>
-  <si>
-    <t>300 $a, $b, $c, $e</t>
-  </si>
-  <si>
-    <t>1 CD : digital ; 22 cm ; 1 Blatt</t>
-  </si>
-  <si>
-    <t>Fingerprint</t>
-  </si>
-  <si>
-    <t>Fingerprint bei alten Drucken mit Herkunftsangabe aus Pica-Feld 2275 mit Unterfeld $a</t>
-  </si>
-  <si>
-    <t>Fingerprint Identifier (Unparsed fingerprint, Institution to which field applies)</t>
-  </si>
-  <si>
-    <t>Ticket #149</t>
-  </si>
-  <si>
-    <t>026 $e $5</t>
-  </si>
-  <si>
-    <t>S.ME u-r- m-r- siRe 3 1700R (UFB Erfurt/Gotha; NLB Hannover; Bibliothek des Herzog Anton Ulrich-Museums Braunschweig; SBB-PK Berlin)</t>
-  </si>
-  <si>
-    <t>t,n, o-s- e-n- Dese C 1539A (SBB; ThULB Jena; Wartburg-Stiftung Eisenach)</t>
-  </si>
-  <si>
-    <t>026 $e, ohne $5</t>
-  </si>
-  <si>
-    <t>UMUM s.m, m.it quRe 3 1779R 1,1</t>
-  </si>
-  <si>
-    <t>Bibliographische Zitate</t>
-  </si>
-  <si>
-    <t>Anzeige des Felds Bibliografische Zitate (PICA-Feld 2277).
-Dient der Identifikation und dem Nachweis von alten Drucken und wird auch für die Suche verwendet.
-Anzeige des Felds:
-Bibliografische Zitate: 510a
-Bibliographic citations: 510a</t>
-  </si>
-  <si>
-    <t>Bibliographic (Name of source)</t>
-  </si>
-  <si>
-    <t>Bibliografische Zitate</t>
-  </si>
-  <si>
-    <t>Bibliographic citations</t>
-  </si>
-  <si>
-    <t>Ticket #150</t>
-  </si>
-  <si>
-    <t>510 $a</t>
-  </si>
-  <si>
-    <t>Bibliographisches Zitat</t>
-  </si>
-  <si>
-    <t>SBN On-line IT\ICCU\MODE\018621</t>
-  </si>
-  <si>
-    <t>VD17 3:009152Z</t>
-  </si>
-  <si>
-    <t>510 $a (wiederholt)</t>
-  </si>
-  <si>
-    <t>IG 1281 ; GW 12189 ; ISTC ih00015000 ; BSB-Ink H-41 ; H 8426</t>
-  </si>
-  <si>
-    <t>ISBN</t>
-  </si>
-  <si>
-    <t>International Standard Book Number</t>
-  </si>
-  <si>
-    <t>Ticket #170</t>
-  </si>
-  <si>
-    <t>020 $9</t>
-  </si>
-  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Darstellungsregel</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Verwende $9 statt $a für die Anzeige, weil es die vorlagetreue Schreibweise (mit den Bindestrichen) enthält.
-Anzeige:
+      <t xml:space="preserve">
+Die Daten werden in Vollanzeige nach der Zeile "Umfang" dargestellt.
 </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t>ISBN:</t>
+      <t>Deskriptorzeichen:</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> $9 : $c
-           $9 : $c
-020 ist wiederholbar. Wenn mehrfach belegt, ISBN untereinander anzeigen</t>
-    </r>
-  </si>
-  <si>
-    <t>020 $c</t>
-  </si>
-  <si>
-    <t>Terms of availability</t>
-  </si>
-  <si>
-    <t>$9</t>
-  </si>
-  <si>
-    <t>3-86025-284-4</t>
-  </si>
-  <si>
-    <t>$9 und $c</t>
-  </si>
-  <si>
-    <t>978-92-897-1568-3
-978-92-2-130471-5 : ILO
-978-92-897-1569-0 : web
-978-92-2-130472-2 : PDF</t>
-  </si>
-  <si>
-    <t>52680498X</t>
-  </si>
-  <si>
-    <t>3-540-69713-6 : EUR 29.95, sfr 46.00
-978-3-540-69713-8 : EUR 29.95, sfr 46.00
-978-3-540-69739-8</t>
-  </si>
-  <si>
-    <t>Falsche ISBN</t>
-  </si>
-  <si>
-    <t>Invalid ISBN</t>
-  </si>
-  <si>
-    <t>020 $z</t>
-  </si>
-  <si>
-    <t>Canceled/invalid ISBN</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">In Solr-Marc ist die falsche ISBN leider nur ohne "-" vorhanden.
-Anzeige:
+      <t xml:space="preserve">
+Komma und Leerzeichen ", "
 </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t>Falsche</t>
+      <t xml:space="preserve">
+Darstellungsregel: </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">
+533 $a(, $b)(, $c)(, $d)(, $e)(, $f)(, $n)(, $7)</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ISBN:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> $z
-</t>
-    </r>
-  </si>
-  <si>
-    <t>$z</t>
-  </si>
-  <si>
-    <t>9784540697138</t>
-  </si>
-  <si>
-    <t>9783643137173</t>
-  </si>
-  <si>
-    <t>ZDB-Nummer</t>
-  </si>
-  <si>
-    <t>Anzeige der ZDB-Nummer</t>
-  </si>
-  <si>
-    <t>System Control Number</t>
-  </si>
-  <si>
-    <t>ZDB-Number</t>
-  </si>
-  <si>
-    <t>Ticket #132</t>
-  </si>
-  <si>
-    <t>035 $a</t>
-  </si>
-  <si>
-    <t>1393051-5</t>
-  </si>
-  <si>
-    <t>Basisklassifikation</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Detailanzeige</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:
-Wenn 084 $2 rvk:
-084 $a
-Trennzeichen bei Wiederholungen von 084 mit $2 = rvk: _;_ (in Worten: Blank Semikolon Blank)
-Auf jede Notation einen </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Suchlink </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">legen: Indexsuche mit Inhalt von 084 $a in rvk_full
-</t>
-    </r>
-  </si>
-  <si>
-    <t>Other Classification Number</t>
-  </si>
-  <si>
-    <t>Sachgebiete</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Ticket #97</t>
-  </si>
-  <si>
-    <t>084 $a</t>
-  </si>
-  <si>
-    <t>Klassifikationsnummer</t>
-  </si>
-  <si>
-    <t>084 ist wiederholbar und darin ist wiederum Subfeld |9 wiederholbar</t>
-  </si>
-  <si>
-    <t>084 $2</t>
-  </si>
-  <si>
-    <t>Klassifikation, hier: bcl</t>
-  </si>
-  <si>
-    <t>084 $9</t>
-  </si>
-  <si>
-    <t>Titel der Klassifikation</t>
-  </si>
-  <si>
-    <t>3x 084 $2 = rvk</t>
-  </si>
-  <si>
-    <t>79.65 Lebenslanges Lernen
-81.92 Berufliche Weiterbildung</t>
-  </si>
-  <si>
-    <t>/vufind/Search/Results?lookfor=“Lebenslanges+Lernen“&amp;type=bklname</t>
-  </si>
-  <si>
-    <t>Gross, Herbert [VerfasserIn]</t>
-  </si>
-  <si>
-    <t>Beerbohm, Max (Sir, 1872-1956) [VerfasserIn]</t>
-  </si>
-  <si>
-    <t>Sherwood, Mary Martha (Mrs, 1775-1851) [VerfasserIn]</t>
-  </si>
-  <si>
-    <t>In: Kommunikation (1991), Seite 173-213</t>
-  </si>
-  <si>
-    <t>Sprache für die Arbeitswelt, 2017</t>
-  </si>
-  <si>
-    <t>Bibel, Luther</t>
-  </si>
-  <si>
-    <t>219 Bl. : graph. Darst.</t>
+  </si>
+  <si>
+    <t>533 $a, $e</t>
+  </si>
+  <si>
+    <t>Mikrofiche-Ausg., 3 Mikrofiches</t>
+  </si>
+  <si>
+    <t>62007003X</t>
+  </si>
+  <si>
+    <t>CD-ROM-Ausg.</t>
+  </si>
+  <si>
+    <t>533 $a</t>
+  </si>
+  <si>
+    <t>Online-Ausg., Springer eBook Collection. Earth and Environmental Science</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2707,6 +2799,17 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2904,7 +3007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3052,6 +3155,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6381,7 +6487,7 @@
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -6656,7 +6762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -7179,8 +7285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7269,257 +7375,257 @@
       <c r="B9" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C9" s="57" t="s">
-        <v>321</v>
+      <c r="C9" s="58" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="C11" s="57"/>
+      <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="58"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="C15" s="57"/>
+      <c r="C15" s="58"/>
     </row>
     <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="C16" s="57"/>
+      <c r="C16" s="58"/>
     </row>
     <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="58"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="C18" s="57"/>
+      <c r="C18" s="58"/>
     </row>
     <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="C19" s="57"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C20" s="57"/>
+      <c r="C20" s="58"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>344</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="C21" s="57"/>
+      <c r="C21" s="58"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="C22" s="57"/>
+      <c r="C22" s="58"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="57"/>
+      <c r="C23" s="58"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C24" s="57"/>
+      <c r="C24" s="58"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="C25" s="57"/>
+        <v>322</v>
+      </c>
+      <c r="C25" s="58"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="C26" s="57"/>
+        <v>324</v>
+      </c>
+      <c r="C26" s="58"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="C27" s="57"/>
+        <v>326</v>
+      </c>
+      <c r="C27" s="58"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C28" s="57"/>
+        <v>328</v>
+      </c>
+      <c r="C28" s="58"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="C29" s="57"/>
+        <v>330</v>
+      </c>
+      <c r="C29" s="58"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="C30" s="57"/>
+        <v>332</v>
+      </c>
+      <c r="C30" s="58"/>
     </row>
     <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="C31" s="57"/>
+        <v>334</v>
+      </c>
+      <c r="C31" s="58"/>
     </row>
     <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C32" s="57"/>
+        <v>336</v>
+      </c>
+      <c r="C32" s="58"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="C33" s="57"/>
+        <v>338</v>
+      </c>
+      <c r="C33" s="58"/>
     </row>
     <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="C34" s="57"/>
+        <v>340</v>
+      </c>
+      <c r="C34" s="58"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C35" s="57"/>
+        <v>342</v>
+      </c>
+      <c r="C35" s="58"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="C36" s="57"/>
+        <v>344</v>
+      </c>
+      <c r="C36" s="58"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="C37" s="57"/>
+        <v>346</v>
+      </c>
+      <c r="C37" s="58"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -7570,13 +7676,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B42" s="24">
         <v>772027102</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
@@ -7584,13 +7690,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B43" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>364</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>365</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -7598,13 +7704,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B44" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>366</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>367</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -7612,13 +7718,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B45" s="24">
         <v>774856556</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -7626,13 +7732,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B46" s="24">
         <v>147213592</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -7640,13 +7746,13 @@
     </row>
     <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="B47" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="B47" s="24" t="s">
-        <v>370</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="21"/>
@@ -7654,13 +7760,13 @@
     </row>
     <row r="48" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B48" s="24">
         <v>622487175</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="21"/>
@@ -7668,13 +7774,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B49" s="24">
         <v>859958280</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="21"/>
@@ -7682,13 +7788,13 @@
     </row>
     <row r="50" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B50" s="24">
         <v>871478110</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="21"/>
@@ -7696,13 +7802,13 @@
     </row>
     <row r="51" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B51" s="24">
         <v>881131350</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="21"/>
@@ -7710,13 +7816,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B52" s="24">
         <v>882661418</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21"/>
@@ -7750,7 +7856,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7763,7 +7869,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -7777,7 +7883,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -7791,7 +7897,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -7805,7 +7911,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7819,7 +7925,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -7833,7 +7939,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -7869,7 +7975,7 @@
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>247</v>
@@ -7922,13 +8028,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B13" s="24">
         <v>509133061</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -7936,13 +8042,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B14" s="24">
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -7950,13 +8056,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B15" s="24">
         <v>349876193</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -7964,13 +8070,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B16" s="24">
         <v>129495476</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -7978,13 +8084,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B17" s="24">
         <v>336079826</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
@@ -7992,13 +8098,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B18" s="24">
         <v>787199796</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="42"/>
@@ -8006,13 +8112,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B19" s="24">
         <v>872316203</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="42"/>
@@ -8020,13 +8126,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B20" s="24">
         <v>683536028</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="42"/>
@@ -8034,13 +8140,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="40" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B21" s="24">
         <v>826257127</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="42"/>
@@ -8062,6 +8168,248 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="62.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="131.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>476</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>477</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>480</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>485</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>483</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>484</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>485</v>
+      </c>
+      <c r="B14" s="24">
+        <v>1019909943</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>486</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>481</v>
+      </c>
+      <c r="B15" s="24">
+        <v>576971693</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>482</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>481</v>
+      </c>
+      <c r="B16" s="24">
+        <v>585243190</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>482</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -8075,7 +8423,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8089,7 +8437,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8103,7 +8451,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -8117,7 +8465,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -8131,7 +8479,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8145,7 +8493,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8181,10 +8529,10 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -8234,13 +8582,13 @@
     </row>
     <row r="13" spans="1:8" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B13" s="24">
         <v>151797196</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8248,13 +8596,13 @@
     </row>
     <row r="14" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B14" s="24">
         <v>770927416</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -8262,241 +8610,13 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B15" s="24">
         <v>194273989</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>409</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>416</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>417</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
-        <v>416</v>
-      </c>
-      <c r="B13" s="24">
-        <v>151797196</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>418</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-    </row>
-    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
-        <v>416</v>
-      </c>
-      <c r="B14" s="24">
-        <v>193804867</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>419</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-    </row>
-    <row r="15" spans="1:8" ht="114" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
-        <v>420</v>
-      </c>
-      <c r="B15" s="24">
-        <v>409606901</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -8517,6 +8637,234 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>415</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>416</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>415</v>
+      </c>
+      <c r="B13" s="24">
+        <v>151797196</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>417</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>415</v>
+      </c>
+      <c r="B14" s="24">
+        <v>193804867</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>418</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" ht="114" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>419</v>
+      </c>
+      <c r="B15" s="24">
+        <v>409606901</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>420</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -8531,7 +8879,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8543,7 +8891,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -8551,7 +8899,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -8559,7 +8907,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -8567,7 +8915,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -8579,7 +8927,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -8608,20 +8956,20 @@
     </row>
     <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>427</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>428</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="3"/>
@@ -8686,13 +9034,13 @@
     </row>
     <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B16" s="24">
         <v>187029679</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -8700,13 +9048,13 @@
     </row>
     <row r="17" spans="1:6" ht="171" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B17" s="24">
         <v>884572641</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -8714,223 +9062,17 @@
     </row>
     <row r="18" spans="1:6" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>433</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>434</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>440</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>433</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>441</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>440</v>
-      </c>
-      <c r="B16" s="24">
-        <v>885659430</v>
-      </c>
-      <c r="C16" s="55" t="s">
-        <v>442</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8953,6 +9095,212 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>439</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>440</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>439</v>
+      </c>
+      <c r="B16" s="24">
+        <v>885659430</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -8967,7 +9315,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8981,7 +9329,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8995,7 +9343,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -9009,7 +9357,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -9023,7 +9371,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -9037,7 +9385,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -9073,7 +9421,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -9124,13 +9472,13 @@
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -9150,7 +9498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -9165,7 +9513,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -9179,7 +9527,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -9193,7 +9541,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -9207,7 +9555,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -9221,7 +9569,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -9235,7 +9583,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -9271,13 +9619,13 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>455</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>456</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="C9" s="60" t="s">
         <v>457</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>458</v>
       </c>
       <c r="D9" s="38"/>
       <c r="F9" s="3"/>
@@ -9286,12 +9634,12 @@
     </row>
     <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>459</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>460</v>
-      </c>
-      <c r="C10" s="59"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="38"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -9299,12 +9647,12 @@
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
+        <v>460</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>461</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>462</v>
-      </c>
-      <c r="C11" s="59"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="38"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
@@ -9352,18 +9700,18 @@
     </row>
     <row r="15" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B15" s="24">
         <v>868759473</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
       <c r="F15" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -9485,7 +9833,7 @@
       <c r="B9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="58" t="s">
         <v>53</v>
       </c>
     </row>
@@ -9496,7 +9844,7 @@
       <c r="B10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -9505,7 +9853,7 @@
       <c r="B11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="57"/>
+      <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -9514,7 +9862,7 @@
       <c r="B12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -9523,7 +9871,7 @@
       <c r="B13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -9532,7 +9880,7 @@
       <c r="B14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="58"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9591,7 +9939,7 @@
         <v>521722950</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -9605,7 +9953,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -9619,7 +9967,7 @@
         <v>725223227</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -9777,7 +10125,7 @@
       <c r="B9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="58" t="s">
         <v>80</v>
       </c>
     </row>
@@ -9788,7 +10136,7 @@
       <c r="B10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -9797,7 +10145,7 @@
       <c r="B11" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="57"/>
+      <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -9806,7 +10154,7 @@
       <c r="B12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -9815,7 +10163,7 @@
       <c r="B13" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -9824,7 +10172,7 @@
       <c r="B14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="58"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -9834,7 +10182,7 @@
       <c r="B15" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="57"/>
+      <c r="C15" s="58"/>
       <c r="F15" s="26" t="s">
         <v>91</v>
       </c>
@@ -9842,22 +10190,22 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="57"/>
+      <c r="C16" s="58"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="57"/>
+      <c r="C17" s="58"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C18" s="57"/>
+      <c r="C18" s="58"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C19" s="57"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C20" s="57"/>
+      <c r="C20" s="58"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C21" s="57"/>
+      <c r="C21" s="58"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -10108,7 +10456,7 @@
       <c r="B9" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="59" t="s">
         <v>109</v>
       </c>
       <c r="E9" s="27"/>
@@ -10120,7 +10468,7 @@
       <c r="B10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="59"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -10129,7 +10477,7 @@
       <c r="B11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="59"/>
     </row>
     <row r="12" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -10138,7 +10486,7 @@
       <c r="B12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="58"/>
+      <c r="C12" s="59"/>
     </row>
     <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -10147,7 +10495,7 @@
       <c r="B13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="58"/>
+      <c r="C13" s="59"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.2">
@@ -10157,7 +10505,7 @@
       <c r="B14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="58"/>
+      <c r="C14" s="59"/>
       <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
@@ -10167,7 +10515,7 @@
       <c r="B15" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="59"/>
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -10176,7 +10524,7 @@
       <c r="B16" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="59"/>
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -10185,7 +10533,7 @@
       <c r="B17" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="58"/>
+      <c r="C17" s="59"/>
     </row>
     <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -10194,7 +10542,7 @@
       <c r="B18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="58"/>
+      <c r="C18" s="59"/>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -10203,7 +10551,7 @@
       <c r="B19" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="59"/>
     </row>
     <row r="20" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -10212,7 +10560,7 @@
       <c r="B20" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="58"/>
+      <c r="C20" s="59"/>
     </row>
     <row r="21" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -10221,7 +10569,7 @@
       <c r="B21" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="58"/>
+      <c r="C21" s="59"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>

</xml_diff>

<commit_message>
Removed subfield $7 from reproduction information. Updated rda.xlsx. refs #369
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vagrant\vf5.1\vufind\module\ThULB\tests\fixtures\spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fe57gop\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="29040" windowHeight="15675" tabRatio="992" firstSheet="9" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="29040" windowHeight="15675" tabRatio="992" firstSheet="12" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -798,9 +798,6 @@
     <t>100 $a, $b, $c und $4</t>
   </si>
   <si>
-    <t>Benedikt XVI. (Papst) [InterviewteR]</t>
-  </si>
-  <si>
     <t>Benedikt XVI. (Papst) [Interviewee]</t>
   </si>
   <si>
@@ -1759,9 +1756,6 @@
   </si>
   <si>
     <t>240 $a (GND)</t>
-  </si>
-  <si>
-    <t>Der @Ehrentag</t>
   </si>
   <si>
     <t>Umfang</t>
@@ -2707,6 +2701,12 @@
 "Reprint der Schreibkalender &amp;#039;Almanach&amp;#039; für 1544 und 1545 von Georg Seyfridt" (Impressum)
 Die Vorlage enthält insgesamt 3 Werke.
 Vorlagen: Exemplare der Ratsschulbibliothek Zwickau (Sign.: 22.9.15.(33) und (35))</t>
+  </si>
+  <si>
+    <t>Benedikt XVI. (Papst, 1927-) [InterviewteR]</t>
+  </si>
+  <si>
+    <t>Der Ehrentag</t>
   </si>
 </sst>
 </file>
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4769,7 +4769,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -4777,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -4785,7 +4785,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -4793,7 +4793,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4805,7 +4805,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -4831,13 +4831,13 @@
     </row>
     <row r="9" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="23" t="s">
         <v>175</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -4888,13 +4888,13 @@
     </row>
     <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="C14" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>179</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -4902,13 +4902,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>180</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>181</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -4916,13 +4916,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B16" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>182</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>183</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -4963,7 +4963,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4976,7 +4976,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -4984,7 +4984,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
@@ -4992,7 +4992,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
@@ -5000,7 +5000,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -5013,7 +5013,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="23"/>
@@ -5082,13 +5082,13 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="C13" s="19" t="s">
         <v>191</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>192</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -5096,13 +5096,13 @@
     </row>
     <row r="14" spans="1:8" ht="114" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" s="24">
         <v>617248613</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -5110,13 +5110,13 @@
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="24">
         <v>881353434</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -5124,13 +5124,13 @@
     </row>
     <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B16" s="24">
         <v>839489048</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -5167,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5181,7 +5181,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5195,7 +5195,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5209,7 +5209,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -5223,7 +5223,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -5237,7 +5237,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5273,7 +5273,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -5324,13 +5324,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B13" s="24">
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -5365,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5379,7 +5379,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5393,7 +5393,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5407,7 +5407,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -5421,7 +5421,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -5435,7 +5435,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5471,7 +5471,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -5522,13 +5522,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="24">
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -5563,7 +5563,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5577,7 +5577,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5591,7 +5591,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5605,7 +5605,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -5619,7 +5619,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -5633,7 +5633,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5669,7 +5669,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -5720,13 +5720,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B13" s="24">
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -5761,7 +5761,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5775,7 +5775,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5789,7 +5789,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -5803,7 +5803,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -5817,7 +5817,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -5831,7 +5831,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -5867,10 +5867,10 @@
     </row>
     <row r="9" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>223</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>224</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
@@ -5920,13 +5920,13 @@
     </row>
     <row r="13" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -5961,7 +5961,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -5975,7 +5975,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5989,7 +5989,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6003,7 +6003,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -6017,7 +6017,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -6031,7 +6031,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6067,10 +6067,10 @@
     </row>
     <row r="9" spans="1:8" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>231</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>232</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
@@ -6120,13 +6120,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -6134,13 +6134,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" s="24">
         <v>502081112</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -6175,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6188,7 +6188,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -6196,7 +6196,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
@@ -6204,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
@@ -6212,7 +6212,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6225,7 +6225,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6255,7 +6255,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="23"/>
@@ -6294,13 +6294,13 @@
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B13" s="24">
         <v>804999864</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -6308,13 +6308,13 @@
     </row>
     <row r="14" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14" s="24">
         <v>773516468</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -6358,7 +6358,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6371,7 +6371,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -6379,7 +6379,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -6387,7 +6387,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -6395,7 +6395,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6408,7 +6408,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6438,7 +6438,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="23"/>
@@ -6477,13 +6477,13 @@
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="24">
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -6491,13 +6491,13 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B14" s="24">
         <v>876614268</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -6505,13 +6505,13 @@
     </row>
     <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B15" s="24">
         <v>894531530</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -6545,7 +6545,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6557,7 +6557,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6565,7 +6565,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6573,7 +6573,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6581,7 +6581,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6593,7 +6593,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -6618,18 +6618,18 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>260</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -6638,10 +6638,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -6650,7 +6650,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>0</v>
@@ -6708,13 +6708,13 @@
     </row>
     <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B17" s="24">
         <v>130559555</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -6722,13 +6722,13 @@
     </row>
     <row r="18" spans="1:6" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B18" s="24">
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -6896,7 +6896,7 @@
         <v>877327637</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -6924,7 +6924,7 @@
         <v>873533267</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -6964,7 +6964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -6978,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6990,7 +6990,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6998,7 +6998,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7006,7 +7006,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7014,7 +7014,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7026,7 +7026,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -7053,42 +7053,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="23" t="s">
         <v>271</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="301.5" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="B10" s="48" t="s">
-        <v>274</v>
-      </c>
       <c r="C10" s="33" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>275</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>276</v>
       </c>
       <c r="C11" s="49"/>
       <c r="F11" s="50"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>278</v>
       </c>
       <c r="C12" s="49"/>
       <c r="E12" s="3"/>
@@ -7096,10 +7096,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>279</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>280</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="51"/>
@@ -7108,10 +7108,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="51"/>
@@ -7120,10 +7120,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15" s="49"/>
       <c r="D15" s="51"/>
@@ -7132,10 +7132,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="51"/>
@@ -7144,10 +7144,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="51"/>
@@ -7156,10 +7156,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="51"/>
@@ -7168,10 +7168,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>281</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>282</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="3"/>
@@ -7180,10 +7180,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>283</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>284</v>
       </c>
       <c r="C20" s="52"/>
       <c r="D20" s="3"/>
@@ -7238,13 +7238,13 @@
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B25" s="24">
         <v>129993549</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -7252,13 +7252,13 @@
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B26" s="24">
         <v>129494860</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -7266,13 +7266,13 @@
     </row>
     <row r="27" spans="1:6" ht="114" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B27" s="24">
         <v>129292834</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -7280,13 +7280,13 @@
     </row>
     <row r="28" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B28" s="24">
         <v>329875515</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -7294,13 +7294,13 @@
     </row>
     <row r="29" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B29" s="24">
         <v>888820720</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -7330,8 +7330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7341,7 +7341,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7353,7 +7353,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -7361,7 +7361,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -7369,7 +7369,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -7377,7 +7377,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7389,7 +7389,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -7415,129 +7415,129 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>294</v>
-      </c>
       <c r="C9" s="64" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>295</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>296</v>
       </c>
       <c r="C10" s="64"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>297</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>298</v>
       </c>
       <c r="C11" s="64"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>299</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>300</v>
       </c>
       <c r="C12" s="64"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>301</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>302</v>
       </c>
       <c r="C13" s="64"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>303</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>304</v>
       </c>
       <c r="C14" s="64"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>305</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>306</v>
       </c>
       <c r="C15" s="64"/>
     </row>
     <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>307</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>308</v>
       </c>
       <c r="C16" s="64"/>
     </row>
     <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>310</v>
       </c>
       <c r="C17" s="64"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>312</v>
       </c>
       <c r="C18" s="64"/>
     </row>
     <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>314</v>
       </c>
       <c r="C19" s="64"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>315</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>316</v>
       </c>
       <c r="C20" s="64"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>317</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>318</v>
       </c>
       <c r="C21" s="64"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="C22" s="64"/>
     </row>
@@ -7548,127 +7548,127 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C24" s="64"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="64"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C26" s="64"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C27" s="64"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C28" s="64"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C29" s="64"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C30" s="64"/>
     </row>
     <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C31" s="64"/>
     </row>
     <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C32" s="64"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C33" s="64"/>
     </row>
     <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C34" s="64"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C35" s="64"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C36" s="64"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C37" s="64"/>
       <c r="F37" s="26"/>
@@ -7721,13 +7721,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B42" s="24">
         <v>772027102</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
@@ -7735,13 +7735,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B43" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>337</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>338</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -7749,13 +7749,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B44" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>339</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>340</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -7763,13 +7763,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B45" s="24">
         <v>774856556</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -7777,13 +7777,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B46" s="24">
         <v>147213592</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -7791,13 +7791,13 @@
     </row>
     <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="B47" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="B47" s="24" t="s">
-        <v>343</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="21"/>
@@ -7805,13 +7805,13 @@
     </row>
     <row r="48" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B48" s="24">
         <v>622487175</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="21"/>
@@ -7819,13 +7819,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B49" s="24">
         <v>859958280</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="21"/>
@@ -7833,13 +7833,13 @@
     </row>
     <row r="50" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B50" s="24">
         <v>871478110</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="21"/>
@@ -7847,13 +7847,13 @@
     </row>
     <row r="51" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B51" s="24">
         <v>881131350</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="21"/>
@@ -7861,13 +7861,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B52" s="24">
         <v>882661418</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>352</v>
+        <v>504</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21"/>
@@ -7914,7 +7914,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -7928,7 +7928,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -7942,7 +7942,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -7956,7 +7956,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7970,7 +7970,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -7984,7 +7984,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8020,10 +8020,10 @@
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
@@ -8073,13 +8073,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B13" s="24">
         <v>509133061</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8087,13 +8087,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B14" s="24">
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -8101,13 +8101,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B15" s="24">
         <v>349876193</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -8115,13 +8115,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B16" s="24">
         <v>129495476</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -8129,13 +8129,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B17" s="24">
         <v>336079826</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
@@ -8143,13 +8143,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B18" s="24">
         <v>787199796</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="42"/>
@@ -8157,13 +8157,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="40" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B19" s="24">
         <v>872316203</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="42"/>
@@ -8171,13 +8171,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="40" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B20" s="24">
         <v>683536028</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="42"/>
@@ -8185,13 +8185,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="40" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B21" s="24">
         <v>826257127</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="42"/>
@@ -8230,7 +8230,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8238,7 +8238,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8246,7 +8246,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -8254,7 +8254,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -8262,7 +8262,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -8270,7 +8270,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -8300,13 +8300,13 @@
     </row>
     <row r="9" spans="1:9" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D9" s="59"/>
       <c r="F9" s="3"/>
@@ -8355,13 +8355,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8369,13 +8369,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B14" s="24">
         <v>1019909943</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -8383,13 +8383,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B15" s="24">
         <v>576971693</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -8397,13 +8397,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B16" s="24">
         <v>585243190</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -8430,7 +8430,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8444,7 +8444,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8458,7 +8458,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -8472,7 +8472,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -8486,7 +8486,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8500,7 +8500,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8536,10 +8536,10 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -8589,13 +8589,13 @@
     </row>
     <row r="13" spans="1:8" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B13" s="24">
         <v>151797196</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8603,13 +8603,13 @@
     </row>
     <row r="14" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B14" s="24">
         <v>770927416</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -8617,13 +8617,13 @@
     </row>
     <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B15" s="24">
         <v>194273989</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -8658,7 +8658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8672,7 +8672,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8686,7 +8686,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -8700,7 +8700,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -8714,7 +8714,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8728,7 +8728,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8764,10 +8764,10 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -8817,13 +8817,13 @@
     </row>
     <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B13" s="24">
         <v>151797196</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8831,13 +8831,13 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B14" s="24">
         <v>193804867</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -8845,13 +8845,13 @@
     </row>
     <row r="15" spans="1:8" ht="114" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B15" s="24">
         <v>409606901</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -8886,7 +8886,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8898,7 +8898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -8906,7 +8906,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -8914,7 +8914,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -8922,7 +8922,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -8934,7 +8934,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -8963,20 +8963,20 @@
     </row>
     <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="3"/>
@@ -9041,13 +9041,13 @@
     </row>
     <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B16" s="24">
         <v>187029679</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -9055,13 +9055,13 @@
     </row>
     <row r="17" spans="1:6" ht="171" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B17" s="24">
         <v>884572641</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -9069,13 +9069,13 @@
     </row>
     <row r="18" spans="1:6" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>406</v>
-      </c>
       <c r="C18" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -9116,7 +9116,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9128,7 +9128,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
@@ -9136,7 +9136,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -9144,7 +9144,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
@@ -9152,7 +9152,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -9164,7 +9164,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -9193,13 +9193,13 @@
     </row>
     <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>410</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>412</v>
       </c>
       <c r="D9" s="10"/>
     </row>
@@ -9261,13 +9261,13 @@
     </row>
     <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -9275,13 +9275,13 @@
     </row>
     <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B16" s="24">
         <v>885659430</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -9322,7 +9322,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -9336,7 +9336,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -9350,7 +9350,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -9364,7 +9364,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -9378,7 +9378,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -9392,7 +9392,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -9428,7 +9428,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -9479,13 +9479,13 @@
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -9520,7 +9520,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -9534,7 +9534,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -9548,7 +9548,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -9562,7 +9562,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -9576,7 +9576,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -9590,7 +9590,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -9626,13 +9626,13 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>427</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>428</v>
+      </c>
+      <c r="C9" s="65" t="s">
         <v>429</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>430</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>431</v>
       </c>
       <c r="D9" s="38"/>
       <c r="F9" s="3"/>
@@ -9641,10 +9641,10 @@
     </row>
     <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C10" s="65"/>
       <c r="D10" s="38"/>
@@ -9654,10 +9654,10 @@
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C11" s="65"/>
       <c r="D11" s="38"/>
@@ -9707,18 +9707,18 @@
     </row>
     <row r="15" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B15" s="24">
         <v>868759473</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
       <c r="F15" s="43" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -9743,7 +9743,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9842,7 +9842,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -9899,50 +9899,50 @@
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C16" s="62"/>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C17" s="62"/>
       <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="62"/>
       <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="62"/>
       <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="62"/>
       <c r="I20" s="28"/>
@@ -10015,10 +10015,10 @@
         <v>521722950</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
@@ -10031,10 +10031,10 @@
         <v>63</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
@@ -10047,10 +10047,10 @@
         <v>725223227</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
@@ -10063,26 +10063,26 @@
         <v>860726789</v>
       </c>
       <c r="C30" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>66</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="24">
         <v>797315829</v>
       </c>
       <c r="C31" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
@@ -10128,7 +10128,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -10141,7 +10141,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -10149,7 +10149,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -10157,7 +10157,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -10165,7 +10165,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -10180,7 +10180,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -10207,54 +10207,54 @@
     </row>
     <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="C9" s="64" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="C10" s="64"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="C11" s="64"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="C12" s="64"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="C13" s="64"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>58</v>
@@ -10264,7 +10264,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>60</v>
@@ -10280,46 +10280,46 @@
     </row>
     <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C17" s="64"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C18" s="64"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="64"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="64"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="64"/>
     </row>
@@ -10379,61 +10379,61 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="24">
         <v>848323173</v>
       </c>
       <c r="C30" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>89</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>90</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B31" s="24">
         <v>520959078</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B32" s="24">
         <v>1005410313</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B33" s="24">
         <v>657009032</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="21"/>
@@ -10441,48 +10441,48 @@
     </row>
     <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>471</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>473</v>
-      </c>
       <c r="D34" s="20" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B35" s="24">
         <v>875683843</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B36" s="24">
         <v>867529938</v>
       </c>
       <c r="C36" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>87</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="22"/>
@@ -10533,7 +10533,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -10554,7 +10554,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -10562,7 +10562,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -10570,7 +10570,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -10613,19 +10613,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="63" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>96</v>
       </c>
       <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>52</v>
@@ -10634,7 +10634,7 @@
     </row>
     <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>54</v>
@@ -10643,7 +10643,7 @@
     </row>
     <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>56</v>
@@ -10652,7 +10652,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>60</v>
@@ -10662,7 +10662,7 @@
     </row>
     <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>58</v>
@@ -10672,52 +10672,52 @@
     </row>
     <row r="15" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="63"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="63"/>
     </row>
     <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="63"/>
     </row>
     <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="63"/>
     </row>
     <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>58</v>
@@ -10726,7 +10726,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>60</v>
@@ -10786,29 +10786,29 @@
     </row>
     <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="C26" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>112</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -10816,13 +10816,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="C28" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -10830,29 +10830,29 @@
     </row>
     <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B29" s="29">
         <v>860726789</v>
       </c>
       <c r="C29" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>120</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="29">
         <v>657009032</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="21"/>
@@ -10860,13 +10860,13 @@
     </row>
     <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="24">
         <v>797315829</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="21"/>
@@ -10910,7 +10910,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -10923,7 +10923,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -10931,7 +10931,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -10939,7 +10939,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -10947,7 +10947,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -10960,7 +10960,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10992,23 +10992,23 @@
     </row>
     <row r="9" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="23" t="s">
         <v>132</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>133</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -11018,10 +11018,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -11031,10 +11031,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -11092,13 +11092,13 @@
     </row>
     <row r="17" spans="1:6" ht="114" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="24">
         <v>881131490</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -11139,7 +11139,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -11153,7 +11153,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -11167,7 +11167,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -11181,7 +11181,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -11195,7 +11195,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -11209,7 +11209,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -11245,7 +11245,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -11296,16 +11296,16 @@
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="24">
         <v>786233990</v>
       </c>
       <c r="C13" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>149</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="43"/>
@@ -11339,7 +11339,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -11353,7 +11353,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -11367,7 +11367,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -11381,7 +11381,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -11395,7 +11395,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -11409,7 +11409,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -11445,7 +11445,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -11496,13 +11496,13 @@
     </row>
     <row r="13" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="24">
         <v>786233990</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -11510,13 +11510,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" s="24">
         <v>569359759</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -11524,13 +11524,13 @@
     </row>
     <row r="15" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="24">
         <v>849562740</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -11568,7 +11568,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -11582,7 +11582,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -11596,7 +11596,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -11610,7 +11610,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -11624,7 +11624,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -11638,7 +11638,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -11674,10 +11674,10 @@
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>165</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>166</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
@@ -11727,13 +11727,13 @@
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="24">
         <v>728470527</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -11741,13 +11741,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" s="24">
         <v>855352329</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -11755,13 +11755,13 @@
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="24">
         <v>537824324</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>

</xml_diff>

<commit_message>
Changed table of contents in detail view. Display values from field 501, too. Added unit test. refs #372
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\AG Discovery\Redmine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vagrant\vf5.1\vufind\module\ThULB\tests\fixtures\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="22" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <sheet name="Basisklassifikation" sheetId="28" r:id="rId31"/>
     <sheet name="Inhaltsangaben" sheetId="30" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -508,7 +508,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="581">
   <si>
     <t>Titel</t>
   </si>
@@ -2748,14 +2748,6 @@
 Ungezählte Beil.: The genome directory; The yeast genome directory; Suppl.; Produktschau für Deutschland; Science in Spain; Science in Latin America; Nature net guide; Nature jobs; Science &amp; technology networks in Scandinavia; Nature outlook; Nature insight; Nature publishing index.</t>
   </si>
   <si>
-    <t>Abweichender Titel auf der Vorderseite des vorderen Banddeckels: Almanach für 1544 und 1545
-Abweichender Titel: Georg Seyfridt 1544 und 1545
-Abweichender Titel: Almanach für 1544 und 1545
-"Reprint der Schreibkalender &amp;#039;Almanach&amp;#039; für 1544 und 1545 von Georg Seyfridt" (Impressum)
-Die Vorlage enthält insgesamt 3 Werke.
-Vorlagen: Exemplare der Ratsschulbibliothek Zwickau (Sign.: 22.9.15.(33) und (35))</t>
-  </si>
-  <si>
     <t>Benedikt XVI. (Papst, 1927-) [InterviewteR]</t>
   </si>
   <si>
@@ -2825,78 +2817,12 @@
     <t>Machine generated contents note:Introduction 1. What is Testimony? 2. The Testimonial Conundrum 3. Testimony, Perception, Memory, and Inference 4. Testimony and Evidence 5. Reductionism and Anti-Reductionism 6. Hybrid Theories of Testimony 7. Testimonial Knowledge: Transmission and Generation 8. Trust and Assurance 9. Expert Testimony 10. Pathologies of Testimony 11. Testimony and the Value of Knowledge Glossary Bibliography Index.</t>
   </si>
   <si>
-    <t xml:space="preserve">Dritte Gewalt im Wandel : veränderte Anforderungen an Legitimität und Effektivität? / Fabian Wittreck; Frauke Brosius-Gersdorf
-Gestaltung des demographischen Wandels als Verwaltungsaufgabe / Jan Ziekow; Stephan Rixen
-Sicherung grund- und menschenrechtlicher Standards gegenüber neuen Gefährdungen durch private und ausländische Akteure / Thilo Marauhn; Magdalena Pöschl
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> XV. Vorgeschichte der slavischen Sprachen und Sprachkontakt /Prehistory of the Slavic Languages and Language Contact; 82. Georg Holzer, Vorhistorische Periode / Prehistoric Period; 83. Jürgen Udolph, Ethnogenese und Urheimat der Slaven / Ethnogenesis and 'Urheimat' of the Slavs; 84. William R. Schmalstieg, Baltoslavic / Baltoslavisch
-85. Heinz Schuster-Šewc, Der Zerfall der slavischen Spracheinheit (des Urslavischen) und die genetische Gliederung der slavischen Sprachen / The Decay of the Slavic Language Unit (of Proto-Slavic) and the Genetic Structure of the Slavic languages Heinz Schuster-Šewc86. Jerzy Bartminski, Basic Assumptions of Slavic Ethnolinguistics / Grundannahmen der slavischen Ethnolinguistik; 87. Walter Breu, Substrate auf slavischem Sprachgebiet (Südslavisch) / Substrates in Slavic language area (South Slavonic)
-88. Harald Haarmann, Finnougrisch-slavische Sprachkontakte / Finno Ugric-Slavic Language Contacts89. Stanislaw Stachowski, Türkischer Einfluss auf den slavischen Wortschatz / Turkish Influence on the Slavic Vocabulary; XVI. Altkirchenslavisch und Kirchenslavisch Old Church Slavonic and Church Slavonic; 90 Helmut Keipert, Kirchenslavisch-Begriffe / Conceptions of Church Slavonic; 91. Heinz Miklas/Velizar Sadovski, Die Struktur des Altkirchenslavischen / The Structure of Old Church Slavonic; 92. Viktor M. Živov (†), Das Kirchenslavische bei den Ostslaven / Church Slavonic among the East Slavs
-93. Johannes Reinhart, Das Kroatisch-Kirchenslavische / Croatian Church Slavonic94. Giorgio Ziffer, Slavia orthodoxa und Slavia romana / Slavia Orthodoxa and Slavia Romana; 95. Nikolaos Trunte, Neukirchenslavisch / New Church Slavonic; 96. Roland Marti, Wirkungsgeschichte des Kirchenslavischen / The Impact of Church Slavonic and its History; 97. Ivan Bujukliev, Sprachbewusstsein bei den orthodoxen Slaven / Language Awareness among the Orthodox Slavs; XVII. Frühe volkssprachliche Überlieferungen Early Vernacular Development
-98. Vadim B. Krys'ko, Frühe volkssprachliche Entwicklung: Das Altostslavische / Early vernacular Development: Old East Slavic99. Juliane Besters-Dilger, Frühe volkssprachliche Entwicklung: Russische Kanzleisprache des 16. und 17. Jahrhunderts / Early vernacular development: Russian firm language of the 16th and 17th century
-100. Michael Moser, Frühe volkssprachliche Entwicklung auf dem Gebiet der heutigen Ukraine und Weißrusslands: Das Mittelukrainische und Mittelweißrussische / Early vernacular development in the area of today's Ukraine and Byelorussia: Middle Ukrainian and Middle White Russian
-100. Frühe volkssprachliche Entwicklung auf dem Gebiet der heutigen Ukraine und Weißrusslands: Das Mittelukrainische und Mittelweißrussische / Early vernacular development in the area of today’s Ukraine and Byelorussia: Middle Ukrainian and Middle White Russian / Moser, Michael
-122. Goals, Tasks, and Lessons of Historical Syntax / Ziele und Aufgaben der historischen Syntax / Timberlake, Alan
-101. Frühe volkssprachliche Entwicklung: Tschechisch / Early vernacular development: Czech / Šlosar, Dušan
-102. Frühe volkssprachliche Entwicklung: Kroatisch / Early vernacular development: Croatian / Wirtz, Gudrun
-103. Frühe volkssprachliche Entwicklung: Slovenisch / Early vernacular development: Slovenian / Seitz Shewmon, Elisabeth
-104. Polabian / Polabisch / Polański, Kazimierz
-105. Herausbildung der Standardsprachen: Ukrainisch und Weißrussisch / History of the Standard Language: Ukrainian and Belarusian / Bieder, Hermann
-106. History of Standard Languages: Slovak / Herausbildung der Standardsprache: Slovakisch / Žigo, Pavol
-107. Herausbildung der Standardsprache: Slovenisch / History of the Standard Language: Slovenian / Herrity, Peter
-108. Herausbildung der Standardsprache bei Serben und Kroaten / History of the Standard Language: Serbian and Croatian / Lehfeldt, Werner
-109. Formation of the Standard Language: Macedonian / Herausbildung der Standardsprache: Makedonisch / Hill, Peter M.
-110. Herausbildung der Standardsprache: Sorbisch / Formation of the Standard Language: Sorbian / Schuster-Šewc, Heinz
-111. Projekte einer gemeinslavischen Schriftsprache / Projects of planned Languages for the Slavs / Ivanova, Diana
-112. Historische Graphematik des Slavischen: Glagolitische und kyrillische Schrift / Historical Graphemics of the Slavic Languages: the Glagolitic and Cyrillic Writing Systems / Marti, Roland
-113. History and Development of the Latin Writing System in the Slavic Languages / Geschichte und Entwicklung der lateinischen Schrift in den slavischen Sprachen / Kučera, Karel
-114. Diachrone Phonologie / Diachronic Phonology / Stadnik-Holzer, Elena
-115. Introduction to Slavic Historical Morphology: Slavic Noun Classes / Die Entwicklung der Morphologie (Nominalklassen) im Slavischen / Janda, Laura A.
-116. Evolution of Verb Classes in Slavic / Die Entwicklung der Verbalklassen im Slavischen / Townsend, Charles E.
-117. Historical Development of Slavic Inflectional Accent / Die historische Entwicklung des slavischen Flexionsakzentes / Baerman, Matthew
-118. Entstehung der Kategorie der Belebtheit/Personalität / The Development of the Grammatical Category of Animacy / Krys’ko, Vadim B.
-119. Definiteness (Diachrony) / Bestimmtheit (Diachronie) / Topolińska, Zuzana
-120. Umbau des Tempussystems / The Reconstruction of the Temporal System / Klimonow, Wladimir D.
-121. Umbau des Partizipialsystems / The Reconstruction of the Participal System / Wiemer, Björn.
-123. The Simple Sentence / Der einfache Satz / Timberlake, Alan
-124. Erweiterung des einfachen Satzes / Extension of the Simple Sentence / Večerka, Radoslav
-125. Complex Sentence: Parataxis / Zusammengesetzter Satz: Parataxe / Klenin, Emily
-126. Complex Sentence: Hypotaxis / Zusammengesetzter Satz: Hypotaxe / Klenin, Emily
-127. Jüngere Lehnwortschatzschichten der slavischen Sprachen / Younger Loanword Strata in the Slavic Languages / Otten, Fred
-128. Westeuropäische Einflüsse in der Wortbildung / Western European Influences in Word Formation / Mengel, Swetlana
-129. Ausgewählte lexikalisch-semantische Gruppen / Selected lexical-semantic groups (Colour Terms, Kinship Terms) / Hill, Peter M.
-130. Phänomene der historischen Phraseologie der slavischen Sprachen / Phenomena of Historical Phraseology in the Slavic Languages / Bierich, Alexander
-131. Slavische Grammatikschreibung / Slavonic Grammaticography / Daiber, Thomas
-132. Grammatikschreibung bei den Tschechen und Slowaken bis zur Aufklärung / Czech and Slovak Grammaticography Before the Enlightenment / Čejka, Mirek
-133. Grammatikschreibung bei den Slowenen / Slovene Grammaticography / Hammel, Robert
-134. Grammatikschreibung bei den Bulgaren zwischen 1835 und 1944 / Grammaticography among the Bulgarians between 1835 and 1944 / Hammel, Robert
-135. Grammatikschreibung bei den Polen bis zur Aufklärung / Polish Grammaticography Before the Enlightenment / Bugajski, Marian
-136. Grammatikschreibung bei den Sorben (bis zum Ende d. 19. Jh.s) / Sorbian Grammaticography (Before the End of the 19th Century) / Wölke, Sonja
-137. Grammatiken der russischen Standardsprache / Grammars of the Russian Standard Language / Wingender, Monika
-138. Grammatiken der ukrainischen und der weißrussischen Standardsprache / Grammars of the Ukrainian and Belarusian Standard Languages / Bieder, Hermann
-139. Grammars of Polish From the 19th and 20th Century / Bugajski, Marian
-140. Dialektlexikographie / Dialect Lexicography / Neweklowsky, Gerhard
-141. Phraseographie / Phraseography / Worbs, Erika
-142. Typen slavischer Standardsprachen / Types of Slavic Standard Languages / Wingender, Monika
-143. Rechtlicher und faktischer Status slavischer Standardsprachen und Sprachenkonflikte / Legal and Factual Status of Slavic Standard Languages and Language Conflicts / Marti, Roland
-144. Sprach(en)politik in Ländern mit slavischer Mehrheitssprache / Language Politics in Countries with a Slavic Majority Language / Lubaś, Władysław.
-</t>
-  </si>
-  <si>
     <t>Der Roman des Freiherrn von Vieren / Adelbert von Chamisso, Friedrich de la Motte Fouqué, Karl Wilhelm Salice-Contessa
 Das Bild der Mutter / Karl Wilhelm Salice-Contessa
 Die Doppelgänger / E.T.A. Hoffmann</t>
   </si>
   <si>
     <t>Ansprache bei der Verleihung des Dr. Leopold Lucas-Preises 2015 / von Jürgen Kampmann</t>
-  </si>
-  <si>
-    <t>501 $t</t>
-  </si>
-  <si>
-    <t>501 $t (mehrfach)</t>
   </si>
   <si>
     <t>Le vent paraclet
@@ -2911,32 +2837,7 @@
     <t>505 $t, $r</t>
   </si>
   <si>
-    <t>Der Roman des Freiherrn von Vieren / Adelbert von Chamisso, Friedrich de la Motte Fouqué, Karl Wilhelm Salice-Contessa</t>
-  </si>
-  <si>
     <t>505 $t, $r (mehrfach)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frontmatter -- ; Editorial -- ; Inhalt -- ; Einleitung |r Hill, Marc / Yıldız, Erol --
-*Wie die Syrer mit den Finnen schwitzten* / Kaminer, Wladimir --
-Die postmigrantische Perspektive: Aushandlungsprozesse in pluralen Gesellschaften / Foroutan, Naika --
-Wann war »die Post-Migration«? Denken über Zeiten und Grenzen / Rupnow, Dirk --
-Vom methodologischen Nationalismus zu postmigrantischen Visionen / Yıldız, Erol --
-Konvivialität – Momente von Post-Otherness / Römhild, Regina --
-Komplexität und Vielheit / Terkessidis, Mark --
-Urbanität ist Mobilität und Diversität / Bukow, Wolf-D. --
-Eine Vision von Vielfalt: Das Stadtleben aus postmigrantischer Perspektive / Hill, Marc --
-Endlich angekommen? / Berger, Karl C. / Hetfleisch, Gerhard --
-Generation Mix – der Versuch einer Annäherung / Schneider, Jens --
-Bewegte Biografien in der postmigrantischen Gesellschaft / Rotter, Anita / Schacht, Frauke --
-Jenseits und diesseits der Grenzen. Transdifferente Verschränkungen in den Kinofilmen »Auf der anderen Seite« und »Almanya – Willkommen in Deutschland« / Ege, Müzeyyen --
-Migration von Architektur. Eigenheime deutsch-türkischer Bauherren in der Türkei / Bürkle, Stefanie --
-Kulturelle Gleichzeitigkeit – Zeitgenössischer Tanz aus Postmigrantischer Perspektive / Chatterjee, Sandra --
-Antirassistische Interventionen als notwendige »Störung« im deutschen Theater |r Sharifi, Azadeh --
-Ain’tegration – Work in Progress. Perspektiven aus dem migrantenstadl / Önder, Tunay --
-Solo für Viele. Ein Hörerlebnis durch Innsbruck / Hill, Marc / Önder, Tunay --
-Autorinnnen und Autoren
-</t>
   </si>
   <si>
     <r>
@@ -3243,9 +3144,6 @@
     <t>249 $a, $b, $c</t>
   </si>
   <si>
-    <t xml:space="preserve">Anhang: Die Negersklaven : ein Lustspiel in einem Aufzuge / Franz Guolfinger von Steinsberg / mit einem Nachwort herausgegeben von André Georgi </t>
-  </si>
-  <si>
     <t>249 $a, $v, $c</t>
   </si>
   <si>
@@ -3253,9 +3151,6 @@
   </si>
   <si>
     <t>249 $a, $v, $a, $v, $a, $v, $c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mit einem unvollendeten Manuskript / von Pierre und Marie-Claire Bourdieu ; Opus infinitum / Christophe Charle ; Selbstporträt als freier Künstler / Pascale Casanova / herausgegeben von Pascale Casanova, Patrick Champagne, Christophe Charle, Franck Poupeau und Marie-Christine Rivière ; aus dem Französischen von Achim Russer und Bernd Schwibs  </t>
   </si>
   <si>
     <r>
@@ -3359,13 +3254,112 @@
     <t>Ėvelina i ee druzʹja ; Velikij muzykant : romany / Gajto Gazdanov</t>
   </si>
   <si>
-    <t>Die Stunde da wir nichts voneinander wußten : ein Schauspiel ; Zurüstungen für die Unsterblichkeit : ein Königsdrama ; Die Fahrt im Einbaum oder Das Stück zum Film vom Krieg ; Warum eine Küche? / Untertagblues : ein Stationendrama ; Spuren der Verirrten ; Bis daß der Tag euch scheidet oder Eine Frage des Lichts : ein Monolog / Immer noch Sturm ; Die schönen Tage von Aranjuez : ein Sommerdialog ; Die Unschuldigen, ich und die Unbekannte am Rand der Landstraße ; Anhang: Filmerzählungen / Peter Handke</t>
-  </si>
-  <si>
     <t>#374</t>
   </si>
   <si>
     <t>Statement of responsibility (R)</t>
+  </si>
+  <si>
+    <t>Die Stunde da wir nichts voneinander wußten : ein Schauspiel ; Zurüstungen für die Unsterblichkeit : ein Königsdrama ; Die Fahrt im Einbaum oder Das Stück zum Film vom Krieg ; Warum eine Küche? ; Untertagblues : ein Stationendrama ; Spuren der Verirrten ; Bis daß der Tag euch scheidet oder Eine Frage des Lichts : ein Monolog ; Immer noch Sturm ; Die schönen Tage von Aranjuez : ein Sommerdialog ; Die Unschuldigen, ich und die Unbekannte am Rand der Landstraße ; Anhang: Filmerzählungen / Peter Handke</t>
+  </si>
+  <si>
+    <t>Mit einem unvollendeten Manuskript / von Pierre und Marie-Claire Bourdieu ; Opus infinitum / Christophe Charle ; Selbstporträt als freier Künstler / Pascale Casanova / herausgegeben von Pascale Casanova, Patrick Champagne, Christophe Charle, Franck Poupeau und Marie-Christine Rivière ; aus dem Französischen von Achim Russer und Bernd Schwibs</t>
+  </si>
+  <si>
+    <t>Anhang: Die Negersklaven : ein Lustspiel in einem Aufzuge / Franz Guolfinger von Steinsberg / mit einem Nachwort herausgegeben von André Georgi</t>
+  </si>
+  <si>
+    <t>Dritte Gewalt im Wandel : veränderte Anforderungen an Legitimität und Effektivität? / Fabian Wittreck; Frauke Brosius-Gersdorf
+Gestaltung des demographischen Wandels als Verwaltungsaufgabe / Jan Ziekow; Stephan Rixen
+Sicherung grund- und menschenrechtlicher Standards gegenüber neuen Gefährdungen durch private und ausländische Akteure / Thilo Marauhn; Magdalena Pöschl</t>
+  </si>
+  <si>
+    <t>505 $t (mehrfach)</t>
+  </si>
+  <si>
+    <t>Kommentar zu Nietzsches "Idyllen aus Messina" / Sebastian Kaufmann</t>
+  </si>
+  <si>
+    <t>Abweichender Titel auf der Vorderseite des vorderen Banddeckels: Almanach für 1544 und 1545
+Abweichender Titel: Georg Seyfridt 1544 und 1545
+Abweichender Titel: Almanach für 1544 und 1545
+"Reprint der Schreibkalender "Almanach" für 1544 und 1545 von Georg Seyfridt" (Impressum)
+Die Vorlage enthält insgesamt 3 Werke.
+Vorlagen: Exemplare der Ratsschulbibliothek Zwickau (Sign.: 22.9.15.(33) und (35))</t>
+  </si>
+  <si>
+    <t>XV. Vorgeschichte der slavischen Sprachen und Sprachkontakt /Prehistory of the Slavic Languages and Language Contact; 82. Georg Holzer, Vorhistorische Periode / Prehistoric Period; 83. Jürgen Udolph, Ethnogenese und Urheimat der Slaven / Ethnogenesis and 'Urheimat' of the Slavs; 84. William R. Schmalstieg, Baltoslavic / Baltoslavisch
+85. Heinz Schuster-Šewc, Der Zerfall der slavischen Spracheinheit (des Urslavischen) und die genetische Gliederung der slavischen Sprachen / The Decay of the Slavic Language Unit (of Proto-Slavic) and the Genetic Structure of the Slavic languages Heinz Schuster-Šewc86. Jerzy Bartminski, Basic Assumptions of Slavic Ethnolinguistics / Grundannahmen der slavischen Ethnolinguistik; 87. Walter Breu, Substrate auf slavischem Sprachgebiet (Südslavisch) / Substrates in Slavic language area (South Slavonic)
+88. Harald Haarmann, Finnougrisch-slavische Sprachkontakte / Finno Ugric-Slavic Language Contacts89. Stanislaw Stachowski, Türkischer Einfluss auf den slavischen Wortschatz / Turkish Influence on the Slavic Vocabulary; XVI. Altkirchenslavisch und Kirchenslavisch Old Church Slavonic and Church Slavonic; 90 Helmut Keipert, Kirchenslavisch-Begriffe / Conceptions of Church Slavonic; 91. Heinz Miklas/Velizar Sadovski, Die Struktur des Altkirchenslavischen / The Structure of Old Church Slavonic; 92. Viktor M. Živov (†), Das Kirchenslavische bei den Ostslaven / Church Slavonic among the East Slavs
+93. Johannes Reinhart, Das Kroatisch-Kirchenslavische / Croatian Church Slavonic94. Giorgio Ziffer, Slavia orthodoxa und Slavia romana / Slavia Orthodoxa and Slavia Romana; 95. Nikolaos Trunte, Neukirchenslavisch / New Church Slavonic; 96. Roland Marti, Wirkungsgeschichte des Kirchenslavischen / The Impact of Church Slavonic and its History; 97. Ivan Bujukliev, Sprachbewusstsein bei den orthodoxen Slaven / Language Awareness among the Orthodox Slavs; XVII. Frühe volkssprachliche Überlieferungen Early Vernacular Development
+98. Vadim B. Krys'ko, Frühe volkssprachliche Entwicklung: Das Altostslavische / Early vernacular Development: Old East Slavic99. Juliane Besters-Dilger, Frühe volkssprachliche Entwicklung: Russische Kanzleisprache des 16. und 17. Jahrhunderts / Early vernacular development: Russian firm language of the 16th and 17th century
+100. Michael Moser, Frühe volkssprachliche Entwicklung auf dem Gebiet der heutigen Ukraine und Weißrusslands: Das Mittelukrainische und Mittelweißrussische / Early vernacular development in the area of today's Ukraine and Byelorussia: Middle Ukrainian and Middle White Russian
+100. Frühe volkssprachliche Entwicklung auf dem Gebiet der heutigen Ukraine und Weißrusslands: Das Mittelukrainische und Mittelweißrussische / Early vernacular development in the area of today’s Ukraine and Byelorussia: Middle Ukrainian and Middle White Russian / Moser, Michael
+122. Goals, Tasks, and Lessons of Historical Syntax / Ziele und Aufgaben der historischen Syntax / Timberlake, Alan
+101. Frühe volkssprachliche Entwicklung: Tschechisch / Early vernacular development: Czech / Šlosar, Dušan
+102. Frühe volkssprachliche Entwicklung: Kroatisch / Early vernacular development: Croatian / Wirtz, Gudrun
+103. Frühe volkssprachliche Entwicklung: Slovenisch / Early vernacular development: Slovenian / Seitz Shewmon, Elisabeth
+104. Polabian / Polabisch / Polański, Kazimierz
+105. Herausbildung der Standardsprachen: Ukrainisch und Weißrussisch / History of the Standard Language: Ukrainian and Belarusian / Bieder, Hermann
+106. History of Standard Languages: Slovak / Herausbildung der Standardsprache: Slovakisch / Žigo, Pavol
+107. Herausbildung der Standardsprache: Slovenisch / History of the Standard Language: Slovenian / Herrity, Peter
+108. Herausbildung der Standardsprache bei Serben und Kroaten / History of the Standard Language: Serbian and Croatian / Lehfeldt, Werner
+109. Formation of the Standard Language: Macedonian / Herausbildung der Standardsprache: Makedonisch / Hill, Peter M.
+110. Herausbildung der Standardsprache: Sorbisch / Formation of the Standard Language: Sorbian / Schuster-Šewc, Heinz
+111. Projekte einer gemeinslavischen Schriftsprache / Projects of planned Languages for the Slavs / Ivanova, Diana
+112. Historische Graphematik des Slavischen: Glagolitische und kyrillische Schrift / Historical Graphemics of the Slavic Languages: the Glagolitic and Cyrillic Writing Systems / Marti, Roland
+113. History and Development of the Latin Writing System in the Slavic Languages / Geschichte und Entwicklung der lateinischen Schrift in den slavischen Sprachen / Kučera, Karel
+114. Diachrone Phonologie / Diachronic Phonology / Stadnik-Holzer, Elena
+115. Introduction to Slavic Historical Morphology: Slavic Noun Classes / Die Entwicklung der Morphologie (Nominalklassen) im Slavischen / Janda, Laura A.
+116. Evolution of Verb Classes in Slavic / Die Entwicklung der Verbalklassen im Slavischen / Townsend, Charles E.
+117. Historical Development of Slavic Inflectional Accent / Die historische Entwicklung des slavischen Flexionsakzentes / Baerman, Matthew
+118. Entstehung der Kategorie der Belebtheit/Personalität / The Development of the Grammatical Category of Animacy / Krys’ko, Vadim B.
+119. Definiteness (Diachrony) / Bestimmtheit (Diachronie) / Topolińska, Zuzana
+120. Umbau des Tempussystems / The Reconstruction of the Temporal System / Klimonow, Wladimir D.
+121. Umbau des Partizipialsystems / The Reconstruction of the Participal System / Wiemer, Björn.
+123. The Simple Sentence / Der einfache Satz / Timberlake, Alan
+124. Erweiterung des einfachen Satzes / Extension of the Simple Sentence / Večerka, Radoslav
+125. Complex Sentence: Parataxis / Zusammengesetzter Satz: Parataxe / Klenin, Emily
+126. Complex Sentence: Hypotaxis / Zusammengesetzter Satz: Hypotaxe / Klenin, Emily
+127. Jüngere Lehnwortschatzschichten der slavischen Sprachen / Younger Loanword Strata in the Slavic Languages / Otten, Fred
+128. Westeuropäische Einflüsse in der Wortbildung / Western European Influences in Word Formation / Mengel, Swetlana
+129. Ausgewählte lexikalisch-semantische Gruppen / Selected lexical-semantic groups (Colour Terms, Kinship Terms) / Hill, Peter M.
+130. Phänomene der historischen Phraseologie der slavischen Sprachen / Phenomena of Historical Phraseology in the Slavic Languages / Bierich, Alexander
+131. Slavische Grammatikschreibung / Slavonic Grammaticography / Daiber, Thomas
+132. Grammatikschreibung bei den Tschechen und Slowaken bis zur Aufklärung / Czech and Slovak Grammaticography Before the Enlightenment / Čejka, Mirek
+133. Grammatikschreibung bei den Slowenen / Slovene Grammaticography / Hammel, Robert
+134. Grammatikschreibung bei den Bulgaren zwischen 1835 und 1944 / Grammaticography among the Bulgarians between 1835 and 1944 / Hammel, Robert
+135. Grammatikschreibung bei den Polen bis zur Aufklärung / Polish Grammaticography Before the Enlightenment / Bugajski, Marian
+136. Grammatikschreibung bei den Sorben (bis zum Ende d. 19. Jh.s) / Sorbian Grammaticography (Before the End of the 19th Century) / Wölke, Sonja
+137. Grammatiken der russischen Standardsprache / Grammars of the Russian Standard Language / Wingender, Monika
+138. Grammatiken der ukrainischen und der weißrussischen Standardsprache / Grammars of the Ukrainian and Belarusian Standard Languages / Bieder, Hermann
+139. Grammars of Polish From the 19th and 20th Century / Bugajski, Marian
+140. Dialektlexikographie / Dialect Lexicography / Neweklowsky, Gerhard
+141. Phraseographie / Phraseography / Worbs, Erika
+142. Typen slavischer Standardsprachen / Types of Slavic Standard Languages / Wingender, Monika
+143. Rechtlicher und faktischer Status slavischer Standardsprachen und Sprachenkonflikte / Legal and Factual Status of Slavic Standard Languages and Language Conflicts / Marti, Roland
+144. Sprach(en)politik in Ländern mit slavischer Mehrheitssprache / Language Politics in Countries with a Slavic Majority Language / Lubaś, Władysław.</t>
+  </si>
+  <si>
+    <t>Frontmatter -- ; Editorial -- ; Inhalt -- ; Einleitung / Hill, Marc / Yıldız, Erol --
+*Wie die Syrer mit den Finnen schwitzten* / Kaminer, Wladimir --
+Die postmigrantische Perspektive: Aushandlungsprozesse in pluralen Gesellschaften / Foroutan, Naika --
+Wann war »die Post-Migration«? Denken über Zeiten und Grenzen / Rupnow, Dirk --
+Vom methodologischen Nationalismus zu postmigrantischen Visionen / Yıldız, Erol --
+Konvivialität – Momente von Post-Otherness / Römhild, Regina --
+Komplexität und Vielheit / Terkessidis, Mark --
+Urbanität ist Mobilität und Diversität / Bukow, Wolf-D. --
+Eine Vision von Vielfalt: Das Stadtleben aus postmigrantischer Perspektive / Hill, Marc --
+Endlich angekommen? / Berger, Karl C. / Hetfleisch, Gerhard --
+Generation Mix – der Versuch einer Annäherung / Schneider, Jens --
+Bewegte Biografien in der postmigrantischen Gesellschaft / Rotter, Anita / Schacht, Frauke --
+Jenseits und diesseits der Grenzen. Transdifferente Verschränkungen in den Kinofilmen »Auf der anderen Seite« und »Almanya – Willkommen in Deutschland« / Ege, Müzeyyen --
+Migration von Architektur. Eigenheime deutsch-türkischer Bauherren in der Türkei / Bürkle, Stefanie --
+Kulturelle Gleichzeitigkeit – Zeitgenössischer Tanz aus Postmigrantischer Perspektive / Chatterjee, Sandra --
+Antirassistische Interventionen als notwendige »Störung« im deutschen Theater / Sharifi, Azadeh --
+Ain’tegration – Work in Progress. Perspektiven aus dem migrantenstadl / Önder, Tunay --
+Solo für Viele. Ein Hörerlebnis durch Innsbruck / Hill, Marc / Önder, Tunay --
+Autorinnnen und Autoren</t>
   </si>
 </sst>
 </file>
@@ -6005,7 +5999,7 @@
         <v>728470527</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -7651,7 +7645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -7665,7 +7659,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7678,7 +7672,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7686,7 +7680,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7694,7 +7688,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7702,7 +7696,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7715,7 +7709,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -7746,22 +7740,22 @@
     </row>
     <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -7771,10 +7765,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -7850,13 +7844,13 @@
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="B18" s="24">
         <v>874210879</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -7864,13 +7858,13 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="B19" s="24">
         <v>881598119</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -7878,13 +7872,13 @@
     </row>
     <row r="20" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="B20" s="24">
         <v>869013548</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -7892,13 +7886,13 @@
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="B21" s="24">
         <v>749845392</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -7906,13 +7900,13 @@
     </row>
     <row r="22" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="B22" s="24">
         <v>225488418</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -7920,13 +7914,13 @@
     </row>
     <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="B23" s="24">
         <v>1588137961</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -8104,7 +8098,7 @@
         <v>876614268</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -8335,7 +8329,7 @@
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -8365,8 +8359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="43.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8701,7 +8695,7 @@
         <v>888820720</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>496</v>
+        <v>578</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -8731,8 +8725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9268,7 +9262,7 @@
         <v>882661418</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21"/>
@@ -10713,7 +10707,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10726,7 +10720,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -10739,7 +10733,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10747,7 +10741,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10755,7 +10749,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10763,7 +10757,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -10776,7 +10770,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10807,22 +10801,22 @@
     </row>
     <row r="9" spans="1:7" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -10832,10 +10826,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -10845,10 +10839,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -10858,10 +10852,10 @@
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -10955,13 +10949,13 @@
     </row>
     <row r="22" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B22" s="24">
         <v>837414458</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -10969,13 +10963,13 @@
     </row>
     <row r="23" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="B23" s="24">
         <v>829179151</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -10983,13 +10977,13 @@
     </row>
     <row r="24" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -10997,13 +10991,13 @@
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="B25" s="24">
         <v>827757425</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -11011,13 +11005,13 @@
     </row>
     <row r="26" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="B26" s="24">
         <v>1666928607</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -11025,13 +11019,13 @@
     </row>
     <row r="27" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="B27" s="24">
         <v>1048425584</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -11039,13 +11033,13 @@
     </row>
     <row r="28" spans="1:8" ht="114" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="B28" s="24">
         <v>1032610050</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -11053,13 +11047,13 @@
     </row>
     <row r="29" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="B29" s="24">
         <v>825759323</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -11519,8 +11513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11533,7 +11527,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -11546,7 +11540,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -11554,7 +11548,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11562,7 +11556,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11570,7 +11564,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -11583,7 +11577,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -11620,16 +11614,16 @@
         <v>281</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>510</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>511</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -11639,10 +11633,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -11652,10 +11646,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -11738,7 +11732,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>280</v>
       </c>
@@ -11746,7 +11740,7 @@
         <v>788134256</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -11754,13 +11748,13 @@
     </row>
     <row r="21" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B21" s="24">
         <v>792994558</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>518</v>
+        <v>579</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -11768,27 +11762,27 @@
     </row>
     <row r="22" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B22" s="24">
         <v>818940786</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>517</v>
+        <v>575</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B23" s="24">
         <v>790280035</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>519</v>
+        <v>577</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -11796,41 +11790,41 @@
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B24" s="24">
         <v>880340185</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B25" s="24">
-        <v>875950426</v>
+        <v>859546233</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>524</v>
+        <v>576</v>
       </c>
       <c r="B26" s="24">
-        <v>859546233</v>
+        <v>875950426</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -11838,13 +11832,13 @@
     </row>
     <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="B27" s="24">
         <v>1042460965</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>527</v>
+        <v>580</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -12031,7 +12025,7 @@
         <v>873533267</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -12392,10 +12386,10 @@
         <v>860726789</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
@@ -12494,7 +12488,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>

</xml_diff>

<commit_message>
Changed title of work to include data from mrc field 700. Updated rda.xlsx. #refs 375
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="19" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="25" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -3296,10 +3296,6 @@
 700 $a, $t, $f</t>
   </si>
   <si>
-    <t>Aufgaben mit Lösungen zum Grundwissen Elektrotechnik, 2005
-Stiny, Leonard, Aufgaben mit Lösungen zur Elektrotechnik, 2008</t>
-  </si>
-  <si>
     <t>130 $a, $g</t>
   </si>
   <si>
@@ -3309,6 +3305,297 @@
   <si>
     <t>240 $a
 700 $t</t>
+  </si>
+  <si>
+    <t>Wirtschaftsrecht, Arbeitsrecht, Sozialrecht
+Grundmann, Wolfgang, Wirtschaft, Arbeit und Soziales</t>
+  </si>
+  <si>
+    <t>The language of life &lt;dt.&gt;
+Collins, Francis S., 1950-, The language of life &lt;dt.&gt;</t>
+  </si>
+  <si>
+    <t>Ticket #375</t>
+  </si>
+  <si>
+    <t>700 $a</t>
+  </si>
+  <si>
+    <t>700 $l</t>
+  </si>
+  <si>
+    <t>700 $t</t>
+  </si>
+  <si>
+    <t>700 $f</t>
+  </si>
+  <si>
+    <t>Personal name (NR)</t>
+  </si>
+  <si>
+    <t>Numeration (NR)</t>
+  </si>
+  <si>
+    <t>Titles and other words associated with a name (R)</t>
+  </si>
+  <si>
+    <t>Title of a work (NR)</t>
+  </si>
+  <si>
+    <t>Date of a work (NR)</t>
+  </si>
+  <si>
+    <t>Language of a work (NR)</t>
+  </si>
+  <si>
+    <t>Schlagworte</t>
+  </si>
+  <si>
+    <t>Abbildung von Schlagwörter und Schlagwortketten</t>
+  </si>
+  <si>
+    <t>Subject Access Fields</t>
+  </si>
+  <si>
+    <t>Subjects</t>
+  </si>
+  <si>
+    <t>Ticket #376</t>
+  </si>
+  <si>
+    <t>Social Web &gt; E-Business &gt; Kartellrecht &gt; Datenschutz &gt; EU-Kartellrecht &gt; Deutschland
+Deutschland &gt; Kartellrecht &gt; Online-Community &gt; Marktbeherrschung
+Deutschland &gt; Online-Community &gt; Kartellrecht &gt; Datenschutz</t>
+  </si>
+  <si>
+    <t>1043586679</t>
+  </si>
+  <si>
+    <t>Gesetzliche Rentenversicherung &gt; Erwerbsverlauf &gt; Lebensverlauf &gt; Deutschland &gt; Anwartschaften
+Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Alterversorgung
+Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Alterversorgung</t>
+  </si>
+  <si>
+    <t>Europäische Union &gt; Auswertige Gewalt</t>
+  </si>
+  <si>
+    <t>Business ethics
+Applied psychology
+Economics—Psychological aspects
+Consulting, Supervision and Coaching</t>
+  </si>
+  <si>
+    <t>650 $a mehrfach keine Kette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">689 $a </t>
+  </si>
+  <si>
+    <t>650 $a 
+689 $a  (mehrfach)</t>
+  </si>
+  <si>
+    <t>650 $a 
+689 $a (mehrfach)</t>
+  </si>
+  <si>
+    <t>Westbalkan &gt; Außenpolitik
+Kosovo
+Montenegro
+Serbien</t>
+  </si>
+  <si>
+    <t>650 Second Indicator</t>
+  </si>
+  <si>
+    <t>Thesaurus</t>
+  </si>
+  <si>
+    <t>Field link and sequence number</t>
+  </si>
+  <si>
+    <t>650 $8</t>
+  </si>
+  <si>
+    <t>689 Second Indicator</t>
+  </si>
+  <si>
+    <t>650 $a</t>
+  </si>
+  <si>
+    <t>Topical term or geographic name entry element</t>
+  </si>
+  <si>
+    <t>Entspreicht der Occurence in Pica-Felds</t>
+  </si>
+  <si>
+    <t>689 First Indicator</t>
+  </si>
+  <si>
+    <t>Entspricht der Reihenfolge in der Schlagwortkette</t>
+  </si>
+  <si>
+    <t>Deskriptor</t>
+  </si>
+  <si>
+    <t>689 $a mehrfach auch ohne Kette</t>
+  </si>
+  <si>
+    <t>Art des Inhalts</t>
+  </si>
+  <si>
+    <t>Anzeige der Publikationsform nach RDA</t>
+  </si>
+  <si>
+    <t>Index Term-Genre/Form</t>
+  </si>
+  <si>
+    <t>Ticket #377</t>
+  </si>
+  <si>
+    <t>655 $a</t>
+  </si>
+  <si>
+    <t>Genre/form data or focus term</t>
+  </si>
+  <si>
+    <t>Quelle</t>
+  </si>
+  <si>
+    <t>Hochschulschrift</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Type of content</t>
+  </si>
+  <si>
+    <t>655 $a, $x, $y, $z</t>
+  </si>
+  <si>
+    <t>Aufsatzsammlung; Konferenzschrift</t>
+  </si>
+  <si>
+    <t>655 $a mehrfach</t>
+  </si>
+  <si>
+    <t>Konferenzschrift (Evangelische Akademie Loccum, 06.12.2017-07.12.2017, Rehburg-Loccum); Konferenzschrift (Studienzentrum der EKD für Genderfragen, 06.12.2017-07.12.2017, Rehburg-Loccum)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Anmerkung: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">655 ist wiederholbar.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Separatoren: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Runde Klammer "()", Komma ", " und Semikolon ";"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Darstellungsregel:
+Art des Inhalts: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>655 $a ($x, $y, $z); 655 $a ($x, $y, $z)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Daten für die Abbildung von Schlagworte in Marc 650 und 689.
+Alle Kategorien sind wiederholbar
+Es werden Schlagworketten anhand von Indikatoren abgebildet.
+Es werden nur Einträge dargestellt, bei denen der zweite Indikator belegt ist.
+Alle Angaben in $a sind verlinkt und lösen eine Suche à http://sucheneu.thulb.uni-jena.de/Search/Results?lookfor=.......&amp;type=Subject aus.
+Jeder Eintrag ist in einer neuen Zeile dargestellt.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Separatoren:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Eckige Klammer zu "&gt; "
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Darstellungsregel:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+650 [$8 1.1\x] $a &gt; [$8 1.2\x] $a &gt; [$8 1.3\x] $a &gt; usw.
+689 [1. Ind. = 0] [2. Ind. = 0] $a &gt; [1. Ind. = 0] [2. Ind. = 1] $a &gt; [1. Ind. = 0] [2. Ind. = 2] $a &gt; usw.
+689 [1. Ind. = 1] [2. Ind. = 0] $a &gt; [1. Ind. = 1] [2. Ind. = 1] $a &gt; [1. Ind. = 1] [2. Ind. = 2] $a &gt; usw
+689 usw.</t>
+    </r>
+  </si>
+  <si>
+    <t>Aufgaben mit Lösungen zum Grundwissen Elektrotechnik, 2005
+Stiny, Leonhard, Aufgaben mit Lösungen zur Elektrotechnik, 2008</t>
   </si>
   <si>
     <r>
@@ -3394,7 +3681,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>nur wo $t belegt ist auch 700 darstellen</t>
+      <t>nur wo $t belegt ist, auch 700 darstellen</t>
     </r>
     <r>
       <rPr>
@@ -3405,294 +3692,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
-700 $a(, $b)(, $c)(, $l)(, $t)(, $f)</t>
-    </r>
-  </si>
-  <si>
-    <t>Wirtschaftsrecht, Arbeitsrecht, Sozialrecht
-Grundmann, Wolfgang, Wirtschaft, Arbeit und Soziales</t>
-  </si>
-  <si>
-    <t>The language of life &lt;dt.&gt;
-Collins, Francis S., 1950-, The language of life &lt;dt.&gt;</t>
-  </si>
-  <si>
-    <t>Ticket #375</t>
-  </si>
-  <si>
-    <t>700 $a</t>
-  </si>
-  <si>
-    <t>700 $l</t>
-  </si>
-  <si>
-    <t>700 $t</t>
-  </si>
-  <si>
-    <t>700 $f</t>
-  </si>
-  <si>
-    <t>Personal name (NR)</t>
-  </si>
-  <si>
-    <t>Numeration (NR)</t>
-  </si>
-  <si>
-    <t>Titles and other words associated with a name (R)</t>
-  </si>
-  <si>
-    <t>Title of a work (NR)</t>
-  </si>
-  <si>
-    <t>Date of a work (NR)</t>
-  </si>
-  <si>
-    <t>Language of a work (NR)</t>
-  </si>
-  <si>
-    <t>Schlagworte</t>
-  </si>
-  <si>
-    <t>Abbildung von Schlagwörter und Schlagwortketten</t>
-  </si>
-  <si>
-    <t>Subject Access Fields</t>
-  </si>
-  <si>
-    <t>Subjects</t>
-  </si>
-  <si>
-    <t>Ticket #376</t>
-  </si>
-  <si>
-    <t>Social Web &gt; E-Business &gt; Kartellrecht &gt; Datenschutz &gt; EU-Kartellrecht &gt; Deutschland
-Deutschland &gt; Kartellrecht &gt; Online-Community &gt; Marktbeherrschung
-Deutschland &gt; Online-Community &gt; Kartellrecht &gt; Datenschutz</t>
-  </si>
-  <si>
-    <t>1043586679</t>
-  </si>
-  <si>
-    <t>Gesetzliche Rentenversicherung &gt; Erwerbsverlauf &gt; Lebensverlauf &gt; Deutschland &gt; Anwartschaften
-Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Alterversorgung
-Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Alterversorgung</t>
-  </si>
-  <si>
-    <t>Europäische Union &gt; Auswertige Gewalt</t>
-  </si>
-  <si>
-    <t>Business ethics
-Applied psychology
-Economics—Psychological aspects
-Consulting, Supervision and Coaching</t>
-  </si>
-  <si>
-    <t>650 $a mehrfach keine Kette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">689 $a </t>
-  </si>
-  <si>
-    <t>650 $a 
-689 $a  (mehrfach)</t>
-  </si>
-  <si>
-    <t>650 $a 
-689 $a (mehrfach)</t>
-  </si>
-  <si>
-    <t>Westbalkan &gt; Außenpolitik
-Kosovo
-Montenegro
-Serbien</t>
-  </si>
-  <si>
-    <t>650 Second Indicator</t>
-  </si>
-  <si>
-    <t>Thesaurus</t>
-  </si>
-  <si>
-    <t>Field link and sequence number</t>
-  </si>
-  <si>
-    <t>650 $8</t>
-  </si>
-  <si>
-    <t>689 Second Indicator</t>
-  </si>
-  <si>
-    <t>650 $a</t>
-  </si>
-  <si>
-    <t>Topical term or geographic name entry element</t>
-  </si>
-  <si>
-    <t>Entspreicht der Occurence in Pica-Felds</t>
-  </si>
-  <si>
-    <t>689 First Indicator</t>
-  </si>
-  <si>
-    <t>Entspricht der Reihenfolge in der Schlagwortkette</t>
-  </si>
-  <si>
-    <t>Deskriptor</t>
-  </si>
-  <si>
-    <t>689 $a mehrfach auch ohne Kette</t>
-  </si>
-  <si>
-    <t>Art des Inhalts</t>
-  </si>
-  <si>
-    <t>Anzeige der Publikationsform nach RDA</t>
-  </si>
-  <si>
-    <t>Index Term-Genre/Form</t>
-  </si>
-  <si>
-    <t>Ticket #377</t>
-  </si>
-  <si>
-    <t>655 $a</t>
-  </si>
-  <si>
-    <t>Genre/form data or focus term</t>
-  </si>
-  <si>
-    <t>Quelle</t>
-  </si>
-  <si>
-    <t>Hochschulschrift</t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Type of content</t>
-  </si>
-  <si>
-    <t>655 $a, $x, $y, $z</t>
-  </si>
-  <si>
-    <t>Aufsatzsammlung; Konferenzschrift</t>
-  </si>
-  <si>
-    <t>655 $a mehrfach</t>
-  </si>
-  <si>
-    <t>Konferenzschrift (Evangelische Akademie Loccum, 06.12.2017-07.12.2017, Rehburg-Loccum); Konferenzschrift (Studienzentrum der EKD für Genderfragen, 06.12.2017-07.12.2017, Rehburg-Loccum)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Anmerkung: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">655 ist wiederholbar.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Separatoren: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Runde Klammer "()", Komma ", " und Semikolon ";"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Darstellungsregel:
-Art des Inhalts: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>655 $a ($x, $y, $z); 655 $a ($x, $y, $z)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Daten für die Abbildung von Schlagworte in Marc 650 und 689.
-Alle Kategorien sind wiederholbar
-Es werden Schlagworketten anhand von Indikatoren abgebildet.
-Es werden nur Einträge dargestellt, bei denen der zweite Indikator belegt ist.
-Alle Angaben in $a sind verlinkt und lösen eine Suche à http://sucheneu.thulb.uni-jena.de/Search/Results?lookfor=.......&amp;type=Subject aus.
-Jeder Eintrag ist in einer neuen Zeile dargestellt.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Separatoren:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Eckige Klammer zu "&gt; "
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Darstellungsregel:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 
-650 [$8 1.1\x] $a &gt; [$8 1.2\x] $a &gt; [$8 1.3\x] $a &gt; usw.
-689 [1. Ind. = 0] [2. Ind. = 0] $a &gt; [1. Ind. = 0] [2. Ind. = 1] $a &gt; [1. Ind. = 0] [2. Ind. = 2] $a &gt; usw.
-689 [1. Ind. = 1] [2. Ind. = 0] $a &gt; [1. Ind. = 1] [2. Ind. = 1] $a &gt; [1. Ind. = 1] [2. Ind. = 2] $a &gt; usw
-689 usw.</t>
+700 $a(, $b)(, $c)(, $d)(, $l)(, $t)(, $f)</t>
     </r>
   </si>
 </sst>
@@ -6421,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6433,7 +6433,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6441,7 +6441,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6449,7 +6449,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6457,7 +6457,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6469,7 +6469,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -6495,30 +6495,30 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C10" s="68"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C11" s="68"/>
     </row>
@@ -6529,28 +6529,28 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C13" s="68"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C14" s="68"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C15" s="68"/>
     </row>
@@ -6713,13 +6713,13 @@
     </row>
     <row r="42" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B42" s="24">
         <v>1039228518</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
@@ -6727,13 +6727,13 @@
     </row>
     <row r="43" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -6741,13 +6741,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B44" s="24">
         <v>1040185495</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -6755,13 +6755,13 @@
     </row>
     <row r="45" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B45" s="24">
         <v>1067367012</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -6769,13 +6769,13 @@
     </row>
     <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B46" s="24">
         <v>1046980084</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -6811,7 +6811,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -6825,7 +6825,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -6839,7 +6839,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6853,7 +6853,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -6867,7 +6867,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -6881,7 +6881,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6917,13 +6917,13 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -6972,13 +6972,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B13" s="24">
         <v>1042191735</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -6986,13 +6986,13 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B14" s="24">
         <v>1067568034</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -7000,13 +7000,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B15" s="24">
         <v>1644814935</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -7014,13 +7014,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B16" s="24">
         <v>839431554</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -7028,13 +7028,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B17" s="24">
         <v>1047237415</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
@@ -9727,8 +9727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9792,7 +9792,7 @@
         <v>289</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -9823,7 +9823,7 @@
         <v>291</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>579</v>
+        <v>635</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -10083,10 +10083,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C39" s="63"/>
       <c r="F39" s="26"/>
@@ -10096,7 +10096,7 @@
         <v>95</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C40" s="63"/>
       <c r="F40" s="26"/>
@@ -10106,37 +10106,37 @@
         <v>96</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C41" s="63"/>
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C42" s="63"/>
       <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C43" s="63"/>
       <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C44" s="63"/>
       <c r="F44" s="26"/>
@@ -10231,7 +10231,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B52" s="24">
         <v>147213592</v>
@@ -10273,13 +10273,13 @@
     </row>
     <row r="55" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B55" s="24">
         <v>871478110</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21"/>
@@ -10287,13 +10287,13 @@
     </row>
     <row r="56" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B56" s="62" t="s">
         <v>334</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21"/>
@@ -10307,7 +10307,7 @@
         <v>881131350</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>575</v>
+        <v>634</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21"/>

</xml_diff>

<commit_message>
Changed hierarchy of subjects in detail view. Added unit test for subjects. Updated rda.xlsx. #refs 376
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="25" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -3371,14 +3371,6 @@
     <t>1043586679</t>
   </si>
   <si>
-    <t>Gesetzliche Rentenversicherung &gt; Erwerbsverlauf &gt; Lebensverlauf &gt; Deutschland &gt; Anwartschaften
-Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Alterversorgung
-Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Alterversorgung</t>
-  </si>
-  <si>
-    <t>Europäische Union &gt; Auswertige Gewalt</t>
-  </si>
-  <si>
     <t>Business ethics
 Applied psychology
 Economics—Psychological aspects
@@ -3694,6 +3686,14 @@
       <t xml:space="preserve">
 700 $a(, $b)(, $c)(, $d)(, $l)(, $t)(, $f)</t>
     </r>
+  </si>
+  <si>
+    <t>Gesetzliche Rentenversicherung &gt; Erwerbsverlauf &gt; Lebensverlauf &gt; Deutschland &gt; Anwartschaften
+Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Altersversorgung
+Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Altersversorgung</t>
+  </si>
+  <si>
+    <t>Europäische Union &gt; Auswärtige Gewalt</t>
   </si>
 </sst>
 </file>
@@ -6407,8 +6407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6495,30 +6495,30 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C10" s="68"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C11" s="68"/>
     </row>
@@ -6529,28 +6529,28 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C13" s="68"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C14" s="68"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C15" s="68"/>
     </row>
@@ -6713,7 +6713,7 @@
     </row>
     <row r="42" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B42" s="24">
         <v>1039228518</v>
@@ -6727,13 +6727,13 @@
     </row>
     <row r="43" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>597</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>598</v>
+        <v>634</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -6741,13 +6741,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B44" s="24">
         <v>1040185495</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>599</v>
+        <v>635</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -6755,13 +6755,13 @@
     </row>
     <row r="45" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B45" s="24">
         <v>1067367012</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -6769,13 +6769,13 @@
     </row>
     <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B46" s="24">
         <v>1046980084</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -6811,7 +6811,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -6825,7 +6825,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -6839,7 +6839,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6853,7 +6853,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -6867,7 +6867,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -6881,7 +6881,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6917,13 +6917,13 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -6972,13 +6972,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B13" s="24">
         <v>1042191735</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -6986,13 +6986,13 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B14" s="24">
         <v>1067568034</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -7000,13 +7000,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B15" s="24">
         <v>1644814935</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -7014,13 +7014,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B16" s="24">
         <v>839431554</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -7028,13 +7028,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B17" s="24">
         <v>1047237415</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
@@ -9727,8 +9727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C37"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9823,7 +9823,7 @@
         <v>291</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -10307,7 +10307,7 @@
         <v>881131350</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21"/>

</xml_diff>

<commit_message>
Fixed removal of escaped parentheses in SolrVZGRecord::getFormattedMarcData. Added new version of rda.xlsx
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="641">
   <si>
     <t>Titel</t>
   </si>
@@ -3694,6 +3694,21 @@
   </si>
   <si>
     <t>Europäische Union &gt; Auswärtige Gewalt</t>
+  </si>
+  <si>
+    <t>655 $a, $y, $z</t>
+  </si>
+  <si>
+    <t>Konferenzschrift (1997, Köln)</t>
+  </si>
+  <si>
+    <t>24416178X</t>
+  </si>
+  <si>
+    <t>655 $a, $z</t>
+  </si>
+  <si>
+    <t>Konferenzschrift (Menaggio); Konferenzschrift</t>
   </si>
 </sst>
 </file>
@@ -6407,7 +6422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -6795,10 +6810,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7039,6 +7054,34 @@
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
       <c r="F17" s="43"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
+        <v>636</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>638</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>637</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="40" t="s">
+        <v>639</v>
+      </c>
+      <c r="B19" s="24">
+        <v>516531425</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>640</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="43"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Removed field 773 from related items. Changed getSeries to include field 773. Added new version of rda.xlsx. refs #379
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -23,29 +23,30 @@
     <sheet name="Sprachangaben" sheetId="7" r:id="rId9"/>
     <sheet name="Angaben über Sprache und Schrif" sheetId="8" r:id="rId10"/>
     <sheet name="Publikationsangaben" sheetId="9" r:id="rId11"/>
-    <sheet name="Schlagworte" sheetId="33" r:id="rId12"/>
-    <sheet name="Art des Inhalts" sheetId="34" r:id="rId13"/>
-    <sheet name="Druckort" sheetId="10" r:id="rId14"/>
-    <sheet name="Hochschulschriftenvermerk" sheetId="11" r:id="rId15"/>
-    <sheet name="Maßstab bei Karten" sheetId="12" r:id="rId16"/>
-    <sheet name="Projektion bei Karten" sheetId="13" r:id="rId17"/>
-    <sheet name="Koordinaten bei Karten" sheetId="14" r:id="rId18"/>
-    <sheet name="Erscheinungsverlauf" sheetId="15" r:id="rId19"/>
-    <sheet name="Anmerkungen zum Erscheinungsver" sheetId="16" r:id="rId20"/>
-    <sheet name="Mehr zum Titel" sheetId="17" r:id="rId21"/>
-    <sheet name="Verwandte Ressourcen" sheetId="18" r:id="rId22"/>
-    <sheet name="Vorheriger Späterer Titel" sheetId="19" r:id="rId23"/>
-    <sheet name="Anmerkungen" sheetId="20" r:id="rId24"/>
-    <sheet name="Werktitel" sheetId="21" r:id="rId25"/>
-    <sheet name="Umfang" sheetId="22" r:id="rId26"/>
-    <sheet name="Sekundäre Ausgabe" sheetId="29" r:id="rId27"/>
-    <sheet name="Fingerprint" sheetId="23" r:id="rId28"/>
-    <sheet name="Bibliographische Zitate" sheetId="24" r:id="rId29"/>
-    <sheet name="ISBN" sheetId="25" r:id="rId30"/>
-    <sheet name="Falsche ISBN" sheetId="26" r:id="rId31"/>
-    <sheet name="ZDB-Nummer" sheetId="27" r:id="rId32"/>
-    <sheet name="Basisklassifikation" sheetId="28" r:id="rId33"/>
-    <sheet name="Inhaltsangaben" sheetId="30" r:id="rId34"/>
+    <sheet name="Teil von" sheetId="35" r:id="rId12"/>
+    <sheet name="Schlagworte" sheetId="33" r:id="rId13"/>
+    <sheet name="Art des Inhalts" sheetId="34" r:id="rId14"/>
+    <sheet name="Druckort" sheetId="10" r:id="rId15"/>
+    <sheet name="Hochschulschriftenvermerk" sheetId="11" r:id="rId16"/>
+    <sheet name="Maßstab bei Karten" sheetId="12" r:id="rId17"/>
+    <sheet name="Projektion bei Karten" sheetId="13" r:id="rId18"/>
+    <sheet name="Koordinaten bei Karten" sheetId="14" r:id="rId19"/>
+    <sheet name="Erscheinungsverlauf" sheetId="15" r:id="rId20"/>
+    <sheet name="Anmerkungen zum Erscheinungsver" sheetId="16" r:id="rId21"/>
+    <sheet name="Mehr zum Titel" sheetId="17" r:id="rId22"/>
+    <sheet name="Verwandte Ressourcen" sheetId="18" r:id="rId23"/>
+    <sheet name="Vorheriger Späterer Titel" sheetId="19" r:id="rId24"/>
+    <sheet name="Anmerkungen" sheetId="20" r:id="rId25"/>
+    <sheet name="Werktitel" sheetId="21" r:id="rId26"/>
+    <sheet name="Umfang" sheetId="22" r:id="rId27"/>
+    <sheet name="Sekundäre Ausgabe" sheetId="29" r:id="rId28"/>
+    <sheet name="Fingerprint" sheetId="23" r:id="rId29"/>
+    <sheet name="Bibliographische Zitate" sheetId="24" r:id="rId30"/>
+    <sheet name="ISBN" sheetId="25" r:id="rId31"/>
+    <sheet name="Falsche ISBN" sheetId="26" r:id="rId32"/>
+    <sheet name="ZDB-Nummer" sheetId="27" r:id="rId33"/>
+    <sheet name="Basisklassifikation" sheetId="28" r:id="rId34"/>
+    <sheet name="Inhaltsangaben" sheetId="30" r:id="rId35"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -359,6 +360,31 @@
 </comments>
 </file>
 
+<file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -535,7 +561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="684">
   <si>
     <t>Titel</t>
   </si>
@@ -3710,12 +3736,240 @@
   <si>
     <t>Konferenzschrift (Menaggio); Konferenzschrift</t>
   </si>
+  <si>
+    <t>Teil von</t>
+  </si>
+  <si>
+    <t>Abbildung von Verknüpfungen zu hierarchischübergeordneten Aufnahmen</t>
+  </si>
+  <si>
+    <t>Host Item Entries / Series Added Entries</t>
+  </si>
+  <si>
+    <t>Part of</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Überordnung in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bücher &amp; mehr</t>
+    </r>
+  </si>
+  <si>
+    <t>490 $a</t>
+  </si>
+  <si>
+    <t>Series statement</t>
+  </si>
+  <si>
+    <t>490 $v</t>
+  </si>
+  <si>
+    <t>Volume/sequential designation</t>
+  </si>
+  <si>
+    <t>800 $w</t>
+  </si>
+  <si>
+    <t>Bibliographic record control number</t>
+  </si>
+  <si>
+    <t>800 $v</t>
+  </si>
+  <si>
+    <t>810 $v</t>
+  </si>
+  <si>
+    <t>810 $w</t>
+  </si>
+  <si>
+    <t>830 $v</t>
+  </si>
+  <si>
+    <t>830 $w</t>
+  </si>
+  <si>
+    <t>773 $t</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Einleitende Texte werden ignoriert.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Separatoren:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Keine
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Darstellungsregel:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+490a (mit PPN-Verlinkung aus 8X0 $w (DE-627) basierend auf $v Abgleich) $v 
+773 $t (mit PPN-Verlinkung basierend auf 773 $w (DE-627)) $q
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ausnahme:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Ist 773 $t nicht belegt, wird 245 $a verwendet.</t>
+    </r>
+  </si>
+  <si>
+    <t>104347336X</t>
+  </si>
+  <si>
+    <t>Related parts</t>
+  </si>
+  <si>
+    <t>Jahrbuch für Kommunikationsgeschichte 20.2018</t>
+  </si>
+  <si>
+    <t>773 $g 
+245 $a</t>
+  </si>
+  <si>
+    <t>773 $t $g mehrfach</t>
+  </si>
+  <si>
+    <t>504196316</t>
+  </si>
+  <si>
+    <t>The American economic review 95(2005), 2, Seite 189-193
+Journal of the ASEAN Federation of Endocrine Societies 95(2005), 2, Seite 189-193</t>
+  </si>
+  <si>
+    <t>2016 IEEE/ACIS 14th International Conference on Software Engineering Research, Management and Applications (SERA) (2016), Seite 209-215</t>
+  </si>
+  <si>
+    <t>773 $t $g</t>
+  </si>
+  <si>
+    <t>Germanistik
+Mittelhochdeutsches Wörterbuch Band 1-</t>
+  </si>
+  <si>
+    <t>102911417X</t>
+  </si>
+  <si>
+    <t>490 $a
+245 $a, 773 $g</t>
+  </si>
+  <si>
+    <t>490 $a, $v
+830 $w (DE-627)</t>
+  </si>
+  <si>
+    <t>490 $a mehrfach</t>
+  </si>
+  <si>
+    <t>Lehr- und Handbuch
+Jura auf den [Punkt] gebracht</t>
+  </si>
+  <si>
+    <t>490 $a
+810 $w
+830 $w</t>
+  </si>
+  <si>
+    <t>490 $a
+830 $w
+245 $a, 773 $g</t>
+  </si>
+  <si>
+    <t>Weimarer Studien zu Kulturpolitik und Kulturökonomie 9
+Kulturbranding 4</t>
+  </si>
+  <si>
+    <t>490 $a
+800 $w
+830 $w</t>
+  </si>
+  <si>
+    <t>Topographische Karte : [Bundesrepublik Deutschland] / hrsg. vom Landesamt für Vermessung und Geoinformation L 5140</t>
+  </si>
+  <si>
+    <t>Transport and environment reporting mechanism (TERM) report 2017
+EEA report No 22/2017</t>
+  </si>
+  <si>
+    <t>Madrigali : opera completa = Complete madrigals / Claudio Monteverdi. Ed. by Michelangelo Gabbrielli  Vol. 9
+Odhecaton  31A</t>
+  </si>
+  <si>
+    <t>Weitere Titel</t>
+  </si>
+  <si>
+    <t>Other titles</t>
+  </si>
+  <si>
+    <t>Concerti
+XII concerti a cinque con violini, violetta, violoncello e basso continue, opera decima (1736) [1]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3832,6 +4086,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -6420,10 +6681,491 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="C10" s="68"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="68"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="C12" s="68"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>650</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="C13" s="68"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="68"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="C15" s="68"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>654</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="C16" s="68"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="68"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="C18" s="68"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="C19" s="68"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="68"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C21" s="68"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="C22" s="68"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="68"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" s="68"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="68"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="68"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="68"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="68"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="68"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="68"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="68"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="68"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="68"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="68"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="68"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="68"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="68"/>
+      <c r="F37" s="26"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>659</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>661</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>664</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>665</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="40" t="s">
+        <v>667</v>
+      </c>
+      <c r="B44" s="24">
+        <v>865263426</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>666</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>670</v>
+      </c>
+      <c r="B45" s="24">
+        <v>527913065</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>670</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>669</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>683</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>671</v>
+      </c>
+      <c r="B47" s="24">
+        <v>671795848</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>678</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="B48" s="24">
+        <v>668495618</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>673</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
+        <v>674</v>
+      </c>
+      <c r="B49" s="24">
+        <v>1018584919</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>679</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
+        <v>675</v>
+      </c>
+      <c r="B50" s="24">
+        <v>813438144</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>676</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
+        <v>677</v>
+      </c>
+      <c r="B51" s="24">
+        <v>664783767</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6808,12 +7550,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7092,7 +7834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -7298,7 +8040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -7502,7 +8244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -7681,204 +8423,6 @@
       </c>
       <c r="C13" s="41" t="s">
         <v>202</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>208</v>
-      </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" s="24">
-        <v>470336242</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>209</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -7902,18 +8446,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -7922,12 +8466,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -7936,12 +8480,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -7950,12 +8494,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7964,12 +8508,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -7978,7 +8522,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -8002,7 +8546,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -8017,9 +8561,9 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -8038,7 +8582,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -8058,7 +8602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -8070,13 +8614,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B13" s="24">
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>476</v>
+        <v>209</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8100,18 +8644,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8120,12 +8664,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8134,12 +8678,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -8148,12 +8692,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -8162,12 +8706,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8176,12 +8720,12 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8200,7 +8744,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -8215,13 +8759,11 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>222</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="B9" s="37"/>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -8238,7 +8780,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -8258,7 +8800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -8268,15 +8810,15 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B13" s="24">
-        <v>233814418</v>
+        <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>223</v>
+        <v>476</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8594,20 +9136,20 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8616,12 +9158,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="114" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8630,12 +9172,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -8649,7 +9191,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -8663,7 +9205,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8677,7 +9219,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -8711,12 +9253,12 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="185.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
@@ -8764,33 +9306,19 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>231</v>
+      <c r="C13" s="41" t="s">
+        <v>223</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
       <c r="F13" s="43"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="B14" s="24">
-        <v>502081112</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>232</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8807,6 +9335,220 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="114" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="185.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="B13" s="24">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="24">
+        <v>502081112</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -8982,7 +9724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -9176,7 +9918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -9379,372 +10121,6 @@
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="63.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>267</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="301.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>270</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>271</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>272</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="F11" s="50"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
-        <v>475</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="B25" s="24">
-        <v>129993549</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>486</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>482</v>
-      </c>
-      <c r="B26" s="24">
-        <v>129494860</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>487</v>
-      </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" ht="114" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="B27" s="24">
-        <v>129292834</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>488</v>
-      </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>484</v>
-      </c>
-      <c r="B28" s="24">
-        <v>329875515</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>483</v>
-      </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="B29" s="24">
-        <v>888820720</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>571</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9767,6 +10143,372 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="43.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="63.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="301.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C13" s="49"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>475</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="C16" s="49"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="49"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="52"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B25" s="24">
+        <v>129993549</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>482</v>
+      </c>
+      <c r="B26" s="24">
+        <v>129494860</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" ht="114" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" s="24">
+        <v>129292834</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>484</v>
+      </c>
+      <c r="B28" s="24">
+        <v>329875515</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B29" s="24">
+        <v>888820720</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
@@ -10394,7 +11136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -10709,7 +11451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -10913,7 +11655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -11122,234 +11864,6 @@
       </c>
       <c r="C15" s="41" t="s">
         <v>372</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="37" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>379</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>380</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
-        <v>379</v>
-      </c>
-      <c r="B13" s="24">
-        <v>151797196</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>381</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
-        <v>379</v>
-      </c>
-      <c r="B14" s="24">
-        <v>193804867</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>382</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-    </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
-        <v>383</v>
-      </c>
-      <c r="B15" s="24">
-        <v>409606901</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>384</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -11373,8 +11887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11416,7 +11930,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>545</v>
+        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11424,7 +11938,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>516</v>
+        <v>682</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -11746,6 +12260,234 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="37" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="B13" s="24">
+        <v>151797196</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>381</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="B14" s="24">
+        <v>193804867</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>382</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" s="24">
+        <v>409606901</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>384</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -11954,212 +12696,6 @@
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>401</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="C15" s="53" t="s">
-        <v>404</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="B16" s="24">
-        <v>885659430</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>405</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12182,6 +12718,212 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="B16" s="24">
+        <v>885659430</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>405</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -12379,7 +13121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -12612,7 +13354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
@@ -13540,7 +14282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed invalid ISBNs from ISBN in detail view. Updated rda.xslx refs# 170
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11445" tabRatio="992" firstSheet="24" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="684">
   <si>
     <t>Titel</t>
   </si>
@@ -2005,43 +2005,6 @@
     <t>020 $9</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Verwende $9 statt $a für die Anzeige, weil es die vorlagetreue Schreibweise (mit den Bindestrichen) enthält.
-Anzeige:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ISBN:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> $9 : $c
-           $9 : $c
-020 ist wiederholbar. Wenn mehrfach belegt, ISBN untereinander anzeigen</t>
-    </r>
-  </si>
-  <si>
     <t>020 $c</t>
   </si>
   <si>
@@ -2057,20 +2020,9 @@
     <t>$9 und $c</t>
   </si>
   <si>
-    <t>978-92-897-1568-3
-978-92-2-130471-5 : ILO
-978-92-897-1569-0 : web
-978-92-2-130472-2 : PDF</t>
-  </si>
-  <si>
     <t>52680498X</t>
   </si>
   <si>
-    <t>3-540-69713-6 : EUR 29.95, sfr 46.00
-978-3-540-69713-8 : EUR 29.95, sfr 46.00
-978-3-540-69739-8</t>
-  </si>
-  <si>
     <t>Falsche ISBN</t>
   </si>
   <si>
@@ -2081,72 +2033,6 @@
   </si>
   <si>
     <t>Canceled/invalid ISBN</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">In Solr-Marc ist die falsche ISBN leider nur ohne "-" vorhanden.
-Anzeige:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Falsche</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ISBN:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> $z
-</t>
-    </r>
-  </si>
-  <si>
-    <t>$z</t>
-  </si>
-  <si>
-    <t>9784540697138</t>
-  </si>
-  <si>
-    <t>9783643137173</t>
   </si>
   <si>
     <t>ZDB-Nummer</t>
@@ -3714,11 +3600,6 @@
     </r>
   </si>
   <si>
-    <t>Gesetzliche Rentenversicherung &gt; Erwerbsverlauf &gt; Lebensverlauf &gt; Deutschland &gt; Anwartschaften
-Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Altersversorgung
-Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Altersversorgung</t>
-  </si>
-  <si>
     <t>Europäische Union &gt; Auswärtige Gewalt</t>
   </si>
   <si>
@@ -3963,6 +3844,107 @@
   <si>
     <t>Concerti
 XII concerti a cinque con violini, violetta, violoncello e basso continue, opera decima (1736) [1]</t>
+  </si>
+  <si>
+    <t>Gesetzliche Rentenversicherung &gt; Erwerbsverlauf &gt; Lebensverlauf &gt; Deutschland &gt; Anwartschaften
+Deutschland &gt; Mittleres Lebensalter &gt; Lebenslauf &gt; Altersversorgung</t>
+  </si>
+  <si>
+    <t>978-3-643-13717-3</t>
+  </si>
+  <si>
+    <t>978-4-540-69713-8</t>
+  </si>
+  <si>
+    <t>978-92-897-1568-3
+978-92-2-130471-5 : ILO</t>
+  </si>
+  <si>
+    <t>$z, $9</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verwende $9 statt $a für die Anzeige, weil es die vorlagetreue Schreibweise (mit den Bindestrichen) enthält.
+Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ISBN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $9 : $c
+           $9 : $c
+020 ist wiederholbar. Wenn mehrfach belegt, ISBN untereinander anzeigen. $9 aus 020-Einträge, wo $z belegt ist, sollen nur in der Zeile "Falsche ISBN" abgebildet werden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In Solr-Marc ist die falsche ISBN leider nur ohne "-" vorhanden.
+Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Falsche</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ISBN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $9 aus 020-Einträgen mit belegtem $z
+</t>
+    </r>
+  </si>
+  <si>
+    <t>3-540-69713-6 : Pb. : EUR 29.95, sfr 46.00
+978-3-540-69713-8 : Pb. : EUR 29.95, sfr 46.00</t>
   </si>
 </sst>
 </file>
@@ -5074,7 +5056,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6631,7 +6613,7 @@
         <v>728470527</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -6683,7 +6665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -6697,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6709,7 +6691,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6717,7 +6699,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6725,7 +6707,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6733,7 +6715,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6745,7 +6727,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -6771,21 +6753,21 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C10" s="68"/>
     </row>
@@ -6796,19 +6778,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C12" s="68"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="C13" s="68"/>
     </row>
@@ -6819,19 +6801,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C15" s="68"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="C16" s="68"/>
     </row>
@@ -6842,19 +6824,19 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C18" s="68"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="C19" s="68"/>
     </row>
@@ -6865,7 +6847,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>257</v>
@@ -6877,7 +6859,7 @@
         <v>245</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="C22" s="68"/>
     </row>
@@ -6888,7 +6870,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>257</v>
@@ -7009,13 +6991,13 @@
     </row>
     <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
@@ -7023,13 +7005,13 @@
     </row>
     <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -7037,13 +7019,13 @@
     </row>
     <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="B44" s="24">
         <v>865263426</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -7051,13 +7033,13 @@
     </row>
     <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B45" s="24">
         <v>527913065</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -7065,13 +7047,13 @@
     </row>
     <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -7079,13 +7061,13 @@
     </row>
     <row r="47" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="B47" s="24">
         <v>671795848</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="21"/>
@@ -7093,13 +7075,13 @@
     </row>
     <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="B48" s="24">
         <v>668495618</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="21"/>
@@ -7107,13 +7089,13 @@
     </row>
     <row r="49" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="B49" s="24">
         <v>1018584919</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="21"/>
@@ -7121,13 +7103,13 @@
     </row>
     <row r="50" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="B50" s="24">
         <v>813438144</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="21"/>
@@ -7135,13 +7117,13 @@
     </row>
     <row r="51" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="B51" s="24">
         <v>664783767</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="21"/>
@@ -7164,8 +7146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7178,7 +7160,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7190,7 +7172,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7198,7 +7180,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7206,7 +7188,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7214,7 +7196,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7226,7 +7208,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -7252,30 +7234,30 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C10" s="68"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="C11" s="68"/>
     </row>
@@ -7286,28 +7268,28 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="C13" s="68"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="C14" s="68"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="C15" s="68"/>
     </row>
@@ -7470,27 +7452,27 @@
     </row>
     <row r="42" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="B42" s="24">
         <v>1039228518</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>634</v>
+        <v>676</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -7498,13 +7480,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="B44" s="24">
         <v>1040185495</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -7512,13 +7494,13 @@
     </row>
     <row r="45" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="B45" s="24">
         <v>1067367012</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -7526,13 +7508,13 @@
     </row>
     <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="B46" s="24">
         <v>1046980084</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -7568,7 +7550,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -7582,7 +7564,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -7596,7 +7578,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -7610,7 +7592,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7624,7 +7606,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -7638,7 +7620,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -7674,13 +7656,13 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -7729,13 +7711,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B13" s="24">
         <v>1042191735</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -7743,13 +7725,13 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="B14" s="24">
         <v>1067568034</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -7757,13 +7739,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B15" s="24">
         <v>1644814935</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -7771,13 +7753,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B16" s="24">
         <v>839431554</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -7785,13 +7767,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="B17" s="24">
         <v>1047237415</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
@@ -7799,13 +7781,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="42"/>
@@ -7813,13 +7795,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="40" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="B19" s="24">
         <v>516531425</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="42"/>
@@ -8818,7 +8800,7 @@
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8856,7 +8838,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8869,7 +8851,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8877,7 +8859,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8885,7 +8867,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8893,7 +8875,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -8906,7 +8888,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -8937,22 +8919,22 @@
     </row>
     <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -8962,10 +8944,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -9041,13 +9023,13 @@
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B18" s="24">
         <v>874210879</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -9055,13 +9037,13 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="B19" s="24">
         <v>881598119</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -9069,13 +9051,13 @@
     </row>
     <row r="20" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="B20" s="24">
         <v>869013548</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -9083,13 +9065,13 @@
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="B21" s="24">
         <v>749845392</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -9097,13 +9079,13 @@
     </row>
     <row r="22" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="B22" s="24">
         <v>225488418</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -9111,13 +9093,13 @@
     </row>
     <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="B23" s="24">
         <v>1588137961</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -9871,7 +9853,7 @@
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -9885,7 +9867,7 @@
         <v>876614268</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -10116,7 +10098,7 @@
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -10208,7 +10190,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10252,7 +10234,7 @@
         <v>271</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -10290,7 +10272,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>268</v>
@@ -10302,7 +10284,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>257</v>
@@ -10314,10 +10296,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="51"/>
@@ -10326,7 +10308,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>275</v>
@@ -10338,7 +10320,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>277</v>
@@ -10420,13 +10402,13 @@
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="B25" s="24">
         <v>129993549</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -10434,13 +10416,13 @@
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="B26" s="24">
         <v>129494860</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -10454,7 +10436,7 @@
         <v>129292834</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -10462,13 +10444,13 @@
     </row>
     <row r="28" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B28" s="24">
         <v>329875515</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -10482,7 +10464,7 @@
         <v>888820720</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -10577,7 +10559,7 @@
         <v>289</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -10608,7 +10590,7 @@
         <v>291</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -10868,10 +10850,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="C39" s="63"/>
       <c r="F39" s="26"/>
@@ -10881,7 +10863,7 @@
         <v>95</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="C40" s="63"/>
       <c r="F40" s="26"/>
@@ -10891,37 +10873,37 @@
         <v>96</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="C41" s="63"/>
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="C42" s="63"/>
       <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="C43" s="63"/>
       <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="C44" s="63"/>
       <c r="F44" s="26"/>
@@ -11016,13 +10998,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="B52" s="24">
         <v>147213592</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21"/>
@@ -11036,7 +11018,7 @@
         <v>339</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="21"/>
@@ -11058,13 +11040,13 @@
     </row>
     <row r="55" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="B55" s="24">
         <v>871478110</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21"/>
@@ -11072,13 +11054,13 @@
     </row>
     <row r="56" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="B56" s="62" t="s">
         <v>334</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21"/>
@@ -11086,13 +11068,13 @@
     </row>
     <row r="57" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="B57" s="24">
         <v>881131350</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21"/>
@@ -11106,7 +11088,7 @@
         <v>882661418</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="21"/>
@@ -11333,7 +11315,7 @@
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -11470,7 +11452,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -11478,7 +11460,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -11486,7 +11468,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -11494,7 +11476,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -11502,7 +11484,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -11510,7 +11492,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -11540,13 +11522,13 @@
     </row>
     <row r="9" spans="1:9" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="D9" s="59"/>
       <c r="F9" s="3"/>
@@ -11595,13 +11577,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -11609,13 +11591,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B14" s="24">
         <v>1019909943</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -11623,13 +11605,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B15" s="24">
         <v>576971693</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -11637,13 +11619,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B16" s="24">
         <v>585243190</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -11901,7 +11883,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -11914,7 +11896,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -11922,7 +11904,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11930,7 +11912,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11938,7 +11920,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -11951,7 +11933,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -11982,22 +11964,22 @@
     </row>
     <row r="9" spans="1:7" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -12007,10 +11989,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -12020,10 +12002,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -12033,10 +12015,10 @@
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -12130,13 +12112,13 @@
     </row>
     <row r="22" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="B22" s="24">
         <v>837414458</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -12144,13 +12126,13 @@
     </row>
     <row r="23" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="B23" s="24">
         <v>829179151</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -12158,13 +12140,13 @@
     </row>
     <row r="24" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -12172,13 +12154,13 @@
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="B25" s="24">
         <v>827757425</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -12186,13 +12168,13 @@
     </row>
     <row r="26" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="B26" s="24">
         <v>1666928607</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -12200,13 +12182,13 @@
     </row>
     <row r="27" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="B27" s="24">
         <v>1048425584</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -12214,13 +12196,13 @@
     </row>
     <row r="28" spans="1:8" ht="114" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="B28" s="24">
         <v>1032610050</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -12228,13 +12210,13 @@
     </row>
     <row r="29" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="B29" s="24">
         <v>825759323</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -12491,11 +12473,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="46.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -12509,7 +12494,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -12517,7 +12502,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -12525,7 +12510,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -12533,7 +12518,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -12545,7 +12530,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -12565,7 +12550,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -12577,22 +12562,22 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="186" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>388</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>390</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>391</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="3"/>
@@ -12615,7 +12600,7 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -12635,7 +12620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
@@ -12645,7 +12630,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -12655,43 +12640,43 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B16" s="24">
         <v>187029679</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="171" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B17" s="24">
         <v>884572641</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>395</v>
+        <v>679</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="199.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>394</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>396</v>
-      </c>
       <c r="C18" s="19" t="s">
-        <v>397</v>
+        <v>683</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -12719,27 +12704,27 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -12747,7 +12732,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -12755,27 +12740,27 @@
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -12795,7 +12780,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -12807,25 +12792,25 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="216" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>402</v>
+        <v>682</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
@@ -12835,73 +12820,81 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="C15" s="53" t="s">
-        <v>404</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="B16" s="24">
-        <v>885659430</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>405</v>
+        <v>680</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>678</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
       <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>680</v>
+      </c>
+      <c r="B17" s="24">
+        <v>885659430</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>677</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12938,7 +12931,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -12952,7 +12945,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -12966,7 +12959,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -12980,7 +12973,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -12994,7 +12987,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -13008,7 +13001,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -13044,7 +13037,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -13095,13 +13088,13 @@
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -13136,7 +13129,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -13150,7 +13143,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -13164,7 +13157,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -13178,7 +13171,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -13192,7 +13185,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -13206,7 +13199,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -13242,13 +13235,13 @@
     </row>
     <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="D9" s="38"/>
       <c r="F9" s="3"/>
@@ -13257,10 +13250,10 @@
     </row>
     <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" s="38"/>
@@ -13270,10 +13263,10 @@
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="38"/>
@@ -13323,18 +13316,18 @@
     </row>
     <row r="15" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="B15" s="24">
         <v>868759473</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
       <c r="F15" s="43" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -13372,7 +13365,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -13385,7 +13378,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -13393,7 +13386,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13401,7 +13394,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13409,7 +13402,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -13422,7 +13415,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -13459,16 +13452,16 @@
         <v>281</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -13478,10 +13471,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -13491,10 +13484,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -13585,7 +13578,7 @@
         <v>788134256</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -13593,13 +13586,13 @@
     </row>
     <row r="21" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B21" s="24">
         <v>792994558</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -13607,13 +13600,13 @@
     </row>
     <row r="22" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B22" s="24">
         <v>818940786</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -13621,13 +13614,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="B23" s="24">
         <v>790280035</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -13635,13 +13628,13 @@
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="B24" s="24">
         <v>880340185</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -13649,13 +13642,13 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="B25" s="24">
         <v>859546233</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -13663,13 +13656,13 @@
     </row>
     <row r="26" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="B26" s="24">
         <v>875950426</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -13677,13 +13670,13 @@
     </row>
     <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="B27" s="24">
         <v>1042460965</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -13842,7 +13835,7 @@
         <v>877327637</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -13870,7 +13863,7 @@
         <v>873533267</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -14010,7 +14003,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -14067,17 +14060,17 @@
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C16" s="66"/>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>277</v>
@@ -14087,7 +14080,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>76</v>
@@ -14097,7 +14090,7 @@
     </row>
     <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>78</v>
@@ -14107,7 +14100,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>80</v>
@@ -14183,10 +14176,10 @@
         <v>521722950</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
@@ -14199,10 +14192,10 @@
         <v>63</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
@@ -14215,10 +14208,10 @@
         <v>725223227</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
@@ -14231,10 +14224,10 @@
         <v>860726789</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
@@ -14325,7 +14318,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -14333,7 +14326,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -14348,7 +14341,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -14381,7 +14374,7 @@
         <v>72</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -14448,16 +14441,16 @@
     </row>
     <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C17" s="68"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>277</v>
@@ -14466,7 +14459,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>76</v>
@@ -14475,7 +14468,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>78</v>
@@ -14484,7 +14477,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>80</v>
@@ -14563,45 +14556,45 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="B31" s="24">
         <v>520959078</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B32" s="24">
         <v>1005410313</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B33" s="24">
         <v>657009032</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="21"/>
@@ -14609,39 +14602,39 @@
     </row>
     <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B35" s="24">
         <v>875683843</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="B36" s="24">
         <v>867529938</v>

</xml_diff>

<commit_message>
Fixed display of basic classifications when bklname is not available. Updated rda.xslx refs #402
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="992" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="992" firstSheet="21" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="701">
   <si>
     <t>Titel</t>
   </si>
@@ -2024,94 +2024,17 @@
     <t>Basisklassifikation</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Detailanzeige</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:
-Wenn 084 $2 rvk:
-084 $a
-Trennzeichen bei Wiederholungen von 084 mit $2 = rvk: _;_ (in Worten: Blank Semikolon Blank)
-Auf jede Notation einen </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Suchlink </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">legen: Indexsuche mit Inhalt von 084 $a in rvk_full
-</t>
-    </r>
-  </si>
-  <si>
     <t>Other Classification Number</t>
   </si>
   <si>
-    <t>Sachgebiete</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Ticket #97</t>
-  </si>
-  <si>
-    <t>084 $a</t>
-  </si>
-  <si>
     <t>Klassifikationsnummer</t>
   </si>
   <si>
-    <t>084 ist wiederholbar und darin ist wiederum Subfeld |9 wiederholbar</t>
-  </si>
-  <si>
-    <t>084 $2</t>
-  </si>
-  <si>
-    <t>Klassifikation, hier: bcl</t>
-  </si>
-  <si>
-    <t>084 $9</t>
-  </si>
-  <si>
     <t>Titel der Klassifikation</t>
-  </si>
-  <si>
-    <t>3x 084 $2 = rvk</t>
   </si>
   <si>
     <t>79.65 Lebenslanges Lernen
 81.92 Berufliche Weiterbildung</t>
-  </si>
-  <si>
-    <t>/vufind/Search/Results?lookfor=“Lebenslanges+Lernen“&amp;type=bklname</t>
   </si>
   <si>
     <t>Sprache für die Arbeitswelt, 2017</t>
@@ -4094,6 +4017,55 @@
   </si>
   <si>
     <t>Klemens XI. (Papst, 1649-1721)</t>
+  </si>
+  <si>
+    <t>Basic Classification</t>
+  </si>
+  <si>
+    <t>Ticket #97, Ticket #402</t>
+  </si>
+  <si>
+    <t>Wenn in 936 Ind. 1 = b und Ind. 2 = k
+936 $a $j
+$j ist wiederholbar &gt; Darstellung nacheineinander, Trennung durch &gt;
+mehrere 936 werden untereinander abgebildet
+Auf jede Notation einen Suchlink legen: Indexsuche mit Inhalt von 936 $a</t>
+  </si>
+  <si>
+    <t>936 $a</t>
+  </si>
+  <si>
+    <t>936 $j</t>
+  </si>
+  <si>
+    <t>2x 936 Ind.1=b Ind. 2=k $a $j</t>
+  </si>
+  <si>
+    <t>/Search/Results?lookfor=%2279.65%22&amp;type=bklnumber
+/Search/Results?lookfor=%2281.92%22&amp;type=bklnumber</t>
+  </si>
+  <si>
+    <t>1x 936 Ind.1=b Ind. 2=k $a $j $j</t>
+  </si>
+  <si>
+    <t>21.80 Kunsthandwerk &gt; Kunstgewerbe: Allgemeines</t>
+  </si>
+  <si>
+    <t>/Search/Results?lookfor=%2221.80%22&amp;type=bklnumber</t>
+  </si>
+  <si>
+    <t>2x 936 Ind.1=b Ind. 2=k $a</t>
+  </si>
+  <si>
+    <t>15.51
+15.31</t>
+  </si>
+  <si>
+    <t>/Search/Results?lookfor=%2215.51%22&amp;type=bklnumber
+/Search/Results?lookfor=%2215.31%22&amp;type=bklnumber</t>
+  </si>
+  <si>
+    <t>021499845</t>
   </si>
 </sst>
 </file>
@@ -4423,7 +4395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4564,9 +4536,6 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4621,6 +4590,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -6783,7 +6754,7 @@
         <v>728470527</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>680</v>
+        <v>669</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -6811,7 +6782,7 @@
         <v>537824324</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>695</v>
+        <v>684</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -6849,7 +6820,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6861,7 +6832,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6869,7 +6840,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6877,7 +6848,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -6885,7 +6856,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6897,7 +6868,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -6923,194 +6894,194 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="C9" s="69" t="s">
         <v>619</v>
-      </c>
-      <c r="C9" s="70" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="C10" s="70"/>
+        <v>610</v>
+      </c>
+      <c r="C10" s="69"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="70"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="C12" s="70"/>
+        <v>610</v>
+      </c>
+      <c r="C12" s="69"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="C13" s="70"/>
+        <v>612</v>
+      </c>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="70"/>
+      <c r="C14" s="69"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="C15" s="70"/>
+        <v>610</v>
+      </c>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>626</v>
+        <v>615</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="C16" s="70"/>
+        <v>612</v>
+      </c>
+      <c r="C16" s="69"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="70"/>
+      <c r="C17" s="69"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="C18" s="70"/>
+        <v>610</v>
+      </c>
+      <c r="C18" s="69"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="C19" s="70"/>
+        <v>612</v>
+      </c>
+      <c r="C19" s="69"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="70"/>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="70"/>
+      <c r="C21" s="69"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>237</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>632</v>
-      </c>
-      <c r="C22" s="70"/>
+        <v>621</v>
+      </c>
+      <c r="C22" s="69"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="70"/>
+      <c r="C23" s="69"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="70"/>
+      <c r="C24" s="69"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="70"/>
+      <c r="C25" s="69"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="70"/>
+      <c r="C26" s="69"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="70"/>
+      <c r="C27" s="69"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="70"/>
+      <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="70"/>
+      <c r="C29" s="69"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="70"/>
+      <c r="C30" s="69"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="70"/>
+      <c r="C31" s="69"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="70"/>
+      <c r="C32" s="69"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="70"/>
+      <c r="C33" s="69"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="70"/>
+      <c r="C34" s="69"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="70"/>
+      <c r="C35" s="69"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="70"/>
+      <c r="C36" s="69"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="70"/>
+      <c r="C37" s="69"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -7161,13 +7132,13 @@
     </row>
     <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>633</v>
+        <v>622</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
@@ -7175,13 +7146,13 @@
     </row>
     <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>635</v>
+        <v>624</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>636</v>
+        <v>625</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>637</v>
+        <v>626</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -7189,13 +7160,13 @@
     </row>
     <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>639</v>
+        <v>628</v>
       </c>
       <c r="B44" s="24">
         <v>865263426</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -7203,13 +7174,13 @@
     </row>
     <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="B45" s="24">
         <v>527913065</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>640</v>
+        <v>629</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -7217,13 +7188,13 @@
     </row>
     <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -7231,13 +7202,13 @@
     </row>
     <row r="47" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B47" s="24">
         <v>671795848</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="21"/>
@@ -7245,13 +7216,13 @@
     </row>
     <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="B48" s="24">
         <v>668495618</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="21"/>
@@ -7259,13 +7230,13 @@
     </row>
     <row r="49" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="B49" s="24">
         <v>1018584919</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="21"/>
@@ -7273,13 +7244,13 @@
     </row>
     <row r="50" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="B50" s="24">
         <v>813438144</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="21"/>
@@ -7287,13 +7258,13 @@
     </row>
     <row r="51" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="B51" s="24">
         <v>664783767</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="21"/>
@@ -7316,8 +7287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7330,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7342,7 +7313,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7350,7 +7321,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7358,7 +7329,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -7366,7 +7337,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7378,7 +7349,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="3"/>
@@ -7404,174 +7375,174 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>579</v>
-      </c>
-      <c r="C9" s="70" t="s">
-        <v>604</v>
+        <v>568</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>580</v>
-      </c>
-      <c r="C10" s="70"/>
+        <v>569</v>
+      </c>
+      <c r="C10" s="69"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>584</v>
-      </c>
-      <c r="C11" s="70"/>
+        <v>573</v>
+      </c>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="70"/>
+      <c r="C12" s="69"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="C13" s="70"/>
+        <v>574</v>
+      </c>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>587</v>
-      </c>
-      <c r="C14" s="70"/>
+        <v>576</v>
+      </c>
+      <c r="C14" s="69"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>588</v>
-      </c>
-      <c r="C15" s="70"/>
+        <v>577</v>
+      </c>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="70"/>
+      <c r="C16" s="69"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="70"/>
+      <c r="C17" s="69"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="70"/>
+      <c r="C18" s="69"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="70"/>
+      <c r="C19" s="69"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="70"/>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="70"/>
+      <c r="C21" s="69"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="70"/>
+      <c r="C22" s="69"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="70"/>
+      <c r="C23" s="69"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="70"/>
+      <c r="C24" s="69"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="70"/>
+      <c r="C25" s="69"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="70"/>
+      <c r="C26" s="69"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="70"/>
+      <c r="C27" s="69"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="70"/>
+      <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="70"/>
+      <c r="C29" s="69"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="70"/>
+      <c r="C30" s="69"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="70"/>
+      <c r="C31" s="69"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="70"/>
+      <c r="C32" s="69"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="70"/>
+      <c r="C33" s="69"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="70"/>
+      <c r="C34" s="69"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="70"/>
+      <c r="C35" s="69"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="70"/>
+      <c r="C36" s="69"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="70"/>
+      <c r="C37" s="69"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -7622,13 +7593,13 @@
     </row>
     <row r="42" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="B42" s="24">
         <v>1039228518</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="21"/>
@@ -7636,13 +7607,13 @@
     </row>
     <row r="43" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="21"/>
@@ -7650,13 +7621,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="40" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="B44" s="24">
         <v>1040185495</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
@@ -7664,13 +7635,13 @@
     </row>
     <row r="45" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="B45" s="24">
         <v>1067367012</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
@@ -7678,13 +7649,13 @@
     </row>
     <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="B46" s="24">
         <v>1046980084</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -7720,7 +7691,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -7734,7 +7705,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -7748,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -7762,7 +7733,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7776,7 +7747,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -7790,7 +7761,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -7826,13 +7797,13 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>595</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>603</v>
+        <v>584</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>592</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -7881,13 +7852,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="B13" s="24">
         <v>1042191735</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -7895,13 +7866,13 @@
     </row>
     <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B14" s="24">
         <v>1067568034</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>696</v>
+        <v>685</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -7909,13 +7880,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="B15" s="24">
         <v>1644814935</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -7923,13 +7894,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="B16" s="24">
         <v>839431554</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -7937,13 +7908,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="B17" s="24">
         <v>1047237415</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="42"/>
@@ -7951,13 +7922,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="40" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="42"/>
@@ -7965,13 +7936,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="40" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="B19" s="24">
         <v>516531425</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="42"/>
@@ -8970,7 +8941,7 @@
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -9008,7 +8979,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -9021,7 +8992,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9029,7 +9000,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9037,7 +9008,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9045,7 +9016,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -9058,7 +9029,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -9089,22 +9060,22 @@
     </row>
     <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -9114,10 +9085,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -9166,9 +9137,9 @@
         <v>19</v>
       </c>
       <c r="B15" s="14"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.2">
@@ -9193,13 +9164,13 @@
     </row>
     <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="B18" s="24">
         <v>874210879</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -9207,13 +9178,13 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="B19" s="24">
         <v>881598119</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -9221,13 +9192,13 @@
     </row>
     <row r="20" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="B20" s="24">
         <v>869013548</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -9235,13 +9206,13 @@
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="B21" s="24">
         <v>749845392</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -9249,13 +9220,13 @@
     </row>
     <row r="22" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="B22" s="24">
         <v>225488418</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -9263,13 +9234,13 @@
     </row>
     <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
       <c r="B23" s="24">
         <v>1588137961</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -9666,7 +9637,7 @@
         <v>233814418</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -9952,10 +9923,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>674</v>
+        <v>664</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>663</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -9984,64 +9955,64 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C9" s="71" t="s">
-        <v>676</v>
+      <c r="C9" s="70" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>664</v>
-      </c>
-      <c r="C10" s="68"/>
+        <v>653</v>
+      </c>
+      <c r="C10" s="67"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="67"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>665</v>
-      </c>
-      <c r="C12" s="68"/>
+        <v>654</v>
+      </c>
+      <c r="C12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>671</v>
+        <v>660</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="C13" s="68"/>
+        <v>655</v>
+      </c>
+      <c r="C13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>671</v>
+        <v>660</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="C14" s="68"/>
+      <c r="C14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="69"/>
+      <c r="C15" s="68"/>
     </row>
     <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
@@ -10077,13 +10048,13 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
       <c r="B19" s="24">
         <v>876614268</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>677</v>
+        <v>666</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -10091,7 +10062,7 @@
     </row>
     <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
       <c r="B20" s="24">
         <v>894531530</v>
@@ -10105,13 +10076,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>673</v>
+        <v>662</v>
       </c>
       <c r="B21" s="24">
         <v>1671011902</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -10201,7 +10172,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10223,7 +10194,7 @@
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="64" t="s">
         <v>8</v>
       </c>
     </row>
@@ -10234,8 +10205,8 @@
       <c r="B9" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C9" s="72" t="s">
-        <v>686</v>
+      <c r="C9" s="71" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -10245,7 +10216,7 @@
       <c r="B10" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="73"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -10257,7 +10228,7 @@
       <c r="B11" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C11" s="73"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -10269,7 +10240,7 @@
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -10340,7 +10311,7 @@
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -10348,13 +10319,13 @@
     </row>
     <row r="19" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>684</v>
+        <v>673</v>
       </c>
       <c r="B19" s="24">
         <v>1066523630</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>685</v>
+        <v>674</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
@@ -10384,7 +10355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -10446,7 +10417,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10490,7 +10461,7 @@
         <v>260</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -10528,7 +10499,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>257</v>
@@ -10540,7 +10511,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>246</v>
@@ -10552,10 +10523,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="C16" s="48"/>
       <c r="D16" s="50"/>
@@ -10564,7 +10535,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>264</v>
@@ -10576,7 +10547,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>266</v>
@@ -10658,13 +10629,13 @@
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="B25" s="24">
         <v>129993549</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>681</v>
+        <v>670</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -10672,13 +10643,13 @@
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="B26" s="24">
         <v>129494860</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -10692,7 +10663,7 @@
         <v>129292834</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -10700,13 +10671,13 @@
     </row>
     <row r="28" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="B28" s="24">
         <v>329875515</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -10720,7 +10691,7 @@
         <v>888820720</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>693</v>
+        <v>682</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -10750,7 +10721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -10815,7 +10786,7 @@
         <v>278</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -10845,8 +10816,8 @@
       <c r="B9" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C9" s="70" t="s">
-        <v>606</v>
+      <c r="C9" s="69" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -10856,7 +10827,7 @@
       <c r="B10" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C10" s="70"/>
+      <c r="C10" s="69"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -10865,7 +10836,7 @@
       <c r="B11" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -10874,7 +10845,7 @@
       <c r="B12" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="69"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -10883,7 +10854,7 @@
       <c r="B13" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="70"/>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -10892,7 +10863,7 @@
       <c r="B14" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="69"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -10901,7 +10872,7 @@
       <c r="B15" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C15" s="70"/>
+      <c r="C15" s="69"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -10910,7 +10881,7 @@
       <c r="B16" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C16" s="70"/>
+      <c r="C16" s="69"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -10919,7 +10890,7 @@
       <c r="B17" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C17" s="70"/>
+      <c r="C17" s="69"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -10928,7 +10899,7 @@
       <c r="B18" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="C18" s="70"/>
+      <c r="C18" s="69"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -10937,7 +10908,7 @@
       <c r="B19" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="70"/>
+      <c r="C19" s="69"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -10946,7 +10917,7 @@
       <c r="B20" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="C20" s="70"/>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -10955,7 +10926,7 @@
       <c r="B21" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C21" s="70"/>
+      <c r="C21" s="69"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
@@ -10964,12 +10935,12 @@
       <c r="B22" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C22" s="70"/>
+      <c r="C22" s="69"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="70"/>
+      <c r="C23" s="69"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
@@ -10978,7 +10949,7 @@
       <c r="B24" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="70"/>
+      <c r="C24" s="69"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
@@ -10987,7 +10958,7 @@
       <c r="B25" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C25" s="70"/>
+      <c r="C25" s="69"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
@@ -10996,7 +10967,7 @@
       <c r="B26" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C26" s="70"/>
+      <c r="C26" s="69"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
@@ -11005,7 +10976,7 @@
       <c r="B27" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C27" s="70"/>
+      <c r="C27" s="69"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
@@ -11014,7 +10985,7 @@
       <c r="B28" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C28" s="70"/>
+      <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
@@ -11023,7 +10994,7 @@
       <c r="B29" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="C29" s="70"/>
+      <c r="C29" s="69"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
@@ -11032,7 +11003,7 @@
       <c r="B30" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C30" s="70"/>
+      <c r="C30" s="69"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
@@ -11041,7 +11012,7 @@
       <c r="B31" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C31" s="70"/>
+      <c r="C31" s="69"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
@@ -11050,7 +11021,7 @@
       <c r="B32" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C32" s="70"/>
+      <c r="C32" s="69"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
@@ -11059,7 +11030,7 @@
       <c r="B33" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="C33" s="70"/>
+      <c r="C33" s="69"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
@@ -11068,7 +11039,7 @@
       <c r="B34" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="C34" s="70"/>
+      <c r="C34" s="69"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
@@ -11077,7 +11048,7 @@
       <c r="B35" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="C35" s="70"/>
+      <c r="C35" s="69"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
@@ -11086,7 +11057,7 @@
       <c r="B36" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C36" s="70"/>
+      <c r="C36" s="69"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
@@ -11095,23 +11066,23 @@
       <c r="B37" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C37" s="70"/>
+      <c r="C37" s="69"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="62"/>
+      <c r="C38" s="61"/>
       <c r="F38" s="26"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>559</v>
-      </c>
-      <c r="C39" s="62"/>
+        <v>548</v>
+      </c>
+      <c r="C39" s="61"/>
       <c r="F39" s="26"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -11119,9 +11090,9 @@
         <v>95</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="C40" s="62"/>
+        <v>549</v>
+      </c>
+      <c r="C40" s="61"/>
       <c r="F40" s="26"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -11129,39 +11100,39 @@
         <v>96</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="C41" s="62"/>
+        <v>550</v>
+      </c>
+      <c r="C41" s="61"/>
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="C42" s="62"/>
+        <v>553</v>
+      </c>
+      <c r="C42" s="61"/>
       <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="C43" s="62"/>
+        <v>551</v>
+      </c>
+      <c r="C43" s="61"/>
       <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>563</v>
-      </c>
-      <c r="C44" s="62"/>
+        <v>552</v>
+      </c>
+      <c r="C44" s="61"/>
       <c r="F44" s="26"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -11254,13 +11225,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="B52" s="24">
         <v>147213592</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="21"/>
@@ -11274,7 +11245,7 @@
         <v>328</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="21"/>
@@ -11296,13 +11267,13 @@
     </row>
     <row r="55" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="B55" s="24">
         <v>871478110</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="21"/>
@@ -11310,13 +11281,13 @@
     </row>
     <row r="56" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="B56" s="61" t="s">
+        <v>539</v>
+      </c>
+      <c r="B56" s="60" t="s">
         <v>323</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="21"/>
@@ -11324,13 +11295,13 @@
     </row>
     <row r="57" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="B57" s="24">
         <v>881131350</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="21"/>
@@ -11344,7 +11315,7 @@
         <v>882661418</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="D58" s="20"/>
       <c r="E58" s="21"/>
@@ -11571,7 +11542,7 @@
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -11708,7 +11679,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -11716,7 +11687,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -11724,7 +11695,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -11732,7 +11703,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -11740,7 +11711,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -11748,17 +11719,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
-      <c r="C7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
+      <c r="C7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
       <c r="I7" s="49"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -11771,22 +11742,22 @@
       <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="58"/>
+      <c r="D8" s="57"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>419</v>
-      </c>
-      <c r="C9" s="55" t="s">
-        <v>458</v>
-      </c>
-      <c r="D9" s="58"/>
+        <v>407</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>408</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="D9" s="57"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -11833,13 +11804,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -11847,13 +11818,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="B14" s="24">
         <v>1019909943</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -11861,13 +11832,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="B15" s="24">
         <v>576971693</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -11875,13 +11846,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="B16" s="24">
         <v>585243190</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
@@ -11898,12 +11869,12 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -11917,7 +11888,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="171" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -11931,7 +11902,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -11945,7 +11916,7 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -11959,7 +11930,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -11973,7 +11944,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -11997,7 +11968,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -12012,7 +11983,7 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>357</v>
       </c>
@@ -12035,7 +12006,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -12055,7 +12026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -12065,7 +12036,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="270.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
         <v>357</v>
       </c>
@@ -12079,7 +12050,7 @@
       <c r="E13" s="42"/>
       <c r="F13" s="43"/>
     </row>
-    <row r="14" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
         <v>357</v>
       </c>
@@ -12093,7 +12064,7 @@
       <c r="E14" s="42"/>
       <c r="F14" s="43"/>
     </row>
-    <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
         <v>360</v>
       </c>
@@ -12139,7 +12110,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -12152,7 +12123,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -12160,7 +12131,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12168,7 +12139,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12176,7 +12147,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -12189,7 +12160,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -12220,22 +12191,22 @@
     </row>
     <row r="9" spans="1:7" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -12245,10 +12216,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -12258,10 +12229,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -12271,10 +12242,10 @@
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -12341,9 +12312,9 @@
         <v>19</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
@@ -12368,13 +12339,13 @@
     </row>
     <row r="22" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="B22" s="24">
         <v>837414458</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -12382,13 +12353,13 @@
     </row>
     <row r="23" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="B23" s="24">
         <v>829179151</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -12396,13 +12367,13 @@
     </row>
     <row r="24" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -12410,13 +12381,13 @@
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
       <c r="B25" s="24">
         <v>827757425</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -12424,13 +12395,13 @@
     </row>
     <row r="26" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="B26" s="24">
         <v>1666928607</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -12438,13 +12409,13 @@
     </row>
     <row r="27" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="B27" s="24">
         <v>1048425584</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>694</v>
+        <v>683</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -12452,13 +12423,13 @@
     </row>
     <row r="28" spans="1:8" ht="114" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="B28" s="24">
         <v>1032610050</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -12466,13 +12437,13 @@
     </row>
     <row r="29" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="B29" s="24">
         <v>825759323</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
@@ -12687,8 +12658,8 @@
       <c r="A14" s="40" t="s">
         <v>368</v>
       </c>
-      <c r="B14" s="66" t="s">
-        <v>683</v>
+      <c r="B14" s="65" t="s">
+        <v>672</v>
       </c>
       <c r="C14" s="41" t="s">
         <v>371</v>
@@ -12824,7 +12795,7 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
       <c r="D9" s="10"/>
     </row>
@@ -12918,7 +12889,7 @@
         <v>884572641</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -12932,7 +12903,7 @@
         <v>383</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -13056,7 +13027,7 @@
         <v>387</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="D9" s="10"/>
     </row>
@@ -13126,13 +13097,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>383</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -13140,13 +13111,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="B17" s="24">
         <v>885659430</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -13177,12 +13148,12 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -13196,7 +13167,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -13210,7 +13181,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -13224,7 +13195,7 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -13238,7 +13209,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -13252,7 +13223,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -13276,7 +13247,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -13291,7 +13262,7 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>393</v>
       </c>
@@ -13312,7 +13283,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -13332,7 +13303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -13342,7 +13313,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
         <v>393</v>
       </c>
@@ -13372,15 +13343,18 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="31.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -13394,12 +13368,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>396</v>
+      <c r="B2" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -13408,12 +13382,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -13422,12 +13396,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -13436,12 +13410,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>399</v>
+        <v>687</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -13450,12 +13424,12 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>400</v>
+        <v>688</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -13474,7 +13448,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -13489,112 +13463,137 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>401</v>
+        <v>690</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>402</v>
-      </c>
-      <c r="C9" s="74" t="s">
-        <v>403</v>
+        <v>397</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>689</v>
       </c>
       <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>404</v>
+        <v>691</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>405</v>
-      </c>
-      <c r="C10" s="74"/>
+        <v>398</v>
+      </c>
+      <c r="C10" s="73"/>
       <c r="D10" s="38"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>407</v>
-      </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="38"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-    </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>692</v>
+      </c>
+      <c r="B14" s="24">
+        <v>868759473</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>399</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>408</v>
+        <v>694</v>
       </c>
       <c r="B15" s="24">
-        <v>868759473</v>
+        <v>219053618</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>409</v>
+        <v>695</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
       <c r="F15" s="43" t="s">
-        <v>410</v>
-      </c>
+        <v>696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>697</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>700</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>698</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="74"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="75"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -13621,7 +13620,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -13634,7 +13633,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -13642,7 +13641,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13650,7 +13649,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13658,7 +13657,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -13671,7 +13670,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -13708,16 +13707,16 @@
         <v>270</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -13727,10 +13726,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -13740,10 +13739,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -13801,9 +13800,9 @@
         <v>19</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
@@ -13834,7 +13833,7 @@
         <v>788134256</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -13842,13 +13841,13 @@
     </row>
     <row r="21" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="B21" s="24">
         <v>792994558</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
@@ -13856,13 +13855,13 @@
     </row>
     <row r="22" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="B22" s="24">
         <v>818940786</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -13870,13 +13869,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="B23" s="24">
         <v>790280035</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -13884,13 +13883,13 @@
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="B24" s="24">
         <v>880340185</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -13898,13 +13897,13 @@
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="B25" s="24">
         <v>859546233</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -13912,13 +13911,13 @@
     </row>
     <row r="26" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>544</v>
+        <v>533</v>
       </c>
       <c r="B26" s="24">
         <v>875950426</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -13926,13 +13925,13 @@
     </row>
     <row r="27" spans="1:8" ht="285" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="B27" s="24">
         <v>1042460965</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -14091,7 +14090,7 @@
         <v>877327637</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -14119,7 +14118,7 @@
         <v>873533267</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -14258,8 +14257,8 @@
       <c r="B9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>447</v>
+      <c r="C9" s="66" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -14269,7 +14268,7 @@
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="67"/>
     </row>
     <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -14278,7 +14277,7 @@
       <c r="B11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="67"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -14287,7 +14286,7 @@
       <c r="B12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="67"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -14296,7 +14295,7 @@
       <c r="B13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="68"/>
+      <c r="C13" s="67"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -14305,80 +14304,80 @@
       <c r="B14" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="68"/>
+      <c r="C14" s="67"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="68"/>
+      <c r="C15" s="67"/>
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="C16" s="68"/>
+        <v>423</v>
+      </c>
+      <c r="C16" s="67"/>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="67"/>
       <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="67"/>
       <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="68"/>
+      <c r="C19" s="67"/>
       <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="68"/>
+      <c r="C20" s="67"/>
       <c r="I20" s="28"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="68"/>
+      <c r="C21" s="67"/>
       <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="69"/>
+      <c r="C22" s="68"/>
       <c r="I22" s="28"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="44"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -14432,10 +14431,10 @@
         <v>521722950</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
@@ -14448,10 +14447,10 @@
         <v>63</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
@@ -14464,10 +14463,10 @@
         <v>725223227</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
@@ -14480,10 +14479,10 @@
         <v>860726789</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
@@ -14574,7 +14573,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -14582,7 +14581,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -14597,7 +14596,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -14629,8 +14628,8 @@
       <c r="B9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="70" t="s">
-        <v>448</v>
+      <c r="C9" s="69" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -14640,7 +14639,7 @@
       <c r="B10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="70"/>
+      <c r="C10" s="69"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -14649,7 +14648,7 @@
       <c r="B11" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="69"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -14658,7 +14657,7 @@
       <c r="B12" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="69"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -14667,7 +14666,7 @@
       <c r="B13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="70"/>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -14676,7 +14675,7 @@
       <c r="B14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="69"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -14686,62 +14685,62 @@
       <c r="B15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="70"/>
+      <c r="C15" s="69"/>
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="70"/>
+      <c r="C16" s="69"/>
       <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="C17" s="70"/>
+        <v>423</v>
+      </c>
+      <c r="C17" s="69"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="70"/>
+      <c r="C18" s="69"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="70"/>
+      <c r="C19" s="69"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="70"/>
+      <c r="C20" s="69"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="70"/>
+      <c r="C21" s="69"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="70"/>
+      <c r="C22" s="69"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -14812,45 +14811,45 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="B31" s="24">
         <v>520959078</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="B32" s="24">
         <v>1005410313</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="B33" s="24">
         <v>657009032</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="21"/>
@@ -14858,39 +14857,39 @@
     </row>
     <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="B35" s="24">
         <v>875683843</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="B36" s="24">
         <v>867529938</v>
@@ -14932,7 +14931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -14974,7 +14973,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -14982,7 +14981,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -14995,7 +14994,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -15035,7 +15034,7 @@
       <c r="B9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="68" t="s">
         <v>94</v>
       </c>
       <c r="E9" s="27"/>
@@ -15047,7 +15046,7 @@
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="68"/>
     </row>
     <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -15056,7 +15055,7 @@
       <c r="B11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="68"/>
     </row>
     <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -15065,7 +15064,7 @@
       <c r="B12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="69"/>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -15074,7 +15073,7 @@
       <c r="B13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="68"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -15084,7 +15083,7 @@
       <c r="B14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="68"/>
       <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="57" x14ac:dyDescent="0.2">
@@ -15094,7 +15093,7 @@
       <c r="B15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="68"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -15103,7 +15102,7 @@
       <c r="B16" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="69"/>
+      <c r="C16" s="68"/>
     </row>
     <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -15112,7 +15111,7 @@
       <c r="B17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="69"/>
+      <c r="C17" s="68"/>
     </row>
     <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -15121,7 +15120,7 @@
       <c r="B18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="69"/>
+      <c r="C18" s="68"/>
     </row>
     <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -15130,7 +15129,7 @@
       <c r="B19" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="69"/>
+      <c r="C19" s="68"/>
     </row>
     <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -15139,7 +15138,7 @@
       <c r="B20" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="69"/>
+      <c r="C20" s="68"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -15148,7 +15147,7 @@
       <c r="B21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="68"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -15233,13 +15232,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>113</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -15247,16 +15246,16 @@
     </row>
     <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
       <c r="B29" s="29">
         <v>860726789</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>690</v>
+        <v>679</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>

</xml_diff>

<commit_message>
Added production information to the detail view of records. Added test for production information. Updated rda.xlsx. refs #371
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vagrant\thulb\vufind\module\ThULB\tests\fixtures\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="992" firstSheet="21" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="992" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -23,30 +23,31 @@
     <sheet name="Sprachangaben" sheetId="7" r:id="rId9"/>
     <sheet name="Angaben über Sprache und Schrif" sheetId="8" r:id="rId10"/>
     <sheet name="Publikationsangaben" sheetId="9" r:id="rId11"/>
-    <sheet name="Teil von" sheetId="35" r:id="rId12"/>
-    <sheet name="Schlagworte" sheetId="33" r:id="rId13"/>
-    <sheet name="Art des Inhalts" sheetId="34" r:id="rId14"/>
-    <sheet name="Druckort" sheetId="10" r:id="rId15"/>
-    <sheet name="Hochschulschriftenvermerk" sheetId="11" r:id="rId16"/>
-    <sheet name="Maßstab bei Karten" sheetId="12" r:id="rId17"/>
-    <sheet name="Projektion bei Karten" sheetId="13" r:id="rId18"/>
-    <sheet name="Koordinaten bei Karten" sheetId="14" r:id="rId19"/>
-    <sheet name="Erscheinungsverlauf" sheetId="15" r:id="rId20"/>
-    <sheet name="Anmerkungen zum Erscheinungsver" sheetId="16" r:id="rId21"/>
-    <sheet name="Mehr zum Titel" sheetId="17" r:id="rId22"/>
-    <sheet name="Verwandte Ressourcen" sheetId="18" r:id="rId23"/>
-    <sheet name="Vorheriger Späterer Titel" sheetId="19" r:id="rId24"/>
-    <sheet name="Anmerkungen" sheetId="20" r:id="rId25"/>
-    <sheet name="Werktitel" sheetId="21" r:id="rId26"/>
-    <sheet name="Umfang" sheetId="22" r:id="rId27"/>
-    <sheet name="Sekundäre Ausgabe" sheetId="29" r:id="rId28"/>
-    <sheet name="Fingerprint" sheetId="23" r:id="rId29"/>
-    <sheet name="Bibliographische Zitate" sheetId="24" r:id="rId30"/>
-    <sheet name="ISBN" sheetId="25" r:id="rId31"/>
-    <sheet name="Falsche ISBN" sheetId="26" r:id="rId32"/>
-    <sheet name="ZDB-Nummer" sheetId="27" r:id="rId33"/>
-    <sheet name="Basisklassifikation" sheetId="28" r:id="rId34"/>
-    <sheet name="Inhaltsangaben" sheetId="30" r:id="rId35"/>
+    <sheet name="Herstellungsangabe" sheetId="38" r:id="rId12"/>
+    <sheet name="Teil von" sheetId="35" r:id="rId13"/>
+    <sheet name="Schlagworte" sheetId="33" r:id="rId14"/>
+    <sheet name="Art des Inhalts" sheetId="34" r:id="rId15"/>
+    <sheet name="Druckort" sheetId="10" r:id="rId16"/>
+    <sheet name="Hochschulschriftenvermerk" sheetId="11" r:id="rId17"/>
+    <sheet name="Maßstab bei Karten" sheetId="12" r:id="rId18"/>
+    <sheet name="Projektion bei Karten" sheetId="13" r:id="rId19"/>
+    <sheet name="Koordinaten bei Karten" sheetId="14" r:id="rId20"/>
+    <sheet name="Erscheinungsverlauf" sheetId="15" r:id="rId21"/>
+    <sheet name="Anmerkungen zum Erscheinungsver" sheetId="16" r:id="rId22"/>
+    <sheet name="Mehr zum Titel" sheetId="17" r:id="rId23"/>
+    <sheet name="Verwandte Ressourcen" sheetId="18" r:id="rId24"/>
+    <sheet name="Vorheriger Späterer Titel" sheetId="19" r:id="rId25"/>
+    <sheet name="Anmerkungen" sheetId="20" r:id="rId26"/>
+    <sheet name="Werktitel" sheetId="21" r:id="rId27"/>
+    <sheet name="Umfang" sheetId="22" r:id="rId28"/>
+    <sheet name="Sekundäre Ausgabe" sheetId="29" r:id="rId29"/>
+    <sheet name="Fingerprint" sheetId="23" r:id="rId30"/>
+    <sheet name="Bibliographische Zitate" sheetId="24" r:id="rId31"/>
+    <sheet name="ISBN" sheetId="25" r:id="rId32"/>
+    <sheet name="Falsche ISBN" sheetId="26" r:id="rId33"/>
+    <sheet name="ZDB-Nummer" sheetId="27" r:id="rId34"/>
+    <sheet name="Basisklassifikation" sheetId="28" r:id="rId35"/>
+    <sheet name="Inhaltsangaben" sheetId="30" r:id="rId36"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -561,7 +562,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="711">
   <si>
     <t>Titel</t>
   </si>
@@ -4066,6 +4067,36 @@
   </si>
   <si>
     <t>021499845</t>
+  </si>
+  <si>
+    <t>Anzeige der Herstellungsangaben</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Ticket #371</t>
+  </si>
+  <si>
+    <t>264 $a und $b</t>
+  </si>
+  <si>
+    <t>Darstellung im Format „264a [; 264a[...]] : 264b“</t>
+  </si>
+  <si>
+    <t>Ind. 2 = 0</t>
+  </si>
+  <si>
+    <t>Ind. 2 = 1 oder 3</t>
+  </si>
+  <si>
+    <t>Herstellungsangabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264 $a, $b </t>
+  </si>
+  <si>
+    <t>Münster : Verl.-Haus Monsenstein und Vannerdat</t>
   </si>
 </sst>
 </file>
@@ -4395,7 +4426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4566,6 +4597,11 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4590,8 +4626,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -6576,7 +6610,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6700,7 +6734,9 @@
       <c r="B9" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="38" t="s">
+        <v>707</v>
+      </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -6789,9 +6825,6 @@
       <c r="F15" s="43"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <extLst>
@@ -6803,6 +6836,203 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="43.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>704</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>705</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>706</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>709</v>
+      </c>
+      <c r="B13" s="24">
+        <v>644808608</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>710</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
@@ -6899,7 +7129,7 @@
       <c r="B9" s="9" t="s">
         <v>608</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="72" t="s">
         <v>619</v>
       </c>
     </row>
@@ -6910,12 +7140,12 @@
       <c r="B10" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="69"/>
+      <c r="C11" s="72"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -6924,7 +7154,7 @@
       <c r="B12" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="C12" s="69"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -6933,12 +7163,12 @@
       <c r="B13" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="72"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="69"/>
+      <c r="C14" s="72"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -6947,7 +7177,7 @@
       <c r="B15" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="72"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -6956,12 +7186,12 @@
       <c r="B16" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="C16" s="69"/>
+      <c r="C16" s="72"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="69"/>
+      <c r="C17" s="72"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -6970,7 +7200,7 @@
       <c r="B18" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="C18" s="69"/>
+      <c r="C18" s="72"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -6979,12 +7209,12 @@
       <c r="B19" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="C19" s="69"/>
+      <c r="C19" s="72"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="69"/>
+      <c r="C20" s="72"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -6993,7 +7223,7 @@
       <c r="B21" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="72"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
@@ -7002,12 +7232,12 @@
       <c r="B22" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="72"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="69"/>
+      <c r="C23" s="72"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
@@ -7016,72 +7246,72 @@
       <c r="B24" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="69"/>
+      <c r="C24" s="72"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="69"/>
+      <c r="C25" s="72"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="69"/>
+      <c r="C26" s="72"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="69"/>
+      <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="69"/>
+      <c r="C28" s="72"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="69"/>
+      <c r="C29" s="72"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="69"/>
+      <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="69"/>
+      <c r="C31" s="72"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="69"/>
+      <c r="C32" s="72"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="69"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="69"/>
+      <c r="C34" s="72"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="69"/>
+      <c r="C35" s="72"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="69"/>
+      <c r="C36" s="72"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="69"/>
+      <c r="C37" s="72"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -7283,7 +7513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
@@ -7380,7 +7610,7 @@
       <c r="B9" s="9" t="s">
         <v>568</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="72" t="s">
         <v>593</v>
       </c>
     </row>
@@ -7391,7 +7621,7 @@
       <c r="B10" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -7400,12 +7630,12 @@
       <c r="B11" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="72"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="69"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -7414,7 +7644,7 @@
       <c r="B13" s="9" t="s">
         <v>574</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="72"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -7423,7 +7653,7 @@
       <c r="B14" s="9" t="s">
         <v>576</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="72"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -7432,117 +7662,117 @@
       <c r="B15" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="72"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="69"/>
+      <c r="C16" s="72"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="69"/>
+      <c r="C17" s="72"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="69"/>
+      <c r="C18" s="72"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="69"/>
+      <c r="C19" s="72"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="69"/>
+      <c r="C20" s="72"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="69"/>
+      <c r="C21" s="72"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="69"/>
+      <c r="C22" s="72"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="69"/>
+      <c r="C23" s="72"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="69"/>
+      <c r="C24" s="72"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="69"/>
+      <c r="C25" s="72"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="69"/>
+      <c r="C26" s="72"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="69"/>
+      <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="69"/>
+      <c r="C28" s="72"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="69"/>
+      <c r="C29" s="72"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="69"/>
+      <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="69"/>
+      <c r="C31" s="72"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="69"/>
+      <c r="C32" s="72"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="69"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="69"/>
+      <c r="C34" s="72"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="69"/>
+      <c r="C35" s="72"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="69"/>
+      <c r="C36" s="72"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="69"/>
+      <c r="C37" s="72"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -7673,7 +7903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -7957,7 +8187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -8163,7 +8393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -8367,7 +8597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -8546,204 +8776,6 @@
       </c>
       <c r="C13" s="41" t="s">
         <v>196</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" s="24">
-        <v>470336242</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>203</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -8767,18 +8799,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -8787,12 +8819,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8801,12 +8833,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -8815,12 +8847,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -8829,12 +8861,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8843,7 +8875,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -8867,7 +8899,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -8882,9 +8914,9 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -8903,7 +8935,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -8923,7 +8955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -8935,13 +8967,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B13" s="24">
         <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>446</v>
+        <v>203</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -9261,18 +9293,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -9281,12 +9313,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -9295,12 +9327,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -9309,12 +9341,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -9323,12 +9355,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -9337,12 +9369,12 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -9361,7 +9393,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -9376,13 +9408,11 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>216</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B9" s="37"/>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -9399,7 +9429,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -9419,7 +9449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -9429,15 +9459,15 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B13" s="24">
-        <v>233814418</v>
+        <v>470336242</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>217</v>
+        <v>446</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -9459,20 +9489,20 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -9481,12 +9511,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -9495,12 +9525,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -9509,12 +9539,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -9523,12 +9553,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -9537,12 +9567,12 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -9561,7 +9591,7 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -9576,12 +9606,12 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
@@ -9599,7 +9629,7 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -9619,7 +9649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -9629,33 +9659,19 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B13" s="24">
         <v>233814418</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>671</v>
+      <c r="C13" s="41" t="s">
+        <v>217</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
       <c r="F13" s="43"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="B14" s="24">
-        <v>502081112</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9672,6 +9688,220 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="24">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>671</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" s="24">
+        <v>502081112</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -9847,7 +10077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9960,7 +10190,7 @@
       <c r="B9" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="73" t="s">
         <v>665</v>
       </c>
     </row>
@@ -9971,7 +10201,7 @@
       <c r="B10" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="70"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -9980,7 +10210,7 @@
       <c r="B11" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="70"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -9989,7 +10219,7 @@
       <c r="B12" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
     </row>
     <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -9998,7 +10228,7 @@
       <c r="B13" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -10007,12 +10237,12 @@
       <c r="B14" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="C14" s="67"/>
+      <c r="C14" s="70"/>
     </row>
     <row r="15" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="68"/>
+      <c r="C15" s="71"/>
     </row>
     <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
@@ -10104,7 +10334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -10205,7 +10435,7 @@
       <c r="B9" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="74" t="s">
         <v>675</v>
       </c>
     </row>
@@ -10216,7 +10446,7 @@
       <c r="B10" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="72"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -10228,7 +10458,7 @@
       <c r="B11" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -10240,7 +10470,7 @@
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="72"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -10351,7 +10581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
@@ -10717,7 +10947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
@@ -10816,7 +11046,7 @@
       <c r="B9" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="72" t="s">
         <v>595</v>
       </c>
     </row>
@@ -10827,7 +11057,7 @@
       <c r="B10" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -10836,7 +11066,7 @@
       <c r="B11" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="72"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -10845,7 +11075,7 @@
       <c r="B12" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C12" s="69"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -10854,7 +11084,7 @@
       <c r="B13" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="72"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -10863,7 +11093,7 @@
       <c r="B14" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="72"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -10872,7 +11102,7 @@
       <c r="B15" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="72"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -10881,7 +11111,7 @@
       <c r="B16" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C16" s="69"/>
+      <c r="C16" s="72"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -10890,7 +11120,7 @@
       <c r="B17" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C17" s="69"/>
+      <c r="C17" s="72"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -10899,7 +11129,7 @@
       <c r="B18" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="C18" s="69"/>
+      <c r="C18" s="72"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -10908,7 +11138,7 @@
       <c r="B19" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="69"/>
+      <c r="C19" s="72"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -10917,7 +11147,7 @@
       <c r="B20" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="C20" s="69"/>
+      <c r="C20" s="72"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -10926,7 +11156,7 @@
       <c r="B21" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="72"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
@@ -10935,12 +11165,12 @@
       <c r="B22" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C22" s="69"/>
+      <c r="C22" s="72"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="69"/>
+      <c r="C23" s="72"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
@@ -10949,7 +11179,7 @@
       <c r="B24" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="69"/>
+      <c r="C24" s="72"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
@@ -10958,7 +11188,7 @@
       <c r="B25" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C25" s="69"/>
+      <c r="C25" s="72"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
@@ -10967,7 +11197,7 @@
       <c r="B26" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C26" s="69"/>
+      <c r="C26" s="72"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
@@ -10976,7 +11206,7 @@
       <c r="B27" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C27" s="69"/>
+      <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
@@ -10985,7 +11215,7 @@
       <c r="B28" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C28" s="69"/>
+      <c r="C28" s="72"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
@@ -10994,7 +11224,7 @@
       <c r="B29" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="72"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
@@ -11003,7 +11233,7 @@
       <c r="B30" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C30" s="69"/>
+      <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
@@ -11012,7 +11242,7 @@
       <c r="B31" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C31" s="69"/>
+      <c r="C31" s="72"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
@@ -11021,7 +11251,7 @@
       <c r="B32" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C32" s="69"/>
+      <c r="C32" s="72"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
@@ -11030,7 +11260,7 @@
       <c r="B33" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="C33" s="69"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
@@ -11039,7 +11269,7 @@
       <c r="B34" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="C34" s="69"/>
+      <c r="C34" s="72"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
@@ -11048,7 +11278,7 @@
       <c r="B35" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="C35" s="69"/>
+      <c r="C35" s="72"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
@@ -11057,7 +11287,7 @@
       <c r="B36" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C36" s="69"/>
+      <c r="C36" s="72"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
@@ -11066,7 +11296,7 @@
       <c r="B37" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="C37" s="69"/>
+      <c r="C37" s="72"/>
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -11345,7 +11575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -11660,7 +11890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -11861,234 +12091,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>357</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>353</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
-        <v>357</v>
-      </c>
-      <c r="B13" s="24">
-        <v>151797196</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>358</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-    </row>
-    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
-        <v>357</v>
-      </c>
-      <c r="B14" s="24">
-        <v>770927416</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>359</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-    </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
-        <v>360</v>
-      </c>
-      <c r="B15" s="24">
-        <v>194273989</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>361</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12473,17 +12475,17 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="37" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -12492,12 +12494,12 @@
       <c r="G1" s="30"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -12506,12 +12508,12 @@
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -12520,12 +12522,12 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -12534,12 +12536,12 @@
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -12553,7 +12555,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -12589,10 +12591,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -12640,29 +12642,29 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="B13" s="24">
         <v>151797196</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
       <c r="F13" s="43"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>368</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>672</v>
+        <v>357</v>
+      </c>
+      <c r="B14" s="24">
+        <v>770927416</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
@@ -12670,13 +12672,13 @@
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="B15" s="24">
-        <v>409606901</v>
+        <v>194273989</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
@@ -12697,6 +12699,234 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="37" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>368</v>
+      </c>
+      <c r="B13" s="24">
+        <v>151797196</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="40" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>672</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>371</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>372</v>
+      </c>
+      <c r="B15" s="24">
+        <v>409606901</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -12908,220 +13138,6 @@
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>651</v>
-      </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>383</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>647</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>649</v>
-      </c>
-      <c r="B17" s="24">
-        <v>885659430</v>
-      </c>
-      <c r="C17" s="53" t="s">
-        <v>646</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13144,6 +13160,220 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>647</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="B17" s="24">
+        <v>885659430</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>646</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -13341,11 +13571,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -13470,7 +13700,7 @@
       <c r="B9" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="76" t="s">
         <v>689</v>
       </c>
       <c r="D9" s="38"/>
@@ -13485,7 +13715,7 @@
       <c r="B10" s="37" t="s">
         <v>398</v>
       </c>
-      <c r="C10" s="73"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="38"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -13580,13 +13810,13 @@
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="74"/>
+      <c r="C19" s="67"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="75"/>
+      <c r="D20" s="68"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="74"/>
+      <c r="D21" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13602,7 +13832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
@@ -14257,7 +14487,7 @@
       <c r="B9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="69" t="s">
         <v>436</v>
       </c>
     </row>
@@ -14268,7 +14498,7 @@
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="70"/>
     </row>
     <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -14277,7 +14507,7 @@
       <c r="B11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="70"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -14286,7 +14516,7 @@
       <c r="B12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="70"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -14295,7 +14525,7 @@
       <c r="B13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="70"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -14304,13 +14534,13 @@
       <c r="B14" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="67"/>
+      <c r="C14" s="70"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="67"/>
+      <c r="C15" s="70"/>
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -14320,7 +14550,7 @@
       <c r="B16" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="C16" s="67"/>
+      <c r="C16" s="70"/>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -14330,7 +14560,7 @@
       <c r="B17" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="67"/>
+      <c r="C17" s="70"/>
       <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -14340,7 +14570,7 @@
       <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="70"/>
       <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -14350,7 +14580,7 @@
       <c r="B19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="67"/>
+      <c r="C19" s="70"/>
       <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -14360,19 +14590,19 @@
       <c r="B20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="67"/>
+      <c r="C20" s="70"/>
       <c r="I20" s="28"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="67"/>
+      <c r="C21" s="70"/>
       <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="68"/>
+      <c r="C22" s="71"/>
       <c r="I22" s="28"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -14628,7 +14858,7 @@
       <c r="B9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="72" t="s">
         <v>437</v>
       </c>
     </row>
@@ -14639,7 +14869,7 @@
       <c r="B10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -14648,7 +14878,7 @@
       <c r="B11" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="72"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -14657,7 +14887,7 @@
       <c r="B12" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="69"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -14666,7 +14896,7 @@
       <c r="B13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="72"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -14675,7 +14905,7 @@
       <c r="B14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="72"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -14685,13 +14915,13 @@
       <c r="B15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="72"/>
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="69"/>
+      <c r="C16" s="72"/>
       <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -14701,7 +14931,7 @@
       <c r="B17" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="C17" s="69"/>
+      <c r="C17" s="72"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -14710,7 +14940,7 @@
       <c r="B18" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="69"/>
+      <c r="C18" s="72"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -14719,7 +14949,7 @@
       <c r="B19" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="69"/>
+      <c r="C19" s="72"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -14728,7 +14958,7 @@
       <c r="B20" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="69"/>
+      <c r="C20" s="72"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -14737,10 +14967,10 @@
       <c r="B21" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="72"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="69"/>
+      <c r="C22" s="72"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -15034,7 +15264,7 @@
       <c r="B9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="71" t="s">
         <v>94</v>
       </c>
       <c r="E9" s="27"/>
@@ -15046,7 +15276,7 @@
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -15055,7 +15285,7 @@
       <c r="B11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="71"/>
     </row>
     <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -15064,7 +15294,7 @@
       <c r="B12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="68"/>
+      <c r="C12" s="71"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -15073,7 +15303,7 @@
       <c r="B13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="68"/>
+      <c r="C13" s="71"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -15083,7 +15313,7 @@
       <c r="B14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="68"/>
+      <c r="C14" s="71"/>
       <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="57" x14ac:dyDescent="0.2">
@@ -15093,7 +15323,7 @@
       <c r="B15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="71"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -15102,7 +15332,7 @@
       <c r="B16" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="71"/>
     </row>
     <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -15111,7 +15341,7 @@
       <c r="B17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="71"/>
     </row>
     <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -15120,7 +15350,7 @@
       <c r="B18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="68"/>
+      <c r="C18" s="71"/>
     </row>
     <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -15129,7 +15359,7 @@
       <c r="B19" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="68"/>
+      <c r="C19" s="71"/>
     </row>
     <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
@@ -15138,7 +15368,7 @@
       <c r="B20" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="68"/>
+      <c r="C20" s="71"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -15147,7 +15377,7 @@
       <c r="B21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="68"/>
+      <c r="C21" s="71"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>

</xml_diff>

<commit_message>
Changed separator for multiple 'j' subfields in basic classification to comma. Updated rda.xlsx refs #402
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vagrant\thulb\vufind\module\ThULB\tests\fixtures\spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="992" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="992" firstSheet="22" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -4026,77 +4026,77 @@
     <t>Ticket #97, Ticket #402</t>
   </si>
   <si>
+    <t>936 $a</t>
+  </si>
+  <si>
+    <t>936 $j</t>
+  </si>
+  <si>
+    <t>2x 936 Ind.1=b Ind. 2=k $a $j</t>
+  </si>
+  <si>
+    <t>/Search/Results?lookfor=%2279.65%22&amp;type=bklnumber
+/Search/Results?lookfor=%2281.92%22&amp;type=bklnumber</t>
+  </si>
+  <si>
+    <t>1x 936 Ind.1=b Ind. 2=k $a $j $j</t>
+  </si>
+  <si>
+    <t>/Search/Results?lookfor=%2221.80%22&amp;type=bklnumber</t>
+  </si>
+  <si>
+    <t>2x 936 Ind.1=b Ind. 2=k $a</t>
+  </si>
+  <si>
+    <t>15.51
+15.31</t>
+  </si>
+  <si>
+    <t>/Search/Results?lookfor=%2215.51%22&amp;type=bklnumber
+/Search/Results?lookfor=%2215.31%22&amp;type=bklnumber</t>
+  </si>
+  <si>
+    <t>021499845</t>
+  </si>
+  <si>
+    <t>Anzeige der Herstellungsangaben</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Ticket #371</t>
+  </si>
+  <si>
+    <t>264 $a und $b</t>
+  </si>
+  <si>
+    <t>Darstellung im Format „264a [; 264a[...]] : 264b“</t>
+  </si>
+  <si>
+    <t>Ind. 2 = 0</t>
+  </si>
+  <si>
+    <t>Ind. 2 = 1 oder 3</t>
+  </si>
+  <si>
+    <t>Herstellungsangabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264 $a, $b </t>
+  </si>
+  <si>
+    <t>Münster : Verl.-Haus Monsenstein und Vannerdat</t>
+  </si>
+  <si>
+    <t>21.80 Kunsthandwerk, Kunstgewerbe: Allgemeines</t>
+  </si>
+  <si>
     <t>Wenn in 936 Ind. 1 = b und Ind. 2 = k
 936 $a $j
-$j ist wiederholbar &gt; Darstellung nacheineinander, Trennung durch &gt;
+$j ist wiederholbar &gt; Darstellung nacheineinander, Trennung durch ","
 mehrere 936 werden untereinander abgebildet
 Auf jede Notation einen Suchlink legen: Indexsuche mit Inhalt von 936 $a</t>
-  </si>
-  <si>
-    <t>936 $a</t>
-  </si>
-  <si>
-    <t>936 $j</t>
-  </si>
-  <si>
-    <t>2x 936 Ind.1=b Ind. 2=k $a $j</t>
-  </si>
-  <si>
-    <t>/Search/Results?lookfor=%2279.65%22&amp;type=bklnumber
-/Search/Results?lookfor=%2281.92%22&amp;type=bklnumber</t>
-  </si>
-  <si>
-    <t>1x 936 Ind.1=b Ind. 2=k $a $j $j</t>
-  </si>
-  <si>
-    <t>21.80 Kunsthandwerk &gt; Kunstgewerbe: Allgemeines</t>
-  </si>
-  <si>
-    <t>/Search/Results?lookfor=%2221.80%22&amp;type=bklnumber</t>
-  </si>
-  <si>
-    <t>2x 936 Ind.1=b Ind. 2=k $a</t>
-  </si>
-  <si>
-    <t>15.51
-15.31</t>
-  </si>
-  <si>
-    <t>/Search/Results?lookfor=%2215.51%22&amp;type=bklnumber
-/Search/Results?lookfor=%2215.31%22&amp;type=bklnumber</t>
-  </si>
-  <si>
-    <t>021499845</t>
-  </si>
-  <si>
-    <t>Anzeige der Herstellungsangaben</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>Ticket #371</t>
-  </si>
-  <si>
-    <t>264 $a und $b</t>
-  </si>
-  <si>
-    <t>Darstellung im Format „264a [; 264a[...]] : 264b“</t>
-  </si>
-  <si>
-    <t>Ind. 2 = 0</t>
-  </si>
-  <si>
-    <t>Ind. 2 = 1 oder 3</t>
-  </si>
-  <si>
-    <t>Herstellungsangabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">264 $a, $b </t>
-  </si>
-  <si>
-    <t>Münster : Verl.-Haus Monsenstein und Vannerdat</t>
   </si>
 </sst>
 </file>
@@ -6735,7 +6735,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -6839,7 +6839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -6853,7 +6853,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -6867,7 +6867,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -6895,7 +6895,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -6909,7 +6909,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -6923,7 +6923,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -6959,13 +6959,13 @@
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
+        <v>702</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>703</v>
+      </c>
+      <c r="C9" s="66" t="s">
         <v>704</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>705</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>706</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -7014,13 +7014,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B13" s="24">
         <v>644808608</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="42"/>
@@ -13575,8 +13575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13695,13 +13695,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>397</v>
       </c>
       <c r="C9" s="76" t="s">
-        <v>689</v>
+        <v>710</v>
       </c>
       <c r="D9" s="38"/>
       <c r="F9" s="3"/>
@@ -13710,7 +13710,7 @@
     </row>
     <row r="10" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B10" s="37" t="s">
         <v>398</v>
@@ -13763,7 +13763,7 @@
     </row>
     <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A14" s="40" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B14" s="24">
         <v>868759473</v>
@@ -13774,39 +13774,39 @@
       <c r="D14" s="20"/>
       <c r="E14" s="42"/>
       <c r="F14" s="43" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B15" s="24">
         <v>219053618</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>695</v>
+        <v>709</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="42"/>
       <c r="F15" s="43" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="42"/>
       <c r="F16" s="43" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
B&m: Display the URN in detail view. Added unit test for URN. Updated rda.xlsx. refs #479
</commit_message>
<xml_diff>
--- a/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
+++ b/vufind/module/ThULB/tests/fixtures/spreadsheet/rda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f6bema\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91AB775-2931-4B1A-B1B3-4B3C9CB2E6FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1B70F38-FD62-4142-8D9E-7E6B3C67E4DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="14148" tabRatio="500" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="14148" tabRatio="500" firstSheet="31" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" r:id="rId1"/>
@@ -48,13 +48,14 @@
     <sheet name="ISSN" sheetId="39" r:id="rId33"/>
     <sheet name="ISMN" sheetId="40" r:id="rId34"/>
     <sheet name="DOI" sheetId="42" r:id="rId35"/>
-    <sheet name="ZDB-Nummer" sheetId="34" r:id="rId36"/>
-    <sheet name="Basisklassifikation" sheetId="35" r:id="rId37"/>
-    <sheet name="Thüringen-Bibliographie" sheetId="36" r:id="rId38"/>
-    <sheet name="Lokale Notationen" sheetId="37" r:id="rId39"/>
-    <sheet name="Inhaltsangaben" sheetId="38" r:id="rId40"/>
-    <sheet name="Rechteinformation" sheetId="41" r:id="rId41"/>
-    <sheet name="Access Status" sheetId="43" r:id="rId42"/>
+    <sheet name="URN" sheetId="44" r:id="rId36"/>
+    <sheet name="ZDB-Nummer" sheetId="34" r:id="rId37"/>
+    <sheet name="Basisklassifikation" sheetId="35" r:id="rId38"/>
+    <sheet name="Thüringen-Bibliographie" sheetId="36" r:id="rId39"/>
+    <sheet name="Lokale Notationen" sheetId="37" r:id="rId40"/>
+    <sheet name="Inhaltsangaben" sheetId="38" r:id="rId41"/>
+    <sheet name="Rechteinformation" sheetId="41" r:id="rId42"/>
+    <sheet name="Access Status" sheetId="43" r:id="rId43"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -421,7 +422,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2700-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D0E47545-6ECC-4327-B4F3-C3C2360EEFAE}">
       <text>
         <r>
           <rPr>
@@ -446,6 +447,31 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2700-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments24.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2800-000001000000}">
       <text>
         <r>
@@ -465,7 +491,7 @@
 </comments>
 </file>
 
-<file path=xl/comments24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments25.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -666,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="821">
   <si>
     <t>Titel</t>
   </si>
@@ -4839,6 +4865,47 @@
   <si>
     <t xml:space="preserve">650 $a (mehrfach)
 689 $a </t>
+  </si>
+  <si>
+    <t>URN</t>
+  </si>
+  <si>
+    <t>Ticket #479</t>
+  </si>
+  <si>
+    <t>024 $a $2urn</t>
+  </si>
+  <si>
+    <t>urn:nbn:de:gbv:27-dbt-20210119-084917-008</t>
+  </si>
+  <si>
+    <t>$a $2urn</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>URN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $a</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5197,7 +5264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5393,6 +5460,12 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -16050,6 +16123,716 @@
 
 <file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>303840</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC940BAB-7654-4043-82BD-DBD2D9BFCA26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="38015220" cy="3505200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1437480</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>170640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24B01CE-594A-4F58-9F8C-D45B4162695E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9529920" cy="6304740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4796DC47-AF76-4980-A290-9BBCC713543A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E0A9B1-D58D-4FD0-A36E-AE2D25BEEC8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{914B8F74-21B6-49D3-8ABA-B7B581861909}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4512A982-3193-47D4-ABE1-838F48C76C9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF9D2999-8311-4772-9D6E-88349D8FACF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A506F7D-91A1-4CD6-8406-759DF06EA44B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADAFB7F6-34E8-499E-A78C-90BA74182E47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89140C26-D057-484D-95AF-7D50412FC685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37E2007A-0111-44A6-8051-F1E5D828D61E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2826F538-5EE4-4CFA-9F9A-11604A253DEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A6F5C21-F448-49A5-A3BF-50C21A81400C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9530715" cy="6305550"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -16807,7 +17590,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17517,7 +18300,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -24495,7 +25278,7 @@
       <c r="B9" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>744</v>
       </c>
     </row>
@@ -24506,12 +25289,12 @@
       <c r="B10" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="79"/>
+      <c r="C11" s="81"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -24520,7 +25303,7 @@
       <c r="B12" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="81"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -24529,12 +25312,12 @@
       <c r="B13" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="79"/>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="79"/>
+      <c r="C14" s="81"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -24543,7 +25326,7 @@
       <c r="B15" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -24552,12 +25335,12 @@
       <c r="B16" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C16" s="79"/>
+      <c r="C16" s="81"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="79"/>
+      <c r="C17" s="81"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -24566,7 +25349,7 @@
       <c r="B18" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="81"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -24575,12 +25358,12 @@
       <c r="B19" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="79"/>
+      <c r="C19" s="81"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="79"/>
+      <c r="C20" s="81"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -24589,7 +25372,7 @@
       <c r="B21" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C21" s="79"/>
+      <c r="C21" s="81"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
@@ -24598,7 +25381,7 @@
       <c r="B22" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="C22" s="79"/>
+      <c r="C22" s="81"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
@@ -24607,12 +25390,12 @@
       <c r="B23" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C23" s="79"/>
+      <c r="C23" s="81"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="79"/>
+      <c r="C24" s="81"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -24621,67 +25404,67 @@
       <c r="B25" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C25" s="79"/>
+      <c r="C25" s="81"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="79"/>
+      <c r="C26" s="81"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="79"/>
+      <c r="C27" s="81"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="79"/>
+      <c r="C28" s="81"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="79"/>
+      <c r="C29" s="81"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="79"/>
+      <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="79"/>
+      <c r="C31" s="81"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="79"/>
+      <c r="C32" s="81"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="79"/>
+      <c r="C33" s="81"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="79"/>
+      <c r="C34" s="81"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="79"/>
+      <c r="C35" s="81"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="79"/>
+      <c r="C36" s="81"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="79"/>
+      <c r="C37" s="81"/>
       <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -24915,7 +25698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -25008,7 +25791,7 @@
       <c r="B9" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>276</v>
       </c>
     </row>
@@ -25019,7 +25802,7 @@
       <c r="B10" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -25028,12 +25811,12 @@
       <c r="B11" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="81"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="79"/>
+      <c r="C12" s="81"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -25042,7 +25825,7 @@
       <c r="B13" s="9" t="s">
         <v>813</v>
       </c>
-      <c r="C13" s="79"/>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -25051,7 +25834,7 @@
       <c r="B14" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C14" s="79"/>
+      <c r="C14" s="81"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -25060,117 +25843,117 @@
       <c r="B15" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="79"/>
+      <c r="C16" s="81"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="79"/>
+      <c r="C17" s="81"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="79"/>
+      <c r="C18" s="81"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="79"/>
+      <c r="C19" s="81"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="79"/>
+      <c r="C20" s="81"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="79"/>
+      <c r="C21" s="81"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="79"/>
+      <c r="C22" s="81"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="79"/>
+      <c r="C23" s="81"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="79"/>
+      <c r="C24" s="81"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="79"/>
+      <c r="C25" s="81"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="79"/>
+      <c r="C26" s="81"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="79"/>
+      <c r="C27" s="81"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="79"/>
+      <c r="C28" s="81"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="79"/>
+      <c r="C29" s="81"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="79"/>
+      <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="79"/>
+      <c r="C31" s="81"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="79"/>
+      <c r="C32" s="81"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="79"/>
+      <c r="C33" s="81"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="79"/>
+      <c r="C34" s="81"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="79"/>
+      <c r="C35" s="81"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="79"/>
+      <c r="C36" s="81"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="79"/>
+      <c r="C37" s="81"/>
       <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -27383,7 +28166,7 @@
       <c r="B9" s="9" t="s">
         <v>777</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="83" t="s">
         <v>769</v>
       </c>
     </row>
@@ -27394,7 +28177,7 @@
       <c r="B10" s="9" t="s">
         <v>780</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="84"/>
     </row>
     <row r="11" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -27403,7 +28186,7 @@
       <c r="B11" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="84"/>
     </row>
     <row r="12" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -27412,7 +28195,7 @@
       <c r="B12" s="9" t="s">
         <v>778</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="85"/>
     </row>
     <row r="13" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -27421,7 +28204,7 @@
       <c r="B13" s="9" t="s">
         <v>782</v>
       </c>
-      <c r="C13" s="84"/>
+      <c r="C13" s="86"/>
     </row>
     <row r="15" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -27643,7 +28426,7 @@
       <c r="B9" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>707</v>
       </c>
     </row>
@@ -27654,7 +28437,7 @@
       <c r="B10" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -27663,7 +28446,7 @@
       <c r="B11" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="81"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -27672,7 +28455,7 @@
       <c r="B12" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="81"/>
     </row>
     <row r="13" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -27681,7 +28464,7 @@
       <c r="B13" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="C13" s="79"/>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -27690,12 +28473,12 @@
       <c r="B14" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="C14" s="79"/>
+      <c r="C14" s="81"/>
     </row>
     <row r="15" spans="1:7" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
     </row>
     <row r="17" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -27942,7 +28725,7 @@
       <c r="B9" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="87" t="s">
         <v>411</v>
       </c>
     </row>
@@ -27953,7 +28736,7 @@
       <c r="B10" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="85"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -27965,7 +28748,7 @@
       <c r="B11" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="C11" s="85"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -27977,7 +28760,7 @@
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="85"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -28543,7 +29326,7 @@
       <c r="B9" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>464</v>
       </c>
     </row>
@@ -28554,7 +29337,7 @@
       <c r="B10" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -28563,7 +29346,7 @@
       <c r="B11" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="81"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -28572,7 +29355,7 @@
       <c r="B12" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="81"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -28581,7 +29364,7 @@
       <c r="B13" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="C13" s="79"/>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -28590,7 +29373,7 @@
       <c r="B14" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="C14" s="79"/>
+      <c r="C14" s="81"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -28599,7 +29382,7 @@
       <c r="B15" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -28608,7 +29391,7 @@
       <c r="B16" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="C16" s="79"/>
+      <c r="C16" s="81"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -28617,7 +29400,7 @@
       <c r="B17" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="81"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -28626,7 +29409,7 @@
       <c r="B18" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="81"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -28635,7 +29418,7 @@
       <c r="B19" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="C19" s="79"/>
+      <c r="C19" s="81"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -28644,7 +29427,7 @@
       <c r="B20" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="C20" s="79"/>
+      <c r="C20" s="81"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -28653,7 +29436,7 @@
       <c r="B21" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="C21" s="79"/>
+      <c r="C21" s="81"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
@@ -28662,12 +29445,12 @@
       <c r="B22" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="C22" s="79"/>
+      <c r="C22" s="81"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="79"/>
+      <c r="C23" s="81"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
@@ -28676,7 +29459,7 @@
       <c r="B24" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="C24" s="79"/>
+      <c r="C24" s="81"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -28685,7 +29468,7 @@
       <c r="B25" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="C25" s="79"/>
+      <c r="C25" s="81"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
@@ -28694,7 +29477,7 @@
       <c r="B26" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="C26" s="79"/>
+      <c r="C26" s="81"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
@@ -28703,7 +29486,7 @@
       <c r="B27" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="C27" s="79"/>
+      <c r="C27" s="81"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
@@ -28712,7 +29495,7 @@
       <c r="B28" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="C28" s="79"/>
+      <c r="C28" s="81"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
@@ -28721,7 +29504,7 @@
       <c r="B29" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="C29" s="79"/>
+      <c r="C29" s="81"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
@@ -28730,7 +29513,7 @@
       <c r="B30" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="79"/>
+      <c r="C30" s="81"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
@@ -28739,7 +29522,7 @@
       <c r="B31" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="C31" s="79"/>
+      <c r="C31" s="81"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
@@ -28748,7 +29531,7 @@
       <c r="B32" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="C32" s="79"/>
+      <c r="C32" s="81"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
@@ -28757,7 +29540,7 @@
       <c r="B33" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="C33" s="79"/>
+      <c r="C33" s="81"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
@@ -28766,7 +29549,7 @@
       <c r="B34" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="C34" s="79"/>
+      <c r="C34" s="81"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
@@ -28775,7 +29558,7 @@
       <c r="B35" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="C35" s="79"/>
+      <c r="C35" s="81"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
@@ -28784,7 +29567,7 @@
       <c r="B36" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="C36" s="79"/>
+      <c r="C36" s="81"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
@@ -28793,7 +29576,7 @@
       <c r="B37" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="C37" s="79"/>
+      <c r="C37" s="81"/>
       <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -31227,7 +32010,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -31411,7 +32194,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #170" xr:uid="{37D7FC97-074F-4506-8E74-513086B37344}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{37D7FC97-074F-4506-8E74-513086B37344}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -31425,6 +32208,194 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9701D3D3-681A-4860-8BB4-44439D106992}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>817</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>819</v>
+      </c>
+      <c r="B15" s="23">
+        <v>1744940304</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>818</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{6DC37B63-56C4-4AA0-849A-2C258D9867B2}"/>
+  </hyperlinks>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -31622,7 +32593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -31751,7 +32722,7 @@
       <c r="B9" s="39" t="s">
         <v>616</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="88" t="s">
         <v>617</v>
       </c>
       <c r="D9" s="40"/>
@@ -31766,7 +32737,7 @@
       <c r="B10" s="39" t="s">
         <v>619</v>
       </c>
-      <c r="C10" s="86"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
@@ -31875,7 +32846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
@@ -32004,7 +32975,7 @@
       <c r="B9" s="39" t="s">
         <v>635</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="89" t="s">
         <v>636</v>
       </c>
       <c r="D9" s="40"/>
@@ -32019,7 +32990,7 @@
       <c r="B10" s="39" t="s">
         <v>638</v>
       </c>
-      <c r="C10" s="87"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="40"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -32099,237 +33070,6 @@
       <c r="F15" s="67" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="65"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
-      <c r="B19" s="69"/>
-      <c r="D19" s="65"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="69"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C9:C10"/>
-  </mergeCells>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
-  <dimension ref="A1:H24"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="29.3984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="40.8984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>645</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="66" t="s">
-        <v>645</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>631</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-    </row>
-    <row r="4" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-    </row>
-    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
-        <v>983</v>
-      </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="88" t="s">
-        <v>646</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
-        <v>983</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="40"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>639</v>
-      </c>
-      <c r="B14" s="23">
-        <v>1047244063</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>647</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>647</v>
-      </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="67"/>
-    </row>
-    <row r="15" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
-        <v>642</v>
-      </c>
-      <c r="B15" s="23">
-        <v>267890168</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>647</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>648</v>
-      </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="67"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" s="65"/>
@@ -32553,6 +33293,237 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.3984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="40.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>645</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>631</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="66"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>983</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="90" t="s">
+        <v>646</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>983</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="40"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>639</v>
+      </c>
+      <c r="B14" s="23">
+        <v>1047244063</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>647</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>647</v>
+      </c>
+      <c r="E14" s="44"/>
+      <c r="F14" s="67"/>
+    </row>
+    <row r="15" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>642</v>
+      </c>
+      <c r="B15" s="23">
+        <v>267890168</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>647</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>648</v>
+      </c>
+      <c r="E15" s="44"/>
+      <c r="F15" s="67"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="65"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="68"/>
+      <c r="B19" s="69"/>
+      <c r="D19" s="65"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C10"/>
+  </mergeCells>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
@@ -32870,7 +33841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -32981,7 +33952,7 @@
       <c r="B9" s="9" t="s">
         <v>735</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>736</v>
       </c>
     </row>
@@ -32992,7 +33963,7 @@
       <c r="B10" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="11" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -33001,27 +33972,27 @@
       <c r="B11" s="9" t="s">
         <v>726</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="81"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="79"/>
+      <c r="C12" s="81"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="79"/>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="79"/>
+      <c r="C14" s="81"/>
     </row>
     <row r="15" spans="1:7" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
     </row>
     <row r="17" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -33125,7 +34096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A53A7B-BA0D-47EB-B9C5-D4EE8A52E7DE}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -33236,7 +34207,7 @@
       <c r="B9" s="9" t="s">
         <v>764</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>768</v>
       </c>
     </row>
@@ -33247,7 +34218,7 @@
       <c r="B10" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="12" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -33440,7 +34411,7 @@
       <c r="B9" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="81" t="s">
         <v>786</v>
       </c>
     </row>
@@ -33451,7 +34422,7 @@
       <c r="B10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="81"/>
     </row>
     <row r="11" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -33460,7 +34431,7 @@
       <c r="B11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="81"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -33469,7 +34440,7 @@
       <c r="B12" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="81"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -33478,7 +34449,7 @@
       <c r="B13" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="79"/>
+      <c r="C13" s="81"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" ht="69" x14ac:dyDescent="0.25">
@@ -33488,7 +34459,7 @@
       <c r="B14" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="79"/>
+      <c r="C14" s="81"/>
       <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -33498,7 +34469,7 @@
       <c r="B15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
@@ -33508,7 +34479,7 @@
       <c r="B16" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="79"/>
+      <c r="C16" s="81"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -33518,7 +34489,7 @@
       <c r="B17" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="81"/>
       <c r="I17" s="25"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -33528,7 +34499,7 @@
       <c r="B18" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="81"/>
       <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -33838,7 +34809,7 @@
       <c r="B9" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="82" t="s">
         <v>133</v>
       </c>
     </row>
@@ -33849,7 +34820,7 @@
       <c r="B10" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="80"/>
+      <c r="C10" s="82"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -33858,7 +34829,7 @@
       <c r="B11" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="80"/>
+      <c r="C11" s="82"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -33867,7 +34838,7 @@
       <c r="B12" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C12" s="80"/>
+      <c r="C12" s="82"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -33876,7 +34847,7 @@
       <c r="B13" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="80"/>
+      <c r="C13" s="82"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -33885,7 +34856,7 @@
       <c r="B14" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="80"/>
+      <c r="C14" s="82"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -33895,13 +34866,13 @@
       <c r="B15" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="80"/>
+      <c r="C15" s="82"/>
       <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="80"/>
+      <c r="C16" s="82"/>
       <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
@@ -33911,7 +34882,7 @@
       <c r="B17" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="80"/>
+      <c r="C17" s="82"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -33920,7 +34891,7 @@
       <c r="B18" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="80"/>
+      <c r="C18" s="82"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -33929,7 +34900,7 @@
       <c r="B19" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="80"/>
+      <c r="C19" s="82"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -33938,7 +34909,7 @@
       <c r="B20" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="80"/>
+      <c r="C20" s="82"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -33947,7 +34918,7 @@
       <c r="B21" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="80"/>
+      <c r="C21" s="82"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
@@ -33956,7 +34927,7 @@
       <c r="B22" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="80"/>
+      <c r="C22" s="82"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -33968,7 +34939,7 @@
       <c r="B23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="80"/>
+      <c r="C23" s="82"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>

</xml_diff>